<commit_message>
LnCO as on Dec 22
</commit_message>
<xml_diff>
--- a/Lnco/Input/Config.xlsx
+++ b/Lnco/Input/Config.xlsx
@@ -132,7 +132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
@@ -182,7 +182,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -533,17 +532,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B84"/>
+  <dimension ref="A1:B86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="114" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="48.5546875" customWidth="1" style="27" min="1" max="1"/>
-    <col width="84.21875" bestFit="1" customWidth="1" style="27" min="2" max="2"/>
-    <col width="30.77734375" bestFit="1" customWidth="1" style="27" min="4" max="4"/>
+    <col width="48.5546875" customWidth="1" style="26" min="1" max="1"/>
+    <col width="84.21875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
+    <col width="30.77734375" bestFit="1" customWidth="1" style="26" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -644,324 +643,342 @@
         </is>
       </c>
     </row>
-    <row r="11"/>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Output_Concentrations_Purchase_sheetname</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Purchase Wise Concentration</t>
-        </is>
-      </c>
-    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Output_Comparatives_Weightage_sheetname</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Comparatives_top_weightage</t>
+        </is>
+      </c>
+    </row>
+    <row r="12"/>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Output_Concentrations_Month_sheetname</t>
+          <t>Output_Concentrations_Purchase_sheetname</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Month Wise Concentration</t>
+          <t>Purchase Wise Concentration</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Output_Concentrations_Plant_sheetname</t>
+          <t>Output_Concentrations_Month_sheetname</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Plant Wise Concentration</t>
+          <t>Month Wise Concentration</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Output_Concentrations_Dom&amp;Imp_sheetname</t>
+          <t>Output_Concentrations_Plant_sheetname</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Dom&amp;Imp Wise Concentration</t>
+          <t>Plant Wise Concentration</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>Output_Concentrations_Dom&amp;Imp_sheetname</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Dom&amp;Imp Wise Concentration</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>Output_Concentration_Vendor_sheetname</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>Vendor Wise Concentration</t>
         </is>
       </c>
     </row>
-    <row r="17"/>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Output_Duplication_of_Vendor_sheetname</t>
+          <t>Output_Concentration_Weightage_sheetname</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Duplication Of Vendor</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Output_Average_Day_Purchase_sheetname</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Average Day Purchase</t>
-        </is>
-      </c>
-    </row>
+          <t>Concentration_top_weightage</t>
+        </is>
+      </c>
+    </row>
+    <row r="19"/>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Output_Same_Material_Purchases_DVDP_sheetname</t>
+          <t>Output_Duplication_of_Vendor_sheetname</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SMP from DVnDP</t>
+          <t>Duplication Of Vendor</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Output_Unit_Price_Comparison_sheetname</t>
+          <t>Output_Average_Day_Purchase_sheetname</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Unit Price Comparison</t>
+          <t>Average Day Purchase</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>Output_Same_Material_Purchases_DVDP_sheetname</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>SMP from DVnDP</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Output_Unit_Price_Comparison_sheetname</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Unit Price Comparison</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
           <t>Output_Inventory_Mapping_Sheetname</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <t>Inventory Mapping</t>
         </is>
       </c>
     </row>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25">
-      <c r="A25" s="21" t="inlineStr">
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27">
+      <c r="A27" s="21" t="inlineStr">
         <is>
           <t>Other Keys</t>
         </is>
       </c>
-      <c r="B25" s="21" t="inlineStr">
+      <c r="B27" s="21" t="inlineStr">
         <is>
           <t>Other Values</t>
         </is>
       </c>
     </row>
-    <row r="26">
-      <c r="B26" s="15" t="n"/>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
+    <row r="28">
+      <c r="B28" s="15" t="n"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
         <is>
           <t>purchase_register_1st_column_name</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
           <t>Plant</t>
         </is>
       </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>purchase_register_2nd_column_name</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>GR Document Number</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" s="15" t="n"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t>purchase_register_2nd_column_name</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>GR Document Number</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" s="15" t="n"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
           <t>MB51_first_column</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B32" t="inlineStr">
         <is>
           <t>Plant</t>
         </is>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>MB51_second_column</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Material</t>
-        </is>
-      </c>
-    </row>
-    <row r="32"/>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>LOCAL_DOTENV_FILE</t>
+          <t>MB51_second_column</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>local_new.env</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>QUALITY_DOTENV_FILE</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>quality.env</t>
-        </is>
-      </c>
-    </row>
+          <t>Material</t>
+        </is>
+      </c>
+    </row>
+    <row r="34"/>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>ENV_FILE</t>
+          <t>LOCAL_DOTENV_FILE</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>LOCAL_DOTENV_FILE</t>
-        </is>
-      </c>
-    </row>
-    <row r="36"/>
+          <t>local_new.env</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>QUALITY_DOTENV_FILE</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>quality.env</t>
+        </is>
+      </c>
+    </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Request Status Name</t>
+          <t>ENV_FILE</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Request Status Name</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>New_Request_Status</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>New</t>
-        </is>
-      </c>
-    </row>
+          <t>LOCAL_DOTENV_FILE</t>
+        </is>
+      </c>
+    </row>
+    <row r="38"/>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>In_Progress_Request_Status</t>
+          <t>Request Status Name</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>In Progress</t>
+          <t>Request Status Name</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Success_Request_Status</t>
+          <t>New_Request_Status</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Completed</t>
+          <t>New</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Fail_Request_Status</t>
+          <t>In_Progress_Request_Status</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Failed</t>
-        </is>
-      </c>
-    </row>
-    <row r="42"/>
+          <t>In Progress</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Success_Request_Status</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+    </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>Fail_Request_Status</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+    </row>
+    <row r="44"/>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
           <t>To_Mail_Address</t>
         </is>
       </c>
-      <c r="B43" s="15" t="inlineStr">
+      <c r="B45" s="15" t="inlineStr">
         <is>
           <t>kalyan.gundu@bradsol.com</t>
         </is>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
+    <row r="46">
+      <c r="A46" t="inlineStr">
         <is>
           <t>CC_Mail_Address</t>
         </is>
       </c>
-      <c r="B44" s="15" t="inlineStr">
+      <c r="B46" s="15" t="inlineStr">
         <is>
           <t>kalyan.gundu@bradsol.com</t>
         </is>
       </c>
-    </row>
-    <row r="45">
-      <c r="B45" s="23" t="n"/>
-    </row>
-    <row r="46">
-      <c r="B46" s="23" t="n"/>
     </row>
     <row r="47">
       <c r="B47" s="23" t="n"/>
@@ -969,234 +986,240 @@
     <row r="48">
       <c r="B48" s="23" t="n"/>
     </row>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51">
-      <c r="A51" s="21" t="inlineStr">
+    <row r="49">
+      <c r="B49" s="23" t="n"/>
+    </row>
+    <row r="50">
+      <c r="B50" s="23" t="n"/>
+    </row>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53">
+      <c r="A53" s="21" t="inlineStr">
         <is>
           <t>Sheet Name keys in Config File</t>
         </is>
       </c>
-      <c r="B51" s="21" t="inlineStr">
+      <c r="B53" s="21" t="inlineStr">
         <is>
           <t>SheetName values in Config file</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>Config_Comparatives_Purchase_sheetname</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Purchase Wise Comparatives</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>Config_Comparatives_Month_sheetname</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>Month Wise Comparatives</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Config_Comparatives_Plant_sheetname</t>
+          <t>Config_Comparatives_Purchase_sheetname</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Plant Wise Comparatives</t>
+          <t>Purchase Wise Comparatives</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Config_Comparatives_Dom&amp;Imp_sheetname</t>
+          <t>Config_Comparatives_Month_sheetname</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Dom&amp;Imp Wise Comparatives</t>
+          <t>Month Wise Comparatives</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Config_Comparatives_Vendor_sheetname</t>
+          <t>Config_Comparatives_Plant_sheetname</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Vendor Wise Comparatives</t>
-        </is>
-      </c>
-    </row>
-    <row r="57"/>
+          <t>Plant Wise Comparatives</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Config_Comparatives_Dom&amp;Imp_sheetname</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Dom&amp;Imp Wise Comparatives</t>
+        </is>
+      </c>
+    </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Config_Concentrations_Purchase_sheetname</t>
+          <t>Config_Comparatives_Vendor_sheetname</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Purchase Wise Concentration</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>Config_Concentrations_Month_sheetname</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>Month Wise Concentration</t>
-        </is>
-      </c>
-    </row>
+          <t>Vendor Wise Comparatives</t>
+        </is>
+      </c>
+    </row>
+    <row r="59"/>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Config_Concentrations_Plant_sheetname</t>
+          <t>Config_Concentrations_Purchase_sheetname</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Plant Wise Concentration</t>
+          <t>Purchase Wise Concentration</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Config_Concentrations_Dom&amp;Imp_sheetname</t>
+          <t>Config_Concentrations_Month_sheetname</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Dom&amp;Imp Wise Concentration</t>
+          <t>Month Wise Concentration</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Config_Concentration_Vendor_sheetname</t>
+          <t>Config_Concentrations_Plant_sheetname</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Vendor Wise Concentration</t>
-        </is>
-      </c>
-    </row>
-    <row r="63"/>
+          <t>Plant Wise Concentration</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Config_Concentrations_Dom&amp;Imp_sheetname</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Dom&amp;Imp Wise Concentration</t>
+        </is>
+      </c>
+    </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Config_Duplication_of_Vendor_sheetname</t>
+          <t>Config_Concentration_Vendor_sheetname</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Duplication Of Vendor</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>Config_Average_Day_Purchase_sheetname</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>Average Day Purchase</t>
-        </is>
-      </c>
-    </row>
+          <t>Vendor Wise Concentration</t>
+        </is>
+      </c>
+    </row>
+    <row r="65"/>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Config_Same_Material_Purchases_DVDP_sheetname</t>
+          <t>Config_Duplication_of_Vendor_sheetname</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>SMP from DVnDP</t>
+          <t>Duplication Of Vendor</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Config_Unit_Price_Comparison_sheetname</t>
+          <t>Config_Average_Day_Purchase_sheetname</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Unit Price Comparison</t>
+          <t>Average Day Purchase</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
+          <t>Config_Same_Material_Purchases_DVDP_sheetname</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>SMP from DVnDP</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Config_Unit_Price_Comparison_sheetname</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Unit Price Comparison</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
           <t>Config_Inventory_Mapping_Sheetname</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
+      <c r="B70" t="inlineStr">
         <is>
           <t>Inventory Mapping</t>
         </is>
       </c>
     </row>
-    <row r="69"/>
-    <row r="70">
-      <c r="A70" s="21" t="inlineStr">
+    <row r="71"/>
+    <row r="72">
+      <c r="A72" s="21" t="inlineStr">
         <is>
           <t>Mails related Keys</t>
         </is>
       </c>
-      <c r="B70" s="21" t="inlineStr">
+      <c r="B72" s="21" t="inlineStr">
         <is>
           <t>Values</t>
         </is>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
+    <row r="73">
+      <c r="A73" t="inlineStr">
         <is>
           <t>Start_Mail_Subject</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
+      <c r="B73" t="inlineStr">
         <is>
           <t xml:space="preserve">Bot execution is started </t>
         </is>
       </c>
     </row>
-    <row r="72" ht="86.40000000000001" customHeight="1" s="27">
-      <c r="A72" t="inlineStr">
+    <row r="74" ht="86.40000000000001" customHeight="1" s="26">
+      <c r="A74" t="inlineStr">
         <is>
           <t>Start_Mail_Body</t>
         </is>
       </c>
-      <c r="B72" s="19" t="inlineStr">
+      <c r="B74" s="19" t="inlineStr">
         <is>
           <t>Hello,
 Bot has started processing the purchase register report automation
@@ -1205,26 +1228,26 @@
         </is>
       </c>
     </row>
-    <row r="73"/>
-    <row r="74">
-      <c r="A74" t="inlineStr">
+    <row r="75"/>
+    <row r="76">
+      <c r="A76" t="inlineStr">
         <is>
           <t>Success_Mail_Subject</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
+      <c r="B76" t="inlineStr">
         <is>
           <t xml:space="preserve">Bot execution is completed </t>
         </is>
       </c>
     </row>
-    <row r="75" ht="86.40000000000001" customHeight="1" s="27">
-      <c r="A75" t="inlineStr">
+    <row r="77" ht="86.40000000000001" customHeight="1" s="26">
+      <c r="A77" t="inlineStr">
         <is>
           <t>Success_Mail_Body</t>
         </is>
       </c>
-      <c r="B75" s="19" t="inlineStr">
+      <c r="B77" s="19" t="inlineStr">
         <is>
           <t>Hello,
 Bot has Successfully completed the purchase register report automation.
@@ -1233,26 +1256,26 @@
         </is>
       </c>
     </row>
-    <row r="76"/>
-    <row r="77">
-      <c r="A77" t="inlineStr">
+    <row r="78"/>
+    <row r="79">
+      <c r="A79" t="inlineStr">
         <is>
           <t>subject_file_not_found</t>
         </is>
       </c>
-      <c r="B77" t="inlineStr">
+      <c r="B79" t="inlineStr">
         <is>
           <t>Bot Execution is stopped - Input file is missing</t>
         </is>
       </c>
     </row>
-    <row r="78" ht="100.8" customHeight="1" s="27">
-      <c r="A78" t="inlineStr">
+    <row r="80" ht="100.8" customHeight="1" s="26">
+      <c r="A80" t="inlineStr">
         <is>
           <t>body_file_not_found</t>
         </is>
       </c>
-      <c r="B78" s="17" t="inlineStr">
+      <c r="B80" s="17" t="inlineStr">
         <is>
           <t xml:space="preserve">Hello,
 Purchase Register Input File is Missing. Hence stopping the execution of the program.
@@ -1262,28 +1285,28 @@
         </is>
       </c>
     </row>
-    <row r="79">
-      <c r="B79" s="13" t="n"/>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
+    <row r="81">
+      <c r="B81" s="13" t="n"/>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
         <is>
           <t>subject_sheet_not_found</t>
         </is>
       </c>
-      <c r="B80" t="inlineStr">
+      <c r="B82" t="inlineStr">
         <is>
           <t>Bot Execution is stopped - Input file sheet is missing</t>
         </is>
       </c>
     </row>
-    <row r="81" ht="100.8" customHeight="1" s="27">
-      <c r="A81" t="inlineStr">
+    <row r="83" ht="100.8" customHeight="1" s="26">
+      <c r="A83" t="inlineStr">
         <is>
           <t>body_sheet_not_found</t>
         </is>
       </c>
-      <c r="B81" s="17" t="inlineStr">
+      <c r="B83" s="17" t="inlineStr">
         <is>
           <t xml:space="preserve">Hello,
 Purchase Register Input File sheet is Missing. Hence stopping the execution of the program.
@@ -1293,26 +1316,26 @@
         </is>
       </c>
     </row>
-    <row r="82"/>
-    <row r="83">
-      <c r="A83" t="inlineStr">
+    <row r="84"/>
+    <row r="85">
+      <c r="A85" t="inlineStr">
         <is>
           <t>subject_in_progress_request_found</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr">
+      <c r="B85" t="inlineStr">
         <is>
           <t>Bot Execution is stopped - prior requests are in progress</t>
         </is>
       </c>
     </row>
-    <row r="84" ht="100.8" customHeight="1" s="27">
-      <c r="A84" t="inlineStr">
+    <row r="86" ht="100.8" customHeight="1" s="26">
+      <c r="A86" t="inlineStr">
         <is>
           <t>body_in_progress_request_found</t>
         </is>
       </c>
-      <c r="B84" s="17" t="inlineStr">
+      <c r="B86" s="17" t="inlineStr">
         <is>
           <t xml:space="preserve">Hello,
 The bot is executing prior requests. Hence stopping the execution of the program.
@@ -1324,13 +1347,13 @@
     </row>
   </sheetData>
   <dataValidations xWindow="832" yWindow="791" count="1">
-    <dataValidation sqref="B35:B36" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Select Correct File" error="Should be same as Input message provided" promptTitle="Select Env File type" prompt="LOCAL_DOTENV_FILE (or) QUALTIY_DOTENV_FILE" type="list">
-      <formula1>$A$33:$A$34</formula1>
+    <dataValidation sqref="B37:B38" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Select Correct File" error="Should be same as Input message provided" promptTitle="Select Env File type" prompt="LOCAL_DOTENV_FILE (or) QUALTIY_DOTENV_FILE" type="list">
+      <formula1>$A$35:$A$36</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B43" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B44" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B45" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B46" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -1351,10 +1374,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="24.5546875" bestFit="1" customWidth="1" style="27" min="1" max="1"/>
-    <col width="92.33203125" bestFit="1" customWidth="1" style="27" min="2" max="2"/>
-    <col width="43.6640625" customWidth="1" style="27" min="5" max="5"/>
-    <col width="36.109375" customWidth="1" style="27" min="6" max="6"/>
+    <col width="24.5546875" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="92.33203125" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
+    <col width="43.6640625" customWidth="1" style="26" min="5" max="5"/>
+    <col width="36.109375" customWidth="1" style="26" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1381,7 +1404,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="3" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A3" s="3" t="inlineStr">
         <is>
           <t>FileNotFound_Body</t>
@@ -1408,7 +1431,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="5" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A5" s="3" t="inlineStr">
         <is>
           <t>EmptyInput_Body</t>
@@ -1435,7 +1458,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="7" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A7" s="3" t="inlineStr">
         <is>
           <t>EmptyValClass_Body</t>
@@ -1462,7 +1485,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="9" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A9" s="3" t="inlineStr">
         <is>
           <t>EmptyValClassTxt_Body</t>
@@ -1489,7 +1512,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="11" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A11" s="3" t="inlineStr">
         <is>
           <t>GRAmt_Subject</t>
@@ -1516,7 +1539,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="13" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A13" s="3" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -1543,7 +1566,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="15" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A15" s="3" t="inlineStr">
         <is>
           <t>SheetMiss_Body</t>
@@ -1570,7 +1593,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="17" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A17" s="3" t="inlineStr">
         <is>
           <t>OutputNotFound_Body</t>
@@ -1597,7 +1620,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="19" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A19" s="3" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -1727,8 +1750,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="49.33203125" customWidth="1" style="27" min="1" max="1"/>
-    <col width="83.88671875" customWidth="1" style="27" min="2" max="2"/>
+    <col width="49.33203125" customWidth="1" style="26" min="1" max="1"/>
+    <col width="83.88671875" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1755,7 +1778,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="100.8" customHeight="1" s="27">
+    <row r="3" ht="100.8" customHeight="1" s="26">
       <c r="A3" t="inlineStr">
         <is>
           <t>Vendor No._Body</t>
@@ -1783,7 +1806,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="100.8" customHeight="1" s="27">
+    <row r="5" ht="100.8" customHeight="1" s="26">
       <c r="A5" t="inlineStr">
         <is>
           <t>Vendor Name_Body</t>
@@ -1811,7 +1834,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="100.8" customHeight="1" s="27">
+    <row r="7" ht="100.8" customHeight="1" s="26">
       <c r="A7" t="inlineStr">
         <is>
           <t>Gr Amt_Body</t>
@@ -1839,7 +1862,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="9" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A9" t="inlineStr">
         <is>
           <t>FileNotFound_Body</t>
@@ -1866,7 +1889,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="11" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A11" t="inlineStr">
         <is>
           <t>EmptyInput_Body</t>
@@ -1881,7 +1904,7 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="12" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A12" t="inlineStr">
         <is>
           <t>EmptyInput_Body1</t>
@@ -1908,7 +1931,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="14" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A14" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -1923,7 +1946,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="15" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A15" t="inlineStr">
         <is>
           <t>ColumnMiss_Body1</t>
@@ -1950,7 +1973,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="17" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A17" t="inlineStr">
         <is>
           <t>SheetMiss_Body</t>
@@ -1977,7 +2000,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="19" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A19" t="inlineStr">
         <is>
           <t>OutputNotFound_Body</t>
@@ -2004,7 +2027,7 @@
         </is>
       </c>
     </row>
-    <row r="21" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="21" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A21" t="inlineStr">
         <is>
           <t>SystemE_Body</t>
@@ -2031,7 +2054,7 @@
         </is>
       </c>
     </row>
-    <row r="23" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="23" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A23" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -2161,8 +2184,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="35.5546875" bestFit="1" customWidth="1" style="27" min="1" max="1"/>
-    <col width="86.88671875" bestFit="1" customWidth="1" style="27" min="2" max="2"/>
+    <col width="35.5546875" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="86.88671875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2189,7 +2212,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="100.8" customHeight="1" s="27">
+    <row r="4" ht="100.8" customHeight="1" s="26">
       <c r="A4" t="inlineStr">
         <is>
           <t>Body_mail</t>
@@ -2217,7 +2240,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="100.8" customHeight="1" s="27">
+    <row r="7" ht="100.8" customHeight="1" s="26">
       <c r="A7" t="inlineStr">
         <is>
           <t>body_file_not_found</t>
@@ -2248,7 +2271,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="100.8" customHeight="1" s="27">
+    <row r="10" ht="100.8" customHeight="1" s="26">
       <c r="A10" t="inlineStr">
         <is>
           <t>Gr Amt_Body</t>
@@ -2276,7 +2299,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="100.8" customHeight="1" s="27">
+    <row r="13" ht="100.8" customHeight="1" s="26">
       <c r="A13" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -2304,7 +2327,7 @@
         </is>
       </c>
     </row>
-    <row r="16" ht="100.8" customHeight="1" s="27">
+    <row r="16" ht="100.8" customHeight="1" s="26">
       <c r="A16" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -2435,8 +2458,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="24.5546875" bestFit="1" customWidth="1" style="27" min="1" max="1"/>
-    <col width="86.88671875" bestFit="1" customWidth="1" style="27" min="2" max="2"/>
+    <col width="24.5546875" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="86.88671875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2463,7 +2486,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="100.8" customHeight="1" s="27">
+    <row r="4" ht="100.8" customHeight="1" s="26">
       <c r="A4" t="inlineStr">
         <is>
           <t>Body_mail</t>
@@ -2491,7 +2514,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="100.8" customHeight="1" s="27">
+    <row r="6" ht="100.8" customHeight="1" s="26">
       <c r="A6" t="inlineStr">
         <is>
           <t>Plant_Body</t>
@@ -2525,7 +2548,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="100.8" customHeight="1" s="27">
+    <row r="10" ht="100.8" customHeight="1" s="26">
       <c r="A10" t="inlineStr">
         <is>
           <t>Gr Amt_Body</t>
@@ -2553,7 +2576,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="100.8" customHeight="1" s="27">
+    <row r="13" ht="100.8" customHeight="1" s="26">
       <c r="A13" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -2584,7 +2607,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="100.8" customHeight="1" s="27">
+    <row r="19" ht="100.8" customHeight="1" s="26">
       <c r="A19" t="inlineStr">
         <is>
           <t>body_file_not_found</t>
@@ -2612,7 +2635,7 @@
         </is>
       </c>
     </row>
-    <row r="22" ht="100.8" customHeight="1" s="27">
+    <row r="22" ht="100.8" customHeight="1" s="26">
       <c r="A22" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -2743,8 +2766,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="17.88671875" bestFit="1" customWidth="1" style="27" min="1" max="1"/>
-    <col width="86.88671875" bestFit="1" customWidth="1" style="27" min="2" max="2"/>
+    <col width="17.88671875" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="86.88671875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2771,7 +2794,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="100.8" customHeight="1" s="27">
+    <row r="4" ht="100.8" customHeight="1" s="26">
       <c r="A4" t="inlineStr">
         <is>
           <t>Body_mail</t>
@@ -2799,7 +2822,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="100.8" customHeight="1" s="27">
+    <row r="6" ht="100.8" customHeight="1" s="26">
       <c r="A6" t="inlineStr">
         <is>
           <t>Month_Body</t>
@@ -2833,7 +2856,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="100.8" customHeight="1" s="27">
+    <row r="10" ht="100.8" customHeight="1" s="26">
       <c r="A10" t="inlineStr">
         <is>
           <t>Gr Amt_Body</t>
@@ -2864,7 +2887,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="100.8" customHeight="1" s="27">
+    <row r="13" ht="100.8" customHeight="1" s="26">
       <c r="A13" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -2895,7 +2918,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="100.8" customHeight="1" s="27">
+    <row r="19" ht="100.8" customHeight="1" s="26">
       <c r="A19" t="inlineStr">
         <is>
           <t>body_file_not_found</t>
@@ -2923,7 +2946,7 @@
         </is>
       </c>
     </row>
-    <row r="22" ht="100.8" customHeight="1" s="27">
+    <row r="22" ht="100.8" customHeight="1" s="26">
       <c r="A22" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -3054,8 +3077,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="26.88671875" bestFit="1" customWidth="1" style="27" min="1" max="1"/>
-    <col width="91.88671875" bestFit="1" customWidth="1" style="27" min="2" max="2"/>
+    <col width="26.88671875" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="91.88671875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3082,7 +3105,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="100.8" customHeight="1" s="27">
+    <row r="4" ht="100.8" customHeight="1" s="26">
       <c r="A4" t="inlineStr">
         <is>
           <t>Body_mail</t>
@@ -3110,7 +3133,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="100.8" customHeight="1" s="27">
+    <row r="6" ht="100.8" customHeight="1" s="26">
       <c r="A6" t="inlineStr">
         <is>
           <t>Valuation Class_Body</t>
@@ -3138,7 +3161,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="100.8" customHeight="1" s="27">
+    <row r="8" ht="100.8" customHeight="1" s="26">
       <c r="A8" t="inlineStr">
         <is>
           <t>Valuation Class Text_Body</t>
@@ -3166,7 +3189,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="100.8" customHeight="1" s="27">
+    <row r="10" ht="100.8" customHeight="1" s="26">
       <c r="A10" t="inlineStr">
         <is>
           <t>Gr Amt_Body</t>
@@ -3197,7 +3220,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="100.8" customHeight="1" s="27">
+    <row r="13" ht="100.8" customHeight="1" s="26">
       <c r="A13" t="inlineStr">
         <is>
           <t>body_file_not_found</t>
@@ -3228,7 +3251,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="100.8" customHeight="1" s="27">
+    <row r="19" ht="100.8" customHeight="1" s="26">
       <c r="A19" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -3256,7 +3279,7 @@
         </is>
       </c>
     </row>
-    <row r="22" ht="100.8" customHeight="1" s="27">
+    <row r="22" ht="100.8" customHeight="1" s="26">
       <c r="A22" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -3387,8 +3410,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="29.33203125" bestFit="1" customWidth="1" style="27" min="1" max="1"/>
-    <col width="94.6640625" bestFit="1" customWidth="1" style="27" min="2" max="2"/>
+    <col width="29.33203125" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="94.6640625" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3454,7 +3477,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="100.8" customHeight="1" s="27">
+    <row r="8" ht="100.8" customHeight="1" s="26">
       <c r="A8" t="inlineStr">
         <is>
           <t>Body_mail</t>
@@ -3482,7 +3505,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="100.8" customHeight="1" s="27">
+    <row r="10" ht="100.8" customHeight="1" s="26">
       <c r="A10" t="inlineStr">
         <is>
           <t>GR Document_Number_Body</t>
@@ -3516,7 +3539,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="100.8" customHeight="1" s="27">
+    <row r="14" ht="100.8" customHeight="1" s="26">
       <c r="A14" t="inlineStr">
         <is>
           <t>Gr Qty_Body</t>
@@ -3544,7 +3567,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="100.8" customHeight="1" s="27">
+    <row r="17" ht="100.8" customHeight="1" s="26">
       <c r="A17" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -3575,7 +3598,7 @@
         </is>
       </c>
     </row>
-    <row r="23" ht="100.8" customHeight="1" s="27">
+    <row r="23" ht="100.8" customHeight="1" s="26">
       <c r="A23" t="inlineStr">
         <is>
           <t>body_file_not_found</t>
@@ -3603,7 +3626,7 @@
         </is>
       </c>
     </row>
-    <row r="26" ht="100.8" customHeight="1" s="27">
+    <row r="26" ht="100.8" customHeight="1" s="26">
       <c r="A26" t="inlineStr">
         <is>
           <t>Purchase_ColumnMiss_Body</t>
@@ -3631,7 +3654,7 @@
         </is>
       </c>
     </row>
-    <row r="29" ht="100.8" customHeight="1" s="27">
+    <row r="29" ht="100.8" customHeight="1" s="26">
       <c r="A29" t="inlineStr">
         <is>
           <t>MB51_ColumnMiss_Body</t>
@@ -3659,7 +3682,7 @@
         </is>
       </c>
     </row>
-    <row r="32" ht="100.8" customHeight="1" s="27">
+    <row r="32" ht="100.8" customHeight="1" s="26">
       <c r="A32" t="inlineStr">
         <is>
           <t>Material_Document_Body</t>
@@ -3693,7 +3716,7 @@
         </is>
       </c>
     </row>
-    <row r="36" ht="100.8" customHeight="1" s="27">
+    <row r="36" ht="100.8" customHeight="1" s="26">
       <c r="A36" t="inlineStr">
         <is>
           <t>Qty_unit_of_entry_Body</t>
@@ -3729,11 +3752,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="35.5546875" bestFit="1" customWidth="1" style="27" min="1" max="1"/>
-    <col width="122" customWidth="1" style="27" min="2" max="2"/>
+    <col width="35.5546875" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="122" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.6" customHeight="1" s="27">
+    <row r="1" ht="18.6" customHeight="1" s="26">
       <c r="A1" s="14" t="inlineStr">
         <is>
           <t>Name</t>
@@ -3757,7 +3780,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="6" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A6" t="inlineStr">
         <is>
           <t>FileNotFound_Body</t>
@@ -3784,7 +3807,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="8" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A8" t="inlineStr">
         <is>
           <t>EmptyInput_Body</t>
@@ -3799,7 +3822,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="9" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A9" t="inlineStr">
         <is>
           <t>EmptyInput_Body1</t>
@@ -3826,7 +3849,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="11" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A11" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -3841,7 +3864,7 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="12" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A12" t="inlineStr">
         <is>
           <t>ColumnMiss_Body1</t>
@@ -3868,7 +3891,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="14" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A14" t="inlineStr">
         <is>
           <t>SheetMiss_Body</t>
@@ -3895,7 +3918,7 @@
         </is>
       </c>
     </row>
-    <row r="16" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="16" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A16" t="inlineStr">
         <is>
           <t>OutputNotFound_Body</t>
@@ -3922,7 +3945,7 @@
         </is>
       </c>
     </row>
-    <row r="18" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="18" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A18" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -4040,11 +4063,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="19.109375" bestFit="1" customWidth="1" style="27" min="1" max="1"/>
-    <col width="143.88671875" customWidth="1" style="27" min="2" max="2"/>
+    <col width="19.109375" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="143.88671875" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" customHeight="1" s="27">
+    <row r="1" ht="15.6" customHeight="1" s="26">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Key</t>
@@ -4056,11 +4079,11 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="15.6" customHeight="1" s="27">
-      <c r="A2" s="26" t="n"/>
-      <c r="B2" s="26" t="n"/>
-    </row>
-    <row r="3" ht="15.6" customHeight="1" s="27">
+    <row r="2" ht="15.6" customHeight="1" s="26">
+      <c r="A2" s="25" t="n"/>
+      <c r="B2" s="25" t="n"/>
+    </row>
+    <row r="3" ht="15.6" customHeight="1" s="26">
       <c r="A3" s="6" t="inlineStr">
         <is>
           <t>Subject_mail</t>
@@ -4072,8 +4095,8 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="93.59999999999999" customHeight="1" s="27">
-      <c r="A4" s="26" t="inlineStr">
+    <row r="4" ht="93.59999999999999" customHeight="1" s="26">
+      <c r="A4" s="25" t="inlineStr">
         <is>
           <t>Body_mail</t>
         </is>
@@ -4087,20 +4110,20 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="15.6" customHeight="1" s="27">
-      <c r="A5" s="26" t="inlineStr">
+    <row r="5" ht="15.6" customHeight="1" s="26">
+      <c r="A5" s="25" t="inlineStr">
         <is>
           <t>Unit_price</t>
         </is>
       </c>
-      <c r="B5" s="26" t="inlineStr">
+      <c r="B5" s="25" t="inlineStr">
         <is>
           <t>The unit price column has no data</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="93.59999999999999" customHeight="1" s="27">
-      <c r="A6" s="26" t="inlineStr">
+    <row r="6" ht="93.59999999999999" customHeight="1" s="26">
+      <c r="A6" s="25" t="inlineStr">
         <is>
           <t>Unit_price_body</t>
         </is>
@@ -4114,19 +4137,19 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="15.6" customHeight="1" s="27">
+    <row r="7" ht="15.6" customHeight="1" s="26">
       <c r="A7" s="6" t="inlineStr">
         <is>
           <t>Document is empty</t>
         </is>
       </c>
-      <c r="B7" s="26" t="inlineStr">
+      <c r="B7" s="25" t="inlineStr">
         <is>
           <t>Document is has no data</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="93.59999999999999" customHeight="1" s="27">
+    <row r="8" ht="93.59999999999999" customHeight="1" s="26">
       <c r="A8" s="22" t="inlineStr">
         <is>
           <t>Doc_bod</t>
@@ -4141,20 +4164,20 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="15.6" customHeight="1" s="27">
-      <c r="A9" s="26" t="inlineStr">
+    <row r="9" ht="15.6" customHeight="1" s="26">
+      <c r="A9" s="25" t="inlineStr">
         <is>
           <t>Key</t>
         </is>
       </c>
-      <c r="B9" s="26" t="inlineStr">
+      <c r="B9" s="25" t="inlineStr">
         <is>
           <t>KeyError</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="93.59999999999999" customHeight="1" s="27">
-      <c r="A10" s="26" t="inlineStr">
+    <row r="10" ht="93.59999999999999" customHeight="1" s="26">
+      <c r="A10" s="25" t="inlineStr">
         <is>
           <t>Key_body</t>
         </is>
@@ -4168,20 +4191,20 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="15.6" customHeight="1" s="27">
-      <c r="A11" s="26" t="inlineStr">
+    <row r="11" ht="15.6" customHeight="1" s="26">
+      <c r="A11" s="25" t="inlineStr">
         <is>
           <t>Syn</t>
         </is>
       </c>
-      <c r="B11" s="26" t="inlineStr">
+      <c r="B11" s="25" t="inlineStr">
         <is>
           <t>SyntaxError</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="93.59999999999999" customHeight="1" s="27">
-      <c r="A12" s="26" t="inlineStr">
+    <row r="12" ht="93.59999999999999" customHeight="1" s="26">
+      <c r="A12" s="25" t="inlineStr">
         <is>
           <t>Synody_</t>
         </is>
@@ -4195,20 +4218,20 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="15.6" customHeight="1" s="27">
-      <c r="A13" s="26" t="inlineStr">
+    <row r="13" ht="15.6" customHeight="1" s="26">
+      <c r="A13" s="25" t="inlineStr">
         <is>
           <t>File_N</t>
         </is>
       </c>
-      <c r="B13" s="26" t="inlineStr">
+      <c r="B13" s="25" t="inlineStr">
         <is>
           <t>FileNotfound</t>
         </is>
       </c>
     </row>
-    <row r="14" ht="93.59999999999999" customHeight="1" s="27">
-      <c r="A14" s="26" t="inlineStr">
+    <row r="14" ht="93.59999999999999" customHeight="1" s="26">
+      <c r="A14" s="25" t="inlineStr">
         <is>
           <t>File_N_body</t>
         </is>
@@ -4222,20 +4245,20 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="15.6" customHeight="1" s="27">
-      <c r="A15" s="26" t="inlineStr">
+    <row r="15" ht="15.6" customHeight="1" s="26">
+      <c r="A15" s="25" t="inlineStr">
         <is>
           <t>Name_E</t>
         </is>
       </c>
-      <c r="B15" s="26" t="inlineStr">
+      <c r="B15" s="25" t="inlineStr">
         <is>
           <t>NameError</t>
         </is>
       </c>
     </row>
-    <row r="16" ht="93.59999999999999" customHeight="1" s="27">
-      <c r="A16" s="26" t="inlineStr">
+    <row r="16" ht="93.59999999999999" customHeight="1" s="26">
+      <c r="A16" s="25" t="inlineStr">
         <is>
           <t>Name_E_body</t>
         </is>
@@ -4249,20 +4272,20 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="15.6" customHeight="1" s="27">
-      <c r="A17" s="26" t="inlineStr">
+    <row r="17" ht="15.6" customHeight="1" s="26">
+      <c r="A17" s="25" t="inlineStr">
         <is>
           <t>Value_E</t>
         </is>
       </c>
-      <c r="B17" s="26" t="inlineStr">
+      <c r="B17" s="25" t="inlineStr">
         <is>
           <t>ValueError</t>
         </is>
       </c>
     </row>
-    <row r="18" ht="93.59999999999999" customHeight="1" s="27">
-      <c r="A18" s="26" t="inlineStr">
+    <row r="18" ht="93.59999999999999" customHeight="1" s="26">
+      <c r="A18" s="25" t="inlineStr">
         <is>
           <t>Value_E_body</t>
         </is>
@@ -4403,8 +4426,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="17.109375" customWidth="1" style="27" min="1" max="1"/>
-    <col width="96.109375" customWidth="1" style="27" min="2" max="2"/>
+    <col width="17.109375" customWidth="1" style="26" min="1" max="1"/>
+    <col width="96.109375" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4423,7 +4446,7 @@
       <c r="A2" s="3" t="n"/>
       <c r="B2" s="10" t="n"/>
     </row>
-    <row r="3" ht="100.8" customHeight="1" s="27">
+    <row r="3" ht="100.8" customHeight="1" s="26">
       <c r="A3" s="3" t="inlineStr">
         <is>
           <t>FileNotFoundError</t>
@@ -4438,7 +4461,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="100.8" customHeight="1" s="27">
+    <row r="4" ht="100.8" customHeight="1" s="26">
       <c r="A4" s="3" t="inlineStr">
         <is>
           <t>FileExistsError</t>
@@ -4454,7 +4477,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="115.2" customHeight="1" s="27">
+    <row r="5" ht="115.2" customHeight="1" s="26">
       <c r="A5" s="3" t="inlineStr">
         <is>
           <t>RuntimeError</t>
@@ -4471,7 +4494,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="115.2" customHeight="1" s="27">
+    <row r="6" ht="115.2" customHeight="1" s="26">
       <c r="A6" s="3" t="inlineStr">
         <is>
           <t>ValueError</t>
@@ -4488,7 +4511,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="115.2" customHeight="1" s="27">
+    <row r="7" ht="115.2" customHeight="1" s="26">
       <c r="A7" s="3" t="inlineStr">
         <is>
           <t>TypeError</t>
@@ -4505,7 +4528,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="100.8" customHeight="1" s="27">
+    <row r="8" ht="100.8" customHeight="1" s="26">
       <c r="A8" s="3" t="inlineStr">
         <is>
           <t>KeyError</t>
@@ -4676,8 +4699,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="26.5546875" bestFit="1" customWidth="1" style="27" min="1" max="1"/>
-    <col width="90.44140625" bestFit="1" customWidth="1" style="27" min="2" max="2"/>
+    <col width="26.5546875" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="90.44140625" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4704,7 +4727,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="3" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A3" t="inlineStr">
         <is>
           <t>ConfigFail_Body</t>
@@ -4731,7 +4754,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="5" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A5" t="inlineStr">
         <is>
           <t>FileNotFound_Body</t>
@@ -4758,7 +4781,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="7" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A7" t="inlineStr">
         <is>
           <t>EmptyInput_Body</t>
@@ -4785,7 +4808,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="9" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A9" t="inlineStr">
         <is>
           <t>EmptyVendorName_Body</t>
@@ -4812,7 +4835,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="11" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A11" t="inlineStr">
         <is>
           <t>EmptyVendorNo_Body</t>
@@ -4839,7 +4862,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="13" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A13" t="inlineStr">
         <is>
           <t>EmptyTax_Body</t>
@@ -4866,7 +4889,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="15" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A15" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -4893,7 +4916,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="17" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A17" t="inlineStr">
         <is>
           <t>SheetMiss_Body</t>
@@ -4920,7 +4943,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="19" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A19" t="inlineStr">
         <is>
           <t>OutputNotFound_Body</t>
@@ -4947,7 +4970,7 @@
         </is>
       </c>
     </row>
-    <row r="21" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="21" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A21" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -4981,11 +5004,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="32.44140625" customWidth="1" style="27" min="1" max="1"/>
-    <col width="106.33203125" customWidth="1" style="27" min="2" max="2"/>
+    <col width="32.44140625" customWidth="1" style="26" min="1" max="1"/>
+    <col width="106.33203125" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" customHeight="1" s="27">
+    <row r="1" ht="15.6" customHeight="1" s="26">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Key</t>
@@ -4997,11 +5020,11 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="15.6" customHeight="1" s="27">
-      <c r="A2" s="26" t="n"/>
-      <c r="B2" s="26" t="n"/>
-    </row>
-    <row r="3" ht="15.6" customHeight="1" s="27">
+    <row r="2" ht="15.6" customHeight="1" s="26">
+      <c r="A2" s="25" t="n"/>
+      <c r="B2" s="25" t="n"/>
+    </row>
+    <row r="3" ht="15.6" customHeight="1" s="26">
       <c r="A3" s="6" t="inlineStr">
         <is>
           <t>Sourcefile_subject</t>
@@ -5013,8 +5036,8 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="15.6" customHeight="1" s="27">
-      <c r="A4" s="26" t="inlineStr">
+    <row r="4" ht="15.6" customHeight="1" s="26">
+      <c r="A4" s="25" t="inlineStr">
         <is>
           <t>Body_mail1</t>
         </is>
@@ -5028,7 +5051,7 @@
     <row r="5">
       <c r="B5" s="19" t="n"/>
     </row>
-    <row r="6" ht="15.6" customHeight="1" s="27">
+    <row r="6" ht="15.6" customHeight="1" s="26">
       <c r="B6" s="8" t="inlineStr">
         <is>
           <t>The given source file is empty. Hence Vendor Wise Concentration process stopped executing.</t>
@@ -5038,34 +5061,34 @@
     <row r="7">
       <c r="B7" s="19" t="n"/>
     </row>
-    <row r="8" ht="15.6" customHeight="1" s="27">
+    <row r="8" ht="15.6" customHeight="1" s="26">
       <c r="B8" s="8" t="inlineStr">
         <is>
           <t>Thanks &amp; Regards,</t>
         </is>
       </c>
     </row>
-    <row r="9" ht="15.6" customHeight="1" s="27">
+    <row r="9" ht="15.6" customHeight="1" s="26">
       <c r="B9" s="8" t="inlineStr">
         <is>
           <t>Ln &amp; Co</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="15.6" customHeight="1" s="27">
-      <c r="A10" s="26" t="inlineStr">
+    <row r="10" ht="15.6" customHeight="1" s="26">
+      <c r="A10" s="25" t="inlineStr">
         <is>
           <t>Gr_amount</t>
         </is>
       </c>
-      <c r="B10" s="26" t="inlineStr">
+      <c r="B10" s="25" t="inlineStr">
         <is>
           <t>Vendor wise concentration -  The GR Amt. in loc.cur. column has no data</t>
         </is>
       </c>
     </row>
-    <row r="11" ht="15.6" customHeight="1" s="27">
-      <c r="A11" s="26" t="inlineStr">
+    <row r="11" ht="15.6" customHeight="1" s="26">
+      <c r="A11" s="25" t="inlineStr">
         <is>
           <t>Gr_amount_body</t>
         </is>
@@ -5079,7 +5102,7 @@
     <row r="12">
       <c r="B12" s="19" t="n"/>
     </row>
-    <row r="13" ht="15.6" customHeight="1" s="27">
+    <row r="13" ht="15.6" customHeight="1" s="26">
       <c r="B13" s="8" t="inlineStr">
         <is>
           <t>GR Amt. in loc.cur. column in source file is empty. Hence the Vendor Wise Concentration  ended executing.</t>
@@ -5089,34 +5112,34 @@
     <row r="14">
       <c r="B14" s="19" t="n"/>
     </row>
-    <row r="15" ht="15.6" customHeight="1" s="27">
+    <row r="15" ht="15.6" customHeight="1" s="26">
       <c r="B15" s="8" t="inlineStr">
         <is>
           <t>Thanks &amp; Regards,</t>
         </is>
       </c>
     </row>
-    <row r="16" ht="15.6" customHeight="1" s="27">
+    <row r="16" ht="15.6" customHeight="1" s="26">
       <c r="B16" s="8" t="inlineStr">
         <is>
           <t>Ln &amp; Co</t>
         </is>
       </c>
     </row>
-    <row r="17" ht="15.6" customHeight="1" s="27">
+    <row r="17" ht="15.6" customHeight="1" s="26">
       <c r="A17" s="6" t="inlineStr">
         <is>
           <t>Vendor_No</t>
         </is>
       </c>
-      <c r="B17" s="26" t="inlineStr">
+      <c r="B17" s="25" t="inlineStr">
         <is>
           <t>Vendor wise concentration -Document is has no data</t>
         </is>
       </c>
     </row>
-    <row r="18" ht="15.6" customHeight="1" s="27">
-      <c r="A18" s="28" t="inlineStr">
+    <row r="18" ht="15.6" customHeight="1" s="26">
+      <c r="A18" s="27" t="inlineStr">
         <is>
           <t>Vendor_No_body</t>
         </is>
@@ -5130,7 +5153,7 @@
     <row r="19">
       <c r="B19" s="19" t="n"/>
     </row>
-    <row r="20" ht="15.6" customHeight="1" s="27">
+    <row r="20" ht="15.6" customHeight="1" s="26">
       <c r="B20" s="8" t="inlineStr">
         <is>
           <t>Vendor class column empty. Hence the Vendor Wise Concentration executing.</t>
@@ -5140,15 +5163,15 @@
     <row r="21">
       <c r="B21" s="19" t="n"/>
     </row>
-    <row r="22" ht="15.6" customHeight="1" s="27">
+    <row r="22" ht="15.6" customHeight="1" s="26">
       <c r="B22" s="8" t="inlineStr">
         <is>
           <t>Thanks &amp; Regards,</t>
         </is>
       </c>
     </row>
-    <row r="23" ht="15.6" customHeight="1" s="27">
-      <c r="A23" s="29" t="n"/>
+    <row r="23" ht="15.6" customHeight="1" s="26">
+      <c r="A23" s="28" t="n"/>
       <c r="B23" s="8" t="inlineStr">
         <is>
           <t>Ln &amp; Co</t>
@@ -5276,8 +5299,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="24.109375" bestFit="1" customWidth="1" style="27" min="1" max="1"/>
-    <col width="90.44140625" bestFit="1" customWidth="1" style="27" min="2" max="2"/>
+    <col width="24.109375" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="90.44140625" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5304,7 +5327,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="3" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A3" t="inlineStr">
         <is>
           <t>FileNotFound_Body</t>
@@ -5331,7 +5354,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="5" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A5" t="inlineStr">
         <is>
           <t>EmptyInput_Body</t>
@@ -5358,7 +5381,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="7" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A7" t="inlineStr">
         <is>
           <t>Key_Body</t>
@@ -5385,7 +5408,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="9" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A9" t="inlineStr">
         <is>
           <t>GRAmt_Subject</t>
@@ -5412,7 +5435,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="11" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A11" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -5439,7 +5462,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="13" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A13" t="inlineStr">
         <is>
           <t>SheetMiss_Body</t>
@@ -5466,7 +5489,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="15" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A15" t="inlineStr">
         <is>
           <t>OutputNotFound_Body</t>
@@ -5493,7 +5516,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="17" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A17" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -5623,11 +5646,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="28.109375" bestFit="1" customWidth="1" style="27" min="1" max="1"/>
-    <col width="86.88671875" bestFit="1" customWidth="1" style="27" min="2" max="2"/>
+    <col width="28.109375" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="86.88671875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.8" customHeight="1" s="27">
+    <row r="1" ht="13.8" customHeight="1" s="26">
       <c r="A1" s="14" t="inlineStr">
         <is>
           <t>Name</t>
@@ -5651,7 +5674,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="3" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A3" t="inlineStr">
         <is>
           <t>FileNotFound_Body</t>
@@ -5678,7 +5701,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="5" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A5" t="inlineStr">
         <is>
           <t>EmptyInput_Body</t>
@@ -5705,7 +5728,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="7" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A7" t="inlineStr">
         <is>
           <t>Plant_Body</t>
@@ -5732,7 +5755,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="9" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A9" t="inlineStr">
         <is>
           <t>GRAmt_Subject</t>
@@ -5759,7 +5782,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="100.8" customHeight="1" s="27">
+    <row r="11" ht="100.8" customHeight="1" s="26">
       <c r="A11" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -5786,7 +5809,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="13" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A13" t="inlineStr">
         <is>
           <t>SheetMiss_Body</t>
@@ -5813,7 +5836,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="15" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A15" t="inlineStr">
         <is>
           <t>OutputNotFound_Body</t>
@@ -5840,7 +5863,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="17" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A17" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -5970,8 +5993,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="28.6640625" bestFit="1" customWidth="1" style="27" min="1" max="1"/>
-    <col width="86.88671875" bestFit="1" customWidth="1" style="27" min="2" max="2"/>
+    <col width="28.6640625" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="86.88671875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5998,7 +6021,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="3" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A3" t="inlineStr">
         <is>
           <t>FileNotFound_Body</t>
@@ -6025,7 +6048,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="5" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A5" t="inlineStr">
         <is>
           <t>EmptyInput_Body</t>
@@ -6052,7 +6075,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="7" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A7" t="inlineStr">
         <is>
           <t>Date_Body</t>
@@ -6079,7 +6102,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="9" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A9" t="inlineStr">
         <is>
           <t>GRAmt_Subject</t>
@@ -6106,7 +6129,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="100.8" customHeight="1" s="27">
+    <row r="11" ht="100.8" customHeight="1" s="26">
       <c r="A11" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -6133,7 +6156,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="13" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A13" t="inlineStr">
         <is>
           <t>SheetMiss_Body</t>
@@ -6160,7 +6183,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="15" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A15" t="inlineStr">
         <is>
           <t>OutputNotFound_Body</t>
@@ -6187,7 +6210,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="86.40000000000001" customHeight="1" s="27">
+    <row r="17" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A17" t="inlineStr">
         <is>
           <t>SystemError_Body</t>

</xml_diff>

<commit_message>
LnCo as on Dec 24 2022
</commit_message>
<xml_diff>
--- a/Lnco/Input/Config.xlsx
+++ b/Lnco/Input/Config.xlsx
@@ -532,10 +532,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B86"/>
+  <dimension ref="A1:B89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="114" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -651,7 +651,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Comparatives_top_weightage</t>
+          <t>Comparatives top weightage</t>
         </is>
       </c>
     </row>
@@ -724,7 +724,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Concentration_top_weightage</t>
+          <t>Concentration top weightage</t>
         </is>
       </c>
     </row>
@@ -741,92 +741,79 @@
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Output_Average_Day_Purchase_sheetname</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Average Day Purchase</t>
-        </is>
-      </c>
-    </row>
+    <row r="21"/>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Output_Same_Material_Purchases_DVDP_sheetname</t>
+          <t>Output_Average_Day_Purchase_sheetname</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>SMP from DVnDP</t>
+          <t>Average Day Purchase</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>Output_Average_Day_Weightage_Sheetname</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Average Day Purchase top rows</t>
+        </is>
+      </c>
+    </row>
+    <row r="24"/>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Output_Same_Material_Purchases_DVDP_sheetname</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>SMP from DVnDP</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>Output_Unit_Price_Comparison_sheetname</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B26" t="inlineStr">
         <is>
           <t>Unit Price Comparison</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
+    <row r="27">
+      <c r="A27" t="inlineStr">
         <is>
           <t>Output_Inventory_Mapping_Sheetname</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B27" t="inlineStr">
         <is>
           <t>Inventory Mapping</t>
         </is>
       </c>
     </row>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27">
-      <c r="A27" s="21" t="inlineStr">
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30">
+      <c r="A30" s="21" t="inlineStr">
         <is>
           <t>Other Keys</t>
         </is>
       </c>
-      <c r="B27" s="21" t="inlineStr">
+      <c r="B30" s="21" t="inlineStr">
         <is>
           <t>Other Values</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" s="15" t="n"/>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>purchase_register_1st_column_name</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Plant</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>purchase_register_2nd_column_name</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>GR Document Number</t>
         </is>
       </c>
     </row>
@@ -836,7 +823,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>MB51_first_column</t>
+          <t>purchase_register_1st_column_name</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -848,409 +835,408 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>MB51_second_column</t>
+          <t>purchase_register_2nd_column_name</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Material</t>
-        </is>
-      </c>
-    </row>
-    <row r="34"/>
+          <t>GR Document Number</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" s="15" t="n"/>
+    </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>LOCAL_DOTENV_FILE</t>
+          <t>MB51_first_column</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>local_new.env</t>
+          <t>Plant</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>QUALITY_DOTENV_FILE</t>
+          <t>MB51_second_column</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>quality.env</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>ENV_FILE</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
+          <t>Material</t>
+        </is>
+      </c>
+    </row>
+    <row r="37"/>
+    <row r="38">
+      <c r="A38" t="inlineStr">
         <is>
           <t>LOCAL_DOTENV_FILE</t>
         </is>
       </c>
-    </row>
-    <row r="38"/>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>local_new.env</t>
+        </is>
+      </c>
+    </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Request Status Name</t>
+          <t>QUALITY_DOTENV_FILE</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Request Status Name</t>
+          <t>quality.env</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>New_Request_Status</t>
+          <t>ENV_FILE</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>New</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>In_Progress_Request_Status</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>In Progress</t>
-        </is>
-      </c>
-    </row>
+          <t>LOCAL_DOTENV_FILE</t>
+        </is>
+      </c>
+    </row>
+    <row r="41"/>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Success_Request_Status</t>
+          <t>Request Status Name</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Completed</t>
+          <t>Request Status Name</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Fail_Request_Status</t>
+          <t>New_Request_Status</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Failed</t>
-        </is>
-      </c>
-    </row>
-    <row r="44"/>
+          <t>New</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>In_Progress_Request_Status</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
+      </c>
+    </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>To_Mail_Address</t>
-        </is>
-      </c>
-      <c r="B45" s="15" t="inlineStr">
-        <is>
-          <t>kalyan.gundu@bradsol.com</t>
+          <t>Success_Request_Status</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Completed</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
+          <t>Fail_Request_Status</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+    </row>
+    <row r="47"/>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>To_Mail_Address</t>
+        </is>
+      </c>
+      <c r="B48" s="15" t="inlineStr">
+        <is>
+          <t>kalyan.gundu@bradsol.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
           <t>CC_Mail_Address</t>
         </is>
       </c>
-      <c r="B46" s="15" t="inlineStr">
+      <c r="B49" s="15" t="inlineStr">
         <is>
           <t>kalyan.gundu@bradsol.com</t>
         </is>
       </c>
-    </row>
-    <row r="47">
-      <c r="B47" s="23" t="n"/>
-    </row>
-    <row r="48">
-      <c r="B48" s="23" t="n"/>
-    </row>
-    <row r="49">
-      <c r="B49" s="23" t="n"/>
     </row>
     <row r="50">
       <c r="B50" s="23" t="n"/>
     </row>
-    <row r="51"/>
-    <row r="52"/>
+    <row r="51">
+      <c r="B51" s="23" t="n"/>
+    </row>
+    <row r="52">
+      <c r="B52" s="23" t="n"/>
+    </row>
     <row r="53">
-      <c r="A53" s="21" t="inlineStr">
+      <c r="B53" s="23" t="n"/>
+    </row>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56">
+      <c r="A56" s="21" t="inlineStr">
         <is>
           <t>Sheet Name keys in Config File</t>
         </is>
       </c>
-      <c r="B53" s="21" t="inlineStr">
+      <c r="B56" s="21" t="inlineStr">
         <is>
           <t>SheetName values in Config file</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>Config_Comparatives_Purchase_sheetname</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Purchase Wise Comparatives</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>Config_Comparatives_Month_sheetname</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Month Wise Comparatives</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>Config_Comparatives_Plant_sheetname</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>Plant Wise Comparatives</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Config_Comparatives_Dom&amp;Imp_sheetname</t>
+          <t>Config_Comparatives_Purchase_sheetname</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Dom&amp;Imp Wise Comparatives</t>
+          <t>Purchase Wise Comparatives</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Config_Comparatives_Vendor_sheetname</t>
+          <t>Config_Comparatives_Month_sheetname</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Vendor Wise Comparatives</t>
-        </is>
-      </c>
-    </row>
-    <row r="59"/>
+          <t>Month Wise Comparatives</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Config_Comparatives_Plant_sheetname</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Plant Wise Comparatives</t>
+        </is>
+      </c>
+    </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Config_Concentrations_Purchase_sheetname</t>
+          <t>Config_Comparatives_Dom&amp;Imp_sheetname</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Purchase Wise Concentration</t>
+          <t>Dom&amp;Imp Wise Comparatives</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Config_Concentrations_Month_sheetname</t>
+          <t>Config_Comparatives_Vendor_sheetname</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Month Wise Concentration</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>Config_Concentrations_Plant_sheetname</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>Plant Wise Concentration</t>
-        </is>
-      </c>
-    </row>
+          <t>Vendor Wise Comparatives</t>
+        </is>
+      </c>
+    </row>
+    <row r="62"/>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Config_Concentrations_Dom&amp;Imp_sheetname</t>
+          <t>Config_Concentrations_Purchase_sheetname</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Dom&amp;Imp Wise Concentration</t>
+          <t>Purchase Wise Concentration</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Config_Concentration_Vendor_sheetname</t>
+          <t>Config_Concentrations_Month_sheetname</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Vendor Wise Concentration</t>
-        </is>
-      </c>
-    </row>
-    <row r="65"/>
+          <t>Month Wise Concentration</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Config_Concentrations_Plant_sheetname</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Plant Wise Concentration</t>
+        </is>
+      </c>
+    </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Config_Duplication_of_Vendor_sheetname</t>
+          <t>Config_Concentrations_Dom&amp;Imp_sheetname</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Duplication Of Vendor</t>
+          <t>Dom&amp;Imp Wise Concentration</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Config_Average_Day_Purchase_sheetname</t>
+          <t>Config_Concentration_Vendor_sheetname</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Average Day Purchase</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Config_Same_Material_Purchases_DVDP_sheetname</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>SMP from DVnDP</t>
-        </is>
-      </c>
-    </row>
+          <t>Vendor Wise Concentration</t>
+        </is>
+      </c>
+    </row>
+    <row r="68"/>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Config_Unit_Price_Comparison_sheetname</t>
+          <t>Config_Duplication_of_Vendor_sheetname</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Unit Price Comparison</t>
+          <t>Duplication Of Vendor</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Config_Inventory_Mapping_Sheetname</t>
+          <t>Config_Average_Day_Purchase_sheetname</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Inventory Mapping</t>
-        </is>
-      </c>
-    </row>
-    <row r="71"/>
+          <t>Average Day Purchase</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Config_Same_Material_Purchases_DVDP_sheetname</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>SMP from DVnDP</t>
+        </is>
+      </c>
+    </row>
     <row r="72">
-      <c r="A72" s="21" t="inlineStr">
-        <is>
-          <t>Mails related Keys</t>
-        </is>
-      </c>
-      <c r="B72" s="21" t="inlineStr">
-        <is>
-          <t>Values</t>
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Config_Unit_Price_Comparison_sheetname</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Unit Price Comparison</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Start_Mail_Subject</t>
+          <t>Config_Inventory_Mapping_Sheetname</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bot execution is started </t>
-        </is>
-      </c>
-    </row>
-    <row r="74" ht="86.40000000000001" customHeight="1" s="26">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>Start_Mail_Body</t>
-        </is>
-      </c>
-      <c r="B74" s="19" t="inlineStr">
-        <is>
-          <t>Hello,
-Bot has started processing the purchase register report automation
-Thanks &amp; Regards,
- LN &amp; Co</t>
-        </is>
-      </c>
-    </row>
-    <row r="75"/>
+          <t>Inventory Mapping</t>
+        </is>
+      </c>
+    </row>
+    <row r="74"/>
+    <row r="75">
+      <c r="A75" s="21" t="inlineStr">
+        <is>
+          <t>Mails related Keys</t>
+        </is>
+      </c>
+      <c r="B75" s="21" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Success_Mail_Subject</t>
+          <t>Start_Mail_Subject</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bot execution is completed </t>
+          <t xml:space="preserve">Bot execution is started </t>
         </is>
       </c>
     </row>
     <row r="77" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Success_Mail_Body</t>
+          <t>Start_Mail_Body</t>
         </is>
       </c>
       <c r="B77" s="19" t="inlineStr">
         <is>
           <t>Hello,
-Bot has Successfully completed the purchase register report automation.
+Bot has started processing the purchase register report automation
 Thanks &amp; Regards,
  LN &amp; Co</t>
         </is>
@@ -1260,22 +1246,50 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
+          <t>Success_Mail_Subject</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bot execution is completed </t>
+        </is>
+      </c>
+    </row>
+    <row r="80" ht="86.40000000000001" customHeight="1" s="26">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Success_Mail_Body</t>
+        </is>
+      </c>
+      <c r="B80" s="19" t="inlineStr">
+        <is>
+          <t>Hello,
+Bot has Successfully completed the purchase register report automation.
+Thanks &amp; Regards,
+ LN &amp; Co</t>
+        </is>
+      </c>
+    </row>
+    <row r="81"/>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
           <t>subject_file_not_found</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr">
+      <c r="B82" t="inlineStr">
         <is>
           <t>Bot Execution is stopped - Input file is missing</t>
         </is>
       </c>
     </row>
-    <row r="80" ht="100.8" customHeight="1" s="26">
-      <c r="A80" t="inlineStr">
+    <row r="83" ht="100.8" customHeight="1" s="26">
+      <c r="A83" t="inlineStr">
         <is>
           <t>body_file_not_found</t>
         </is>
       </c>
-      <c r="B80" s="17" t="inlineStr">
+      <c r="B83" s="17" t="inlineStr">
         <is>
           <t xml:space="preserve">Hello,
 Purchase Register Input File is Missing. Hence stopping the execution of the program.
@@ -1285,28 +1299,28 @@
         </is>
       </c>
     </row>
-    <row r="81">
-      <c r="B81" s="13" t="n"/>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
+    <row r="84">
+      <c r="B84" s="13" t="n"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
         <is>
           <t>subject_sheet_not_found</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr">
+      <c r="B85" t="inlineStr">
         <is>
           <t>Bot Execution is stopped - Input file sheet is missing</t>
         </is>
       </c>
     </row>
-    <row r="83" ht="100.8" customHeight="1" s="26">
-      <c r="A83" t="inlineStr">
+    <row r="86" ht="100.8" customHeight="1" s="26">
+      <c r="A86" t="inlineStr">
         <is>
           <t>body_sheet_not_found</t>
         </is>
       </c>
-      <c r="B83" s="17" t="inlineStr">
+      <c r="B86" s="17" t="inlineStr">
         <is>
           <t xml:space="preserve">Hello,
 Purchase Register Input File sheet is Missing. Hence stopping the execution of the program.
@@ -1316,26 +1330,26 @@
         </is>
       </c>
     </row>
-    <row r="84"/>
-    <row r="85">
-      <c r="A85" t="inlineStr">
+    <row r="87"/>
+    <row r="88">
+      <c r="A88" t="inlineStr">
         <is>
           <t>subject_in_progress_request_found</t>
         </is>
       </c>
-      <c r="B85" t="inlineStr">
+      <c r="B88" t="inlineStr">
         <is>
           <t>Bot Execution is stopped - prior requests are in progress</t>
         </is>
       </c>
     </row>
-    <row r="86" ht="100.8" customHeight="1" s="26">
-      <c r="A86" t="inlineStr">
+    <row r="89" ht="100.8" customHeight="1" s="26">
+      <c r="A89" t="inlineStr">
         <is>
           <t>body_in_progress_request_found</t>
         </is>
       </c>
-      <c r="B86" s="17" t="inlineStr">
+      <c r="B89" s="17" t="inlineStr">
         <is>
           <t xml:space="preserve">Hello,
 The bot is executing prior requests. Hence stopping the execution of the program.
@@ -1347,13 +1361,13 @@
     </row>
   </sheetData>
   <dataValidations xWindow="832" yWindow="791" count="1">
-    <dataValidation sqref="B37:B38" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Select Correct File" error="Should be same as Input message provided" promptTitle="Select Env File type" prompt="LOCAL_DOTENV_FILE (or) QUALTIY_DOTENV_FILE" type="list">
-      <formula1>$A$35:$A$36</formula1>
+    <dataValidation sqref="B40:B41" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Select Correct File" error="Should be same as Input message provided" promptTitle="Select Env File type" prompt="LOCAL_DOTENV_FILE (or) QUALTIY_DOTENV_FILE" type="list">
+      <formula1>$A$38:$A$39</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B45" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B46" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B48" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B49" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
LnCo as on 25 Dec
</commit_message>
<xml_diff>
--- a/Lnco/Input/Config.xlsx
+++ b/Lnco/Input/Config.xlsx
@@ -132,7 +132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
@@ -188,6 +188,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,17 +533,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B89"/>
+  <dimension ref="A1:B95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="114" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="114" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="48.5546875" customWidth="1" style="26" min="1" max="1"/>
-    <col width="84.21875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
-    <col width="30.77734375" bestFit="1" customWidth="1" style="26" min="4" max="4"/>
+    <col width="48.5546875" customWidth="1" style="29" min="1" max="1"/>
+    <col width="84.21875" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
+    <col width="30.77734375" bestFit="1" customWidth="1" style="29" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -651,7 +652,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Comparatives top weightage</t>
+          <t>exceptions – COMPARITIVES</t>
         </is>
       </c>
     </row>
@@ -724,7 +725,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Concentration top weightage</t>
+          <t>exceptions – CONCENTRATIONS</t>
         </is>
       </c>
     </row>
@@ -755,14 +756,14 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="21" t="inlineStr">
         <is>
           <t>Output_Average_Day_Weightage_Sheetname</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Average Day Purchase top rows</t>
+          <t>exceptions average day</t>
         </is>
       </c>
     </row>
@@ -779,193 +780,171 @@
         </is>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Output_Unit_Price_Comparison_sheetname</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Unit Price Comparison</t>
-        </is>
-      </c>
-    </row>
+    <row r="26"/>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Output_Inventory_Mapping_Sheetname</t>
+          <t>Output_Unit_Price_Comparison_sheetname</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Inventory Mapping</t>
-        </is>
-      </c>
-    </row>
-    <row r="28"/>
+          <t>Unit Price Comparison</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="21" t="inlineStr">
+        <is>
+          <t>Output_Unit_Price_Exceptions_sheetname</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>exceptions unit price</t>
+        </is>
+      </c>
+    </row>
     <row r="29"/>
     <row r="30">
-      <c r="A30" s="21" t="inlineStr">
-        <is>
-          <t>Other Keys</t>
-        </is>
-      </c>
-      <c r="B30" s="21" t="inlineStr">
-        <is>
-          <t>Other Values</t>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Output_Inventory_Mapping_Sheetname</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Inventory Mapping</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="B31" s="15" t="n"/>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>purchase_register_1st_column_name</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Plant</t>
-        </is>
-      </c>
-    </row>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Output_inventory_mapping_exceptions_sheetname</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>exceptions – inventory mapping</t>
+        </is>
+      </c>
+    </row>
+    <row r="32"/>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>purchase_register_2nd_column_name</t>
+          <t>Output_Security_Cutoff_Sheet_name</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>GR Document Number</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="B34" s="15" t="n"/>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>MB51_first_column</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Plant</t>
-        </is>
-      </c>
-    </row>
+          <t>Security Cutoff</t>
+        </is>
+      </c>
+    </row>
+    <row r="34"/>
+    <row r="35"/>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>MB51_second_column</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Material</t>
-        </is>
-      </c>
-    </row>
-    <row r="37"/>
+      <c r="A36" s="21" t="inlineStr">
+        <is>
+          <t>Other Keys</t>
+        </is>
+      </c>
+      <c r="B36" s="21" t="inlineStr">
+        <is>
+          <t>Other Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" s="15" t="n"/>
+    </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>LOCAL_DOTENV_FILE</t>
+          <t>purchase_register_1st_column_name</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>local_new.env</t>
+          <t>Plant</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>QUALITY_DOTENV_FILE</t>
+          <t>purchase_register_2nd_column_name</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>quality.env</t>
+          <t>GR Document Number</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>ENV_FILE</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>LOCAL_DOTENV_FILE</t>
-        </is>
-      </c>
-    </row>
-    <row r="41"/>
+      <c r="B40" s="15" t="n"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>MB51_first_column</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Plant</t>
+        </is>
+      </c>
+    </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Request Status Name</t>
+          <t>MB51_second_column</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Request Status Name</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>New_Request_Status</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>New</t>
-        </is>
-      </c>
-    </row>
+          <t>Material</t>
+        </is>
+      </c>
+    </row>
+    <row r="43"/>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>In_Progress_Request_Status</t>
+          <t>LOCAL_DOTENV_FILE</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>In Progress</t>
+          <t>local_new.env</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Success_Request_Status</t>
+          <t>QUALITY_DOTENV_FILE</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Completed</t>
+          <t>quality.env</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Fail_Request_Status</t>
+          <t>ENV_FILE</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Failed</t>
+          <t>LOCAL_DOTENV_FILE</t>
         </is>
       </c>
     </row>
@@ -973,171 +952,171 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>To_Mail_Address</t>
-        </is>
-      </c>
-      <c r="B48" s="15" t="inlineStr">
-        <is>
-          <t>kalyan.gundu@bradsol.com</t>
+          <t>Request Status Name</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Request Status Name</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
+          <t>New_Request_Status</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>In_Progress_Request_Status</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Success_Request_Status</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Fail_Request_Status</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+    </row>
+    <row r="53"/>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>To_Mail_Address</t>
+        </is>
+      </c>
+      <c r="B54" s="15" t="inlineStr">
+        <is>
+          <t>kalyan.gundu@bradsol.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
           <t>CC_Mail_Address</t>
         </is>
       </c>
-      <c r="B49" s="15" t="inlineStr">
+      <c r="B55" s="15" t="inlineStr">
         <is>
           <t>kalyan.gundu@bradsol.com</t>
         </is>
       </c>
     </row>
-    <row r="50">
-      <c r="B50" s="23" t="n"/>
-    </row>
-    <row r="51">
-      <c r="B51" s="23" t="n"/>
-    </row>
-    <row r="52">
-      <c r="B52" s="23" t="n"/>
-    </row>
-    <row r="53">
-      <c r="B53" s="23" t="n"/>
-    </row>
-    <row r="54"/>
-    <row r="55"/>
     <row r="56">
-      <c r="A56" s="21" t="inlineStr">
+      <c r="B56" s="23" t="n"/>
+    </row>
+    <row r="57">
+      <c r="B57" s="23" t="n"/>
+    </row>
+    <row r="58">
+      <c r="B58" s="23" t="n"/>
+    </row>
+    <row r="59">
+      <c r="B59" s="23" t="n"/>
+    </row>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62">
+      <c r="A62" s="21" t="inlineStr">
         <is>
           <t>Sheet Name keys in Config File</t>
         </is>
       </c>
-      <c r="B56" s="21" t="inlineStr">
+      <c r="B62" s="21" t="inlineStr">
         <is>
           <t>SheetName values in Config file</t>
         </is>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>Config_Comparatives_Purchase_sheetname</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Purchase Wise Comparatives</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>Config_Comparatives_Month_sheetname</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>Month Wise Comparatives</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>Config_Comparatives_Plant_sheetname</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>Plant Wise Comparatives</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>Config_Comparatives_Dom&amp;Imp_sheetname</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>Dom&amp;Imp Wise Comparatives</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>Config_Comparatives_Vendor_sheetname</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>Vendor Wise Comparatives</t>
-        </is>
-      </c>
-    </row>
-    <row r="62"/>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Config_Concentrations_Purchase_sheetname</t>
+          <t>Config_Comparatives_Purchase_sheetname</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Purchase Wise Concentration</t>
+          <t>Purchase Wise Comparatives</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Config_Concentrations_Month_sheetname</t>
+          <t>Config_Comparatives_Month_sheetname</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Month Wise Concentration</t>
+          <t>Month Wise Comparatives</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Config_Concentrations_Plant_sheetname</t>
+          <t>Config_Comparatives_Plant_sheetname</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Plant Wise Concentration</t>
+          <t>Plant Wise Comparatives</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Config_Concentrations_Dom&amp;Imp_sheetname</t>
+          <t>Config_Comparatives_Dom&amp;Imp_sheetname</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Dom&amp;Imp Wise Concentration</t>
+          <t>Dom&amp;Imp Wise Comparatives</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Config_Concentration_Vendor_sheetname</t>
+          <t>Config_Comparatives_Vendor_sheetname</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Vendor Wise Concentration</t>
+          <t>Vendor Wise Comparatives</t>
         </is>
       </c>
     </row>
@@ -1145,188 +1124,189 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Config_Duplication_of_Vendor_sheetname</t>
+          <t>Config_Concentrations_Purchase_sheetname</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Duplication Of Vendor</t>
+          <t>Purchase Wise Concentration</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Config_Average_Day_Purchase_sheetname</t>
+          <t>Config_Concentrations_Month_sheetname</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Average Day Purchase</t>
+          <t>Month Wise Concentration</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Config_Same_Material_Purchases_DVDP_sheetname</t>
+          <t>Config_Concentrations_Plant_sheetname</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>SMP from DVnDP</t>
+          <t>Plant Wise Concentration</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Config_Unit_Price_Comparison_sheetname</t>
+          <t>Config_Concentrations_Dom&amp;Imp_sheetname</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Unit Price Comparison</t>
+          <t>Dom&amp;Imp Wise Concentration</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Config_Inventory_Mapping_Sheetname</t>
+          <t>Config_Concentration_Vendor_sheetname</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Inventory Mapping</t>
+          <t>Vendor Wise Concentration</t>
         </is>
       </c>
     </row>
     <row r="74"/>
     <row r="75">
-      <c r="A75" s="21" t="inlineStr">
-        <is>
-          <t>Mails related Keys</t>
-        </is>
-      </c>
-      <c r="B75" s="21" t="inlineStr">
-        <is>
-          <t>Values</t>
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Config_Duplication_of_Vendor_sheetname</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Duplication Of Vendor</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Start_Mail_Subject</t>
+          <t>Config_Average_Day_Purchase_sheetname</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bot execution is started </t>
-        </is>
-      </c>
-    </row>
-    <row r="77" ht="86.40000000000001" customHeight="1" s="26">
+          <t>Average Day Purchase</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Start_Mail_Body</t>
-        </is>
-      </c>
-      <c r="B77" s="19" t="inlineStr">
-        <is>
-          <t>Hello,
-Bot has started processing the purchase register report automation
-Thanks &amp; Regards,
- LN &amp; Co</t>
-        </is>
-      </c>
-    </row>
-    <row r="78"/>
+          <t>Config_Same_Material_Purchases_DVDP_sheetname</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>SMP from DVnDP</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Config_Unit_Price_Comparison_sheetname</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Unit Price Comparison</t>
+        </is>
+      </c>
+    </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Success_Mail_Subject</t>
+          <t>Config_Inventory_Mapping_Sheetname</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bot execution is completed </t>
-        </is>
-      </c>
-    </row>
-    <row r="80" ht="86.40000000000001" customHeight="1" s="26">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>Success_Mail_Body</t>
-        </is>
-      </c>
-      <c r="B80" s="19" t="inlineStr">
-        <is>
-          <t>Hello,
-Bot has Successfully completed the purchase register report automation.
-Thanks &amp; Regards,
- LN &amp; Co</t>
-        </is>
-      </c>
-    </row>
-    <row r="81"/>
+          <t>Inventory Mapping</t>
+        </is>
+      </c>
+    </row>
+    <row r="80"/>
+    <row r="81">
+      <c r="A81" s="21" t="inlineStr">
+        <is>
+          <t>Mails related Keys</t>
+        </is>
+      </c>
+      <c r="B81" s="21" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>subject_file_not_found</t>
+          <t>Start_Mail_Subject</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Bot Execution is stopped - Input file is missing</t>
-        </is>
-      </c>
-    </row>
-    <row r="83" ht="100.8" customHeight="1" s="26">
+          <t xml:space="preserve">Bot execution is started </t>
+        </is>
+      </c>
+    </row>
+    <row r="83" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A83" t="inlineStr">
         <is>
-          <t>body_file_not_found</t>
-        </is>
-      </c>
-      <c r="B83" s="17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Hello,
-Purchase Register Input File is Missing. Hence stopping the execution of the program.
-Thanks &amp; Regards,
-L &amp; Co
-                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                              </t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="B84" s="13" t="n"/>
-    </row>
+          <t>Start_Mail_Body</t>
+        </is>
+      </c>
+      <c r="B83" s="19" t="inlineStr">
+        <is>
+          <t>Hello,
+Bot has started processing the purchase register report automation
+Thanks &amp; Regards,
+ LN &amp; Co</t>
+        </is>
+      </c>
+    </row>
+    <row r="84"/>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>subject_sheet_not_found</t>
+          <t>Success_Mail_Subject</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Bot Execution is stopped - Input file sheet is missing</t>
-        </is>
-      </c>
-    </row>
-    <row r="86" ht="100.8" customHeight="1" s="26">
+          <t xml:space="preserve">Bot execution is completed </t>
+        </is>
+      </c>
+    </row>
+    <row r="86" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A86" t="inlineStr">
         <is>
-          <t>body_sheet_not_found</t>
-        </is>
-      </c>
-      <c r="B86" s="17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Hello,
-Purchase Register Input File sheet is Missing. Hence stopping the execution of the program.
-Thanks &amp; Regards,
-L &amp; Co
-                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                              </t>
+          <t>Success_Mail_Body</t>
+        </is>
+      </c>
+      <c r="B86" s="19" t="inlineStr">
+        <is>
+          <t>Hello,
+Bot has Successfully completed the purchase register report automation.
+Thanks &amp; Regards,
+ LN &amp; Co</t>
         </is>
       </c>
     </row>
@@ -1334,22 +1314,82 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
+          <t>subject_file_not_found</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Bot Execution is stopped - Input file is missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="89" ht="100.8" customHeight="1" s="29">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>body_file_not_found</t>
+        </is>
+      </c>
+      <c r="B89" s="17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello,
+Purchase Register Input File is Missing. Hence stopping the execution of the program.
+Thanks &amp; Regards,
+L &amp; Co
+                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                              </t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="B90" s="13" t="n"/>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>subject_sheet_not_found</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Bot Execution is stopped - Input file sheet is missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="92" ht="100.8" customHeight="1" s="29">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>body_sheet_not_found</t>
+        </is>
+      </c>
+      <c r="B92" s="17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello,
+Purchase Register Input File sheet is Missing. Hence stopping the execution of the program.
+Thanks &amp; Regards,
+L &amp; Co
+                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                              </t>
+        </is>
+      </c>
+    </row>
+    <row r="93"/>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
           <t>subject_in_progress_request_found</t>
         </is>
       </c>
-      <c r="B88" t="inlineStr">
+      <c r="B94" t="inlineStr">
         <is>
           <t>Bot Execution is stopped - prior requests are in progress</t>
         </is>
       </c>
     </row>
-    <row r="89" ht="100.8" customHeight="1" s="26">
-      <c r="A89" t="inlineStr">
+    <row r="95" ht="100.8" customHeight="1" s="29">
+      <c r="A95" t="inlineStr">
         <is>
           <t>body_in_progress_request_found</t>
         </is>
       </c>
-      <c r="B89" s="17" t="inlineStr">
+      <c r="B95" s="17" t="inlineStr">
         <is>
           <t xml:space="preserve">Hello,
 The bot is executing prior requests. Hence stopping the execution of the program.
@@ -1361,13 +1401,13 @@
     </row>
   </sheetData>
   <dataValidations xWindow="832" yWindow="791" count="1">
-    <dataValidation sqref="B40:B41" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Select Correct File" error="Should be same as Input message provided" promptTitle="Select Env File type" prompt="LOCAL_DOTENV_FILE (or) QUALTIY_DOTENV_FILE" type="list">
-      <formula1>$A$38:$A$39</formula1>
+    <dataValidation sqref="B46:B47" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Select Correct File" error="Should be same as Input message provided" promptTitle="Select Env File type" prompt="LOCAL_DOTENV_FILE (or) QUALTIY_DOTENV_FILE" type="list">
+      <formula1>$A$44:$A$45</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B48" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B49" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B54" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B55" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -1388,10 +1428,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="24.5546875" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
-    <col width="92.33203125" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
-    <col width="43.6640625" customWidth="1" style="26" min="5" max="5"/>
-    <col width="36.109375" customWidth="1" style="26" min="6" max="6"/>
+    <col width="24.5546875" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
+    <col width="92.33203125" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
+    <col width="43.6640625" customWidth="1" style="29" min="5" max="5"/>
+    <col width="36.109375" customWidth="1" style="29" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1418,7 +1458,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="3" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A3" s="3" t="inlineStr">
         <is>
           <t>FileNotFound_Body</t>
@@ -1445,7 +1485,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="5" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A5" s="3" t="inlineStr">
         <is>
           <t>EmptyInput_Body</t>
@@ -1472,7 +1512,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="7" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A7" s="3" t="inlineStr">
         <is>
           <t>EmptyValClass_Body</t>
@@ -1499,7 +1539,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="9" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A9" s="3" t="inlineStr">
         <is>
           <t>EmptyValClassTxt_Body</t>
@@ -1526,7 +1566,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="11" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A11" s="3" t="inlineStr">
         <is>
           <t>GRAmt_Subject</t>
@@ -1553,7 +1593,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="13" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A13" s="3" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -1580,7 +1620,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="15" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A15" s="3" t="inlineStr">
         <is>
           <t>SheetMiss_Body</t>
@@ -1607,7 +1647,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="17" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A17" s="3" t="inlineStr">
         <is>
           <t>OutputNotFound_Body</t>
@@ -1634,7 +1674,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="19" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A19" s="3" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -1764,8 +1804,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="49.33203125" customWidth="1" style="26" min="1" max="1"/>
-    <col width="83.88671875" customWidth="1" style="26" min="2" max="2"/>
+    <col width="49.33203125" customWidth="1" style="29" min="1" max="1"/>
+    <col width="83.88671875" customWidth="1" style="29" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1792,7 +1832,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="100.8" customHeight="1" s="26">
+    <row r="3" ht="100.8" customHeight="1" s="29">
       <c r="A3" t="inlineStr">
         <is>
           <t>Vendor No._Body</t>
@@ -1820,7 +1860,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="100.8" customHeight="1" s="26">
+    <row r="5" ht="100.8" customHeight="1" s="29">
       <c r="A5" t="inlineStr">
         <is>
           <t>Vendor Name_Body</t>
@@ -1848,7 +1888,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="100.8" customHeight="1" s="26">
+    <row r="7" ht="100.8" customHeight="1" s="29">
       <c r="A7" t="inlineStr">
         <is>
           <t>Gr Amt_Body</t>
@@ -1876,7 +1916,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="9" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A9" t="inlineStr">
         <is>
           <t>FileNotFound_Body</t>
@@ -1903,7 +1943,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="11" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A11" t="inlineStr">
         <is>
           <t>EmptyInput_Body</t>
@@ -1918,7 +1958,7 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="12" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A12" t="inlineStr">
         <is>
           <t>EmptyInput_Body1</t>
@@ -1945,7 +1985,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="14" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A14" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -1960,7 +2000,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="15" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A15" t="inlineStr">
         <is>
           <t>ColumnMiss_Body1</t>
@@ -1987,7 +2027,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="17" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A17" t="inlineStr">
         <is>
           <t>SheetMiss_Body</t>
@@ -2014,7 +2054,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="19" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A19" t="inlineStr">
         <is>
           <t>OutputNotFound_Body</t>
@@ -2041,7 +2081,7 @@
         </is>
       </c>
     </row>
-    <row r="21" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="21" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A21" t="inlineStr">
         <is>
           <t>SystemE_Body</t>
@@ -2068,7 +2108,7 @@
         </is>
       </c>
     </row>
-    <row r="23" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="23" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A23" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -2198,8 +2238,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="35.5546875" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
-    <col width="86.88671875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
+    <col width="35.5546875" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
+    <col width="86.88671875" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2226,7 +2266,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="100.8" customHeight="1" s="26">
+    <row r="4" ht="100.8" customHeight="1" s="29">
       <c r="A4" t="inlineStr">
         <is>
           <t>Body_mail</t>
@@ -2254,7 +2294,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="100.8" customHeight="1" s="26">
+    <row r="7" ht="100.8" customHeight="1" s="29">
       <c r="A7" t="inlineStr">
         <is>
           <t>body_file_not_found</t>
@@ -2285,7 +2325,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="100.8" customHeight="1" s="26">
+    <row r="10" ht="100.8" customHeight="1" s="29">
       <c r="A10" t="inlineStr">
         <is>
           <t>Gr Amt_Body</t>
@@ -2313,7 +2353,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="100.8" customHeight="1" s="26">
+    <row r="13" ht="100.8" customHeight="1" s="29">
       <c r="A13" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -2341,7 +2381,7 @@
         </is>
       </c>
     </row>
-    <row r="16" ht="100.8" customHeight="1" s="26">
+    <row r="16" ht="100.8" customHeight="1" s="29">
       <c r="A16" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -2472,8 +2512,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="24.5546875" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
-    <col width="86.88671875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
+    <col width="24.5546875" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
+    <col width="86.88671875" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2500,7 +2540,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="100.8" customHeight="1" s="26">
+    <row r="4" ht="100.8" customHeight="1" s="29">
       <c r="A4" t="inlineStr">
         <is>
           <t>Body_mail</t>
@@ -2528,7 +2568,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="100.8" customHeight="1" s="26">
+    <row r="6" ht="100.8" customHeight="1" s="29">
       <c r="A6" t="inlineStr">
         <is>
           <t>Plant_Body</t>
@@ -2562,7 +2602,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="100.8" customHeight="1" s="26">
+    <row r="10" ht="100.8" customHeight="1" s="29">
       <c r="A10" t="inlineStr">
         <is>
           <t>Gr Amt_Body</t>
@@ -2590,7 +2630,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="100.8" customHeight="1" s="26">
+    <row r="13" ht="100.8" customHeight="1" s="29">
       <c r="A13" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -2621,7 +2661,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="100.8" customHeight="1" s="26">
+    <row r="19" ht="100.8" customHeight="1" s="29">
       <c r="A19" t="inlineStr">
         <is>
           <t>body_file_not_found</t>
@@ -2649,7 +2689,7 @@
         </is>
       </c>
     </row>
-    <row r="22" ht="100.8" customHeight="1" s="26">
+    <row r="22" ht="100.8" customHeight="1" s="29">
       <c r="A22" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -2780,8 +2820,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="17.88671875" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
-    <col width="86.88671875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
+    <col width="17.88671875" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
+    <col width="86.88671875" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2808,7 +2848,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="100.8" customHeight="1" s="26">
+    <row r="4" ht="100.8" customHeight="1" s="29">
       <c r="A4" t="inlineStr">
         <is>
           <t>Body_mail</t>
@@ -2836,7 +2876,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="100.8" customHeight="1" s="26">
+    <row r="6" ht="100.8" customHeight="1" s="29">
       <c r="A6" t="inlineStr">
         <is>
           <t>Month_Body</t>
@@ -2870,7 +2910,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="100.8" customHeight="1" s="26">
+    <row r="10" ht="100.8" customHeight="1" s="29">
       <c r="A10" t="inlineStr">
         <is>
           <t>Gr Amt_Body</t>
@@ -2901,7 +2941,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="100.8" customHeight="1" s="26">
+    <row r="13" ht="100.8" customHeight="1" s="29">
       <c r="A13" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -2932,7 +2972,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="100.8" customHeight="1" s="26">
+    <row r="19" ht="100.8" customHeight="1" s="29">
       <c r="A19" t="inlineStr">
         <is>
           <t>body_file_not_found</t>
@@ -2960,7 +3000,7 @@
         </is>
       </c>
     </row>
-    <row r="22" ht="100.8" customHeight="1" s="26">
+    <row r="22" ht="100.8" customHeight="1" s="29">
       <c r="A22" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -3091,8 +3131,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="26.88671875" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
-    <col width="91.88671875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
+    <col width="26.88671875" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
+    <col width="91.88671875" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3119,7 +3159,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="100.8" customHeight="1" s="26">
+    <row r="4" ht="100.8" customHeight="1" s="29">
       <c r="A4" t="inlineStr">
         <is>
           <t>Body_mail</t>
@@ -3147,7 +3187,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="100.8" customHeight="1" s="26">
+    <row r="6" ht="100.8" customHeight="1" s="29">
       <c r="A6" t="inlineStr">
         <is>
           <t>Valuation Class_Body</t>
@@ -3175,7 +3215,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="100.8" customHeight="1" s="26">
+    <row r="8" ht="100.8" customHeight="1" s="29">
       <c r="A8" t="inlineStr">
         <is>
           <t>Valuation Class Text_Body</t>
@@ -3203,7 +3243,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="100.8" customHeight="1" s="26">
+    <row r="10" ht="100.8" customHeight="1" s="29">
       <c r="A10" t="inlineStr">
         <is>
           <t>Gr Amt_Body</t>
@@ -3234,7 +3274,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="100.8" customHeight="1" s="26">
+    <row r="13" ht="100.8" customHeight="1" s="29">
       <c r="A13" t="inlineStr">
         <is>
           <t>body_file_not_found</t>
@@ -3265,7 +3305,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="100.8" customHeight="1" s="26">
+    <row r="19" ht="100.8" customHeight="1" s="29">
       <c r="A19" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -3293,7 +3333,7 @@
         </is>
       </c>
     </row>
-    <row r="22" ht="100.8" customHeight="1" s="26">
+    <row r="22" ht="100.8" customHeight="1" s="29">
       <c r="A22" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -3424,8 +3464,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="29.33203125" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
-    <col width="94.6640625" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
+    <col width="29.33203125" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
+    <col width="94.6640625" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3491,7 +3531,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="100.8" customHeight="1" s="26">
+    <row r="8" ht="100.8" customHeight="1" s="29">
       <c r="A8" t="inlineStr">
         <is>
           <t>Body_mail</t>
@@ -3519,7 +3559,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="100.8" customHeight="1" s="26">
+    <row r="10" ht="100.8" customHeight="1" s="29">
       <c r="A10" t="inlineStr">
         <is>
           <t>GR Document_Number_Body</t>
@@ -3553,7 +3593,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="100.8" customHeight="1" s="26">
+    <row r="14" ht="100.8" customHeight="1" s="29">
       <c r="A14" t="inlineStr">
         <is>
           <t>Gr Qty_Body</t>
@@ -3581,7 +3621,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="100.8" customHeight="1" s="26">
+    <row r="17" ht="100.8" customHeight="1" s="29">
       <c r="A17" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -3612,7 +3652,7 @@
         </is>
       </c>
     </row>
-    <row r="23" ht="100.8" customHeight="1" s="26">
+    <row r="23" ht="100.8" customHeight="1" s="29">
       <c r="A23" t="inlineStr">
         <is>
           <t>body_file_not_found</t>
@@ -3640,7 +3680,7 @@
         </is>
       </c>
     </row>
-    <row r="26" ht="100.8" customHeight="1" s="26">
+    <row r="26" ht="100.8" customHeight="1" s="29">
       <c r="A26" t="inlineStr">
         <is>
           <t>Purchase_ColumnMiss_Body</t>
@@ -3668,7 +3708,7 @@
         </is>
       </c>
     </row>
-    <row r="29" ht="100.8" customHeight="1" s="26">
+    <row r="29" ht="100.8" customHeight="1" s="29">
       <c r="A29" t="inlineStr">
         <is>
           <t>MB51_ColumnMiss_Body</t>
@@ -3696,7 +3736,7 @@
         </is>
       </c>
     </row>
-    <row r="32" ht="100.8" customHeight="1" s="26">
+    <row r="32" ht="100.8" customHeight="1" s="29">
       <c r="A32" t="inlineStr">
         <is>
           <t>Material_Document_Body</t>
@@ -3730,7 +3770,7 @@
         </is>
       </c>
     </row>
-    <row r="36" ht="100.8" customHeight="1" s="26">
+    <row r="36" ht="100.8" customHeight="1" s="29">
       <c r="A36" t="inlineStr">
         <is>
           <t>Qty_unit_of_entry_Body</t>
@@ -3766,11 +3806,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="35.5546875" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
-    <col width="122" customWidth="1" style="26" min="2" max="2"/>
+    <col width="35.5546875" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
+    <col width="122" customWidth="1" style="29" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.6" customHeight="1" s="26">
+    <row r="1" ht="18.6" customHeight="1" s="29">
       <c r="A1" s="14" t="inlineStr">
         <is>
           <t>Name</t>
@@ -3794,7 +3834,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="6" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A6" t="inlineStr">
         <is>
           <t>FileNotFound_Body</t>
@@ -3821,7 +3861,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="8" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A8" t="inlineStr">
         <is>
           <t>EmptyInput_Body</t>
@@ -3836,7 +3876,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="9" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A9" t="inlineStr">
         <is>
           <t>EmptyInput_Body1</t>
@@ -3863,7 +3903,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="11" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A11" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -3878,7 +3918,7 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="12" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A12" t="inlineStr">
         <is>
           <t>ColumnMiss_Body1</t>
@@ -3905,7 +3945,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="14" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A14" t="inlineStr">
         <is>
           <t>SheetMiss_Body</t>
@@ -3932,7 +3972,7 @@
         </is>
       </c>
     </row>
-    <row r="16" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="16" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A16" t="inlineStr">
         <is>
           <t>OutputNotFound_Body</t>
@@ -3959,7 +3999,7 @@
         </is>
       </c>
     </row>
-    <row r="18" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="18" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A18" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -4077,11 +4117,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="19.109375" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
-    <col width="143.88671875" customWidth="1" style="26" min="2" max="2"/>
+    <col width="19.109375" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
+    <col width="143.88671875" customWidth="1" style="29" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" customHeight="1" s="26">
+    <row r="1" ht="15.6" customHeight="1" s="29">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Key</t>
@@ -4093,11 +4133,11 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="15.6" customHeight="1" s="26">
+    <row r="2" ht="15.6" customHeight="1" s="29">
       <c r="A2" s="25" t="n"/>
       <c r="B2" s="25" t="n"/>
     </row>
-    <row r="3" ht="15.6" customHeight="1" s="26">
+    <row r="3" ht="15.6" customHeight="1" s="29">
       <c r="A3" s="6" t="inlineStr">
         <is>
           <t>Subject_mail</t>
@@ -4109,7 +4149,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="93.59999999999999" customHeight="1" s="26">
+    <row r="4" ht="93.59999999999999" customHeight="1" s="29">
       <c r="A4" s="25" t="inlineStr">
         <is>
           <t>Body_mail</t>
@@ -4124,7 +4164,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="15.6" customHeight="1" s="26">
+    <row r="5" ht="15.6" customHeight="1" s="29">
       <c r="A5" s="25" t="inlineStr">
         <is>
           <t>Unit_price</t>
@@ -4136,7 +4176,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="93.59999999999999" customHeight="1" s="26">
+    <row r="6" ht="93.59999999999999" customHeight="1" s="29">
       <c r="A6" s="25" t="inlineStr">
         <is>
           <t>Unit_price_body</t>
@@ -4151,7 +4191,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="15.6" customHeight="1" s="26">
+    <row r="7" ht="15.6" customHeight="1" s="29">
       <c r="A7" s="6" t="inlineStr">
         <is>
           <t>Document is empty</t>
@@ -4163,7 +4203,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="93.59999999999999" customHeight="1" s="26">
+    <row r="8" ht="93.59999999999999" customHeight="1" s="29">
       <c r="A8" s="22" t="inlineStr">
         <is>
           <t>Doc_bod</t>
@@ -4178,7 +4218,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="15.6" customHeight="1" s="26">
+    <row r="9" ht="15.6" customHeight="1" s="29">
       <c r="A9" s="25" t="inlineStr">
         <is>
           <t>Key</t>
@@ -4190,7 +4230,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="93.59999999999999" customHeight="1" s="26">
+    <row r="10" ht="93.59999999999999" customHeight="1" s="29">
       <c r="A10" s="25" t="inlineStr">
         <is>
           <t>Key_body</t>
@@ -4205,7 +4245,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="15.6" customHeight="1" s="26">
+    <row r="11" ht="15.6" customHeight="1" s="29">
       <c r="A11" s="25" t="inlineStr">
         <is>
           <t>Syn</t>
@@ -4217,7 +4257,7 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="93.59999999999999" customHeight="1" s="26">
+    <row r="12" ht="93.59999999999999" customHeight="1" s="29">
       <c r="A12" s="25" t="inlineStr">
         <is>
           <t>Synody_</t>
@@ -4232,7 +4272,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="15.6" customHeight="1" s="26">
+    <row r="13" ht="15.6" customHeight="1" s="29">
       <c r="A13" s="25" t="inlineStr">
         <is>
           <t>File_N</t>
@@ -4244,7 +4284,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="93.59999999999999" customHeight="1" s="26">
+    <row r="14" ht="93.59999999999999" customHeight="1" s="29">
       <c r="A14" s="25" t="inlineStr">
         <is>
           <t>File_N_body</t>
@@ -4259,7 +4299,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="15.6" customHeight="1" s="26">
+    <row r="15" ht="15.6" customHeight="1" s="29">
       <c r="A15" s="25" t="inlineStr">
         <is>
           <t>Name_E</t>
@@ -4271,7 +4311,7 @@
         </is>
       </c>
     </row>
-    <row r="16" ht="93.59999999999999" customHeight="1" s="26">
+    <row r="16" ht="93.59999999999999" customHeight="1" s="29">
       <c r="A16" s="25" t="inlineStr">
         <is>
           <t>Name_E_body</t>
@@ -4286,7 +4326,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="15.6" customHeight="1" s="26">
+    <row r="17" ht="15.6" customHeight="1" s="29">
       <c r="A17" s="25" t="inlineStr">
         <is>
           <t>Value_E</t>
@@ -4298,7 +4338,7 @@
         </is>
       </c>
     </row>
-    <row r="18" ht="93.59999999999999" customHeight="1" s="26">
+    <row r="18" ht="93.59999999999999" customHeight="1" s="29">
       <c r="A18" s="25" t="inlineStr">
         <is>
           <t>Value_E_body</t>
@@ -4440,8 +4480,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="17.109375" customWidth="1" style="26" min="1" max="1"/>
-    <col width="96.109375" customWidth="1" style="26" min="2" max="2"/>
+    <col width="17.109375" customWidth="1" style="29" min="1" max="1"/>
+    <col width="96.109375" customWidth="1" style="29" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4460,7 +4500,7 @@
       <c r="A2" s="3" t="n"/>
       <c r="B2" s="10" t="n"/>
     </row>
-    <row r="3" ht="100.8" customHeight="1" s="26">
+    <row r="3" ht="100.8" customHeight="1" s="29">
       <c r="A3" s="3" t="inlineStr">
         <is>
           <t>FileNotFoundError</t>
@@ -4475,7 +4515,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="100.8" customHeight="1" s="26">
+    <row r="4" ht="100.8" customHeight="1" s="29">
       <c r="A4" s="3" t="inlineStr">
         <is>
           <t>FileExistsError</t>
@@ -4491,7 +4531,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="115.2" customHeight="1" s="26">
+    <row r="5" ht="115.2" customHeight="1" s="29">
       <c r="A5" s="3" t="inlineStr">
         <is>
           <t>RuntimeError</t>
@@ -4508,7 +4548,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="115.2" customHeight="1" s="26">
+    <row r="6" ht="115.2" customHeight="1" s="29">
       <c r="A6" s="3" t="inlineStr">
         <is>
           <t>ValueError</t>
@@ -4525,7 +4565,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="115.2" customHeight="1" s="26">
+    <row r="7" ht="115.2" customHeight="1" s="29">
       <c r="A7" s="3" t="inlineStr">
         <is>
           <t>TypeError</t>
@@ -4542,7 +4582,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="100.8" customHeight="1" s="26">
+    <row r="8" ht="100.8" customHeight="1" s="29">
       <c r="A8" s="3" t="inlineStr">
         <is>
           <t>KeyError</t>
@@ -4713,8 +4753,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="26.5546875" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
-    <col width="90.44140625" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
+    <col width="26.5546875" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
+    <col width="90.44140625" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4741,7 +4781,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="3" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A3" t="inlineStr">
         <is>
           <t>ConfigFail_Body</t>
@@ -4768,7 +4808,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="5" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A5" t="inlineStr">
         <is>
           <t>FileNotFound_Body</t>
@@ -4795,7 +4835,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="7" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A7" t="inlineStr">
         <is>
           <t>EmptyInput_Body</t>
@@ -4822,7 +4862,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="9" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A9" t="inlineStr">
         <is>
           <t>EmptyVendorName_Body</t>
@@ -4849,7 +4889,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="11" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A11" t="inlineStr">
         <is>
           <t>EmptyVendorNo_Body</t>
@@ -4876,7 +4916,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="13" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A13" t="inlineStr">
         <is>
           <t>EmptyTax_Body</t>
@@ -4903,7 +4943,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="15" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A15" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -4930,7 +4970,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="17" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A17" t="inlineStr">
         <is>
           <t>SheetMiss_Body</t>
@@ -4957,7 +4997,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="19" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A19" t="inlineStr">
         <is>
           <t>OutputNotFound_Body</t>
@@ -4984,7 +5024,7 @@
         </is>
       </c>
     </row>
-    <row r="21" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="21" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A21" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -5018,11 +5058,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="32.44140625" customWidth="1" style="26" min="1" max="1"/>
-    <col width="106.33203125" customWidth="1" style="26" min="2" max="2"/>
+    <col width="32.44140625" customWidth="1" style="29" min="1" max="1"/>
+    <col width="106.33203125" customWidth="1" style="29" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" customHeight="1" s="26">
+    <row r="1" ht="15.6" customHeight="1" s="29">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Key</t>
@@ -5034,11 +5074,11 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="15.6" customHeight="1" s="26">
+    <row r="2" ht="15.6" customHeight="1" s="29">
       <c r="A2" s="25" t="n"/>
       <c r="B2" s="25" t="n"/>
     </row>
-    <row r="3" ht="15.6" customHeight="1" s="26">
+    <row r="3" ht="15.6" customHeight="1" s="29">
       <c r="A3" s="6" t="inlineStr">
         <is>
           <t>Sourcefile_subject</t>
@@ -5050,7 +5090,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="15.6" customHeight="1" s="26">
+    <row r="4" ht="15.6" customHeight="1" s="29">
       <c r="A4" s="25" t="inlineStr">
         <is>
           <t>Body_mail1</t>
@@ -5065,7 +5105,7 @@
     <row r="5">
       <c r="B5" s="19" t="n"/>
     </row>
-    <row r="6" ht="15.6" customHeight="1" s="26">
+    <row r="6" ht="15.6" customHeight="1" s="29">
       <c r="B6" s="8" t="inlineStr">
         <is>
           <t>The given source file is empty. Hence Vendor Wise Concentration process stopped executing.</t>
@@ -5075,21 +5115,21 @@
     <row r="7">
       <c r="B7" s="19" t="n"/>
     </row>
-    <row r="8" ht="15.6" customHeight="1" s="26">
+    <row r="8" ht="15.6" customHeight="1" s="29">
       <c r="B8" s="8" t="inlineStr">
         <is>
           <t>Thanks &amp; Regards,</t>
         </is>
       </c>
     </row>
-    <row r="9" ht="15.6" customHeight="1" s="26">
+    <row r="9" ht="15.6" customHeight="1" s="29">
       <c r="B9" s="8" t="inlineStr">
         <is>
           <t>Ln &amp; Co</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="15.6" customHeight="1" s="26">
+    <row r="10" ht="15.6" customHeight="1" s="29">
       <c r="A10" s="25" t="inlineStr">
         <is>
           <t>Gr_amount</t>
@@ -5101,7 +5141,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="15.6" customHeight="1" s="26">
+    <row r="11" ht="15.6" customHeight="1" s="29">
       <c r="A11" s="25" t="inlineStr">
         <is>
           <t>Gr_amount_body</t>
@@ -5116,7 +5156,7 @@
     <row r="12">
       <c r="B12" s="19" t="n"/>
     </row>
-    <row r="13" ht="15.6" customHeight="1" s="26">
+    <row r="13" ht="15.6" customHeight="1" s="29">
       <c r="B13" s="8" t="inlineStr">
         <is>
           <t>GR Amt. in loc.cur. column in source file is empty. Hence the Vendor Wise Concentration  ended executing.</t>
@@ -5126,21 +5166,21 @@
     <row r="14">
       <c r="B14" s="19" t="n"/>
     </row>
-    <row r="15" ht="15.6" customHeight="1" s="26">
+    <row r="15" ht="15.6" customHeight="1" s="29">
       <c r="B15" s="8" t="inlineStr">
         <is>
           <t>Thanks &amp; Regards,</t>
         </is>
       </c>
     </row>
-    <row r="16" ht="15.6" customHeight="1" s="26">
+    <row r="16" ht="15.6" customHeight="1" s="29">
       <c r="B16" s="8" t="inlineStr">
         <is>
           <t>Ln &amp; Co</t>
         </is>
       </c>
     </row>
-    <row r="17" ht="15.6" customHeight="1" s="26">
+    <row r="17" ht="15.6" customHeight="1" s="29">
       <c r="A17" s="6" t="inlineStr">
         <is>
           <t>Vendor_No</t>
@@ -5152,7 +5192,7 @@
         </is>
       </c>
     </row>
-    <row r="18" ht="15.6" customHeight="1" s="26">
+    <row r="18" ht="15.6" customHeight="1" s="29">
       <c r="A18" s="27" t="inlineStr">
         <is>
           <t>Vendor_No_body</t>
@@ -5167,7 +5207,7 @@
     <row r="19">
       <c r="B19" s="19" t="n"/>
     </row>
-    <row r="20" ht="15.6" customHeight="1" s="26">
+    <row r="20" ht="15.6" customHeight="1" s="29">
       <c r="B20" s="8" t="inlineStr">
         <is>
           <t>Vendor class column empty. Hence the Vendor Wise Concentration executing.</t>
@@ -5177,14 +5217,14 @@
     <row r="21">
       <c r="B21" s="19" t="n"/>
     </row>
-    <row r="22" ht="15.6" customHeight="1" s="26">
+    <row r="22" ht="15.6" customHeight="1" s="29">
       <c r="B22" s="8" t="inlineStr">
         <is>
           <t>Thanks &amp; Regards,</t>
         </is>
       </c>
     </row>
-    <row r="23" ht="15.6" customHeight="1" s="26">
+    <row r="23" ht="15.6" customHeight="1" s="29">
       <c r="A23" s="28" t="n"/>
       <c r="B23" s="8" t="inlineStr">
         <is>
@@ -5313,8 +5353,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="24.109375" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
-    <col width="90.44140625" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
+    <col width="24.109375" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
+    <col width="90.44140625" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5341,7 +5381,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="3" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A3" t="inlineStr">
         <is>
           <t>FileNotFound_Body</t>
@@ -5368,7 +5408,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="5" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A5" t="inlineStr">
         <is>
           <t>EmptyInput_Body</t>
@@ -5395,7 +5435,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="7" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A7" t="inlineStr">
         <is>
           <t>Key_Body</t>
@@ -5422,7 +5462,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="9" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A9" t="inlineStr">
         <is>
           <t>GRAmt_Subject</t>
@@ -5449,7 +5489,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="11" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A11" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -5476,7 +5516,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="13" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A13" t="inlineStr">
         <is>
           <t>SheetMiss_Body</t>
@@ -5503,7 +5543,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="15" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A15" t="inlineStr">
         <is>
           <t>OutputNotFound_Body</t>
@@ -5530,7 +5570,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="17" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A17" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -5660,11 +5700,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="28.109375" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
-    <col width="86.88671875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
+    <col width="28.109375" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
+    <col width="86.88671875" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.8" customHeight="1" s="26">
+    <row r="1" ht="13.8" customHeight="1" s="29">
       <c r="A1" s="14" t="inlineStr">
         <is>
           <t>Name</t>
@@ -5688,7 +5728,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="3" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A3" t="inlineStr">
         <is>
           <t>FileNotFound_Body</t>
@@ -5715,7 +5755,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="5" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A5" t="inlineStr">
         <is>
           <t>EmptyInput_Body</t>
@@ -5742,7 +5782,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="7" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A7" t="inlineStr">
         <is>
           <t>Plant_Body</t>
@@ -5769,7 +5809,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="9" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A9" t="inlineStr">
         <is>
           <t>GRAmt_Subject</t>
@@ -5796,7 +5836,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="100.8" customHeight="1" s="26">
+    <row r="11" ht="100.8" customHeight="1" s="29">
       <c r="A11" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -5823,7 +5863,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="13" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A13" t="inlineStr">
         <is>
           <t>SheetMiss_Body</t>
@@ -5850,7 +5890,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="15" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A15" t="inlineStr">
         <is>
           <t>OutputNotFound_Body</t>
@@ -5877,7 +5917,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="17" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A17" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -6007,8 +6047,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="28.6640625" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
-    <col width="86.88671875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
+    <col width="28.6640625" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
+    <col width="86.88671875" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6035,7 +6075,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="3" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A3" t="inlineStr">
         <is>
           <t>FileNotFound_Body</t>
@@ -6062,7 +6102,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="5" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A5" t="inlineStr">
         <is>
           <t>EmptyInput_Body</t>
@@ -6089,7 +6129,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="7" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A7" t="inlineStr">
         <is>
           <t>Date_Body</t>
@@ -6116,7 +6156,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="9" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A9" t="inlineStr">
         <is>
           <t>GRAmt_Subject</t>
@@ -6143,7 +6183,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="100.8" customHeight="1" s="26">
+    <row r="11" ht="100.8" customHeight="1" s="29">
       <c r="A11" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -6170,7 +6210,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="13" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A13" t="inlineStr">
         <is>
           <t>SheetMiss_Body</t>
@@ -6197,7 +6237,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="15" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A15" t="inlineStr">
         <is>
           <t>OutputNotFound_Body</t>
@@ -6224,7 +6264,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="86.40000000000001" customHeight="1" s="26">
+    <row r="17" ht="86.40000000000001" customHeight="1" s="29">
       <c r="A17" t="inlineStr">
         <is>
           <t>SystemError_Body</t>

</xml_diff>

<commit_message>
LnCo as on Dec 26
</commit_message>
<xml_diff>
--- a/Lnco/Input/Config.xlsx
+++ b/Lnco/Input/Config.xlsx
@@ -132,7 +132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
@@ -188,7 +188,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,15 +534,15 @@
   </sheetPr>
   <dimension ref="A1:B95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="114" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="114" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="48.5546875" customWidth="1" style="29" min="1" max="1"/>
-    <col width="84.21875" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
-    <col width="30.77734375" bestFit="1" customWidth="1" style="29" min="4" max="4"/>
+    <col width="48.5546875" customWidth="1" style="26" min="1" max="1"/>
+    <col width="84.21875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
+    <col width="30.77734375" bestFit="1" customWidth="1" style="26" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1038,7 +1037,16 @@
       <c r="B56" s="23" t="n"/>
     </row>
     <row r="57">
-      <c r="B57" s="23" t="n"/>
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>security_cutoff_date_list</t>
+        </is>
+      </c>
+      <c r="B57" s="23" t="inlineStr">
+        <is>
+          <t>[26, 27, 28, 29, 30, 31]</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="B58" s="23" t="n"/>
@@ -1267,7 +1275,7 @@
         </is>
       </c>
     </row>
-    <row r="83" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="83" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A83" t="inlineStr">
         <is>
           <t>Start_Mail_Body</t>
@@ -1295,7 +1303,7 @@
         </is>
       </c>
     </row>
-    <row r="86" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="86" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A86" t="inlineStr">
         <is>
           <t>Success_Mail_Body</t>
@@ -1323,7 +1331,7 @@
         </is>
       </c>
     </row>
-    <row r="89" ht="100.8" customHeight="1" s="29">
+    <row r="89" ht="100.8" customHeight="1" s="26">
       <c r="A89" t="inlineStr">
         <is>
           <t>body_file_not_found</t>
@@ -1354,7 +1362,7 @@
         </is>
       </c>
     </row>
-    <row r="92" ht="100.8" customHeight="1" s="29">
+    <row r="92" ht="100.8" customHeight="1" s="26">
       <c r="A92" t="inlineStr">
         <is>
           <t>body_sheet_not_found</t>
@@ -1383,7 +1391,7 @@
         </is>
       </c>
     </row>
-    <row r="95" ht="100.8" customHeight="1" s="29">
+    <row r="95" ht="100.8" customHeight="1" s="26">
       <c r="A95" t="inlineStr">
         <is>
           <t>body_in_progress_request_found</t>
@@ -1428,10 +1436,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="24.5546875" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
-    <col width="92.33203125" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
-    <col width="43.6640625" customWidth="1" style="29" min="5" max="5"/>
-    <col width="36.109375" customWidth="1" style="29" min="6" max="6"/>
+    <col width="24.5546875" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="92.33203125" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
+    <col width="43.6640625" customWidth="1" style="26" min="5" max="5"/>
+    <col width="36.109375" customWidth="1" style="26" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1458,7 +1466,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="3" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A3" s="3" t="inlineStr">
         <is>
           <t>FileNotFound_Body</t>
@@ -1485,7 +1493,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="5" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A5" s="3" t="inlineStr">
         <is>
           <t>EmptyInput_Body</t>
@@ -1512,7 +1520,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="7" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A7" s="3" t="inlineStr">
         <is>
           <t>EmptyValClass_Body</t>
@@ -1539,7 +1547,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="9" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A9" s="3" t="inlineStr">
         <is>
           <t>EmptyValClassTxt_Body</t>
@@ -1566,7 +1574,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="11" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A11" s="3" t="inlineStr">
         <is>
           <t>GRAmt_Subject</t>
@@ -1593,7 +1601,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="13" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A13" s="3" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -1620,7 +1628,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="15" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A15" s="3" t="inlineStr">
         <is>
           <t>SheetMiss_Body</t>
@@ -1647,7 +1655,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="17" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A17" s="3" t="inlineStr">
         <is>
           <t>OutputNotFound_Body</t>
@@ -1674,7 +1682,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="19" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A19" s="3" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -1804,8 +1812,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="49.33203125" customWidth="1" style="29" min="1" max="1"/>
-    <col width="83.88671875" customWidth="1" style="29" min="2" max="2"/>
+    <col width="49.33203125" customWidth="1" style="26" min="1" max="1"/>
+    <col width="83.88671875" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1832,7 +1840,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="100.8" customHeight="1" s="29">
+    <row r="3" ht="100.8" customHeight="1" s="26">
       <c r="A3" t="inlineStr">
         <is>
           <t>Vendor No._Body</t>
@@ -1860,7 +1868,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="100.8" customHeight="1" s="29">
+    <row r="5" ht="100.8" customHeight="1" s="26">
       <c r="A5" t="inlineStr">
         <is>
           <t>Vendor Name_Body</t>
@@ -1888,7 +1896,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="100.8" customHeight="1" s="29">
+    <row r="7" ht="100.8" customHeight="1" s="26">
       <c r="A7" t="inlineStr">
         <is>
           <t>Gr Amt_Body</t>
@@ -1916,7 +1924,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="9" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A9" t="inlineStr">
         <is>
           <t>FileNotFound_Body</t>
@@ -1943,7 +1951,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="11" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A11" t="inlineStr">
         <is>
           <t>EmptyInput_Body</t>
@@ -1958,7 +1966,7 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="12" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A12" t="inlineStr">
         <is>
           <t>EmptyInput_Body1</t>
@@ -1985,7 +1993,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="14" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A14" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -2000,7 +2008,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="15" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A15" t="inlineStr">
         <is>
           <t>ColumnMiss_Body1</t>
@@ -2027,7 +2035,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="17" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A17" t="inlineStr">
         <is>
           <t>SheetMiss_Body</t>
@@ -2054,7 +2062,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="19" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A19" t="inlineStr">
         <is>
           <t>OutputNotFound_Body</t>
@@ -2081,7 +2089,7 @@
         </is>
       </c>
     </row>
-    <row r="21" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="21" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A21" t="inlineStr">
         <is>
           <t>SystemE_Body</t>
@@ -2108,7 +2116,7 @@
         </is>
       </c>
     </row>
-    <row r="23" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="23" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A23" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -2238,8 +2246,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="35.5546875" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
-    <col width="86.88671875" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
+    <col width="35.5546875" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="86.88671875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2266,7 +2274,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="100.8" customHeight="1" s="29">
+    <row r="4" ht="100.8" customHeight="1" s="26">
       <c r="A4" t="inlineStr">
         <is>
           <t>Body_mail</t>
@@ -2294,7 +2302,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="100.8" customHeight="1" s="29">
+    <row r="7" ht="100.8" customHeight="1" s="26">
       <c r="A7" t="inlineStr">
         <is>
           <t>body_file_not_found</t>
@@ -2325,7 +2333,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="100.8" customHeight="1" s="29">
+    <row r="10" ht="100.8" customHeight="1" s="26">
       <c r="A10" t="inlineStr">
         <is>
           <t>Gr Amt_Body</t>
@@ -2353,7 +2361,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="100.8" customHeight="1" s="29">
+    <row r="13" ht="100.8" customHeight="1" s="26">
       <c r="A13" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -2381,7 +2389,7 @@
         </is>
       </c>
     </row>
-    <row r="16" ht="100.8" customHeight="1" s="29">
+    <row r="16" ht="100.8" customHeight="1" s="26">
       <c r="A16" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -2512,8 +2520,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="24.5546875" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
-    <col width="86.88671875" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
+    <col width="24.5546875" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="86.88671875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2540,7 +2548,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="100.8" customHeight="1" s="29">
+    <row r="4" ht="100.8" customHeight="1" s="26">
       <c r="A4" t="inlineStr">
         <is>
           <t>Body_mail</t>
@@ -2568,7 +2576,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="100.8" customHeight="1" s="29">
+    <row r="6" ht="100.8" customHeight="1" s="26">
       <c r="A6" t="inlineStr">
         <is>
           <t>Plant_Body</t>
@@ -2602,7 +2610,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="100.8" customHeight="1" s="29">
+    <row r="10" ht="100.8" customHeight="1" s="26">
       <c r="A10" t="inlineStr">
         <is>
           <t>Gr Amt_Body</t>
@@ -2630,7 +2638,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="100.8" customHeight="1" s="29">
+    <row r="13" ht="100.8" customHeight="1" s="26">
       <c r="A13" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -2661,7 +2669,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="100.8" customHeight="1" s="29">
+    <row r="19" ht="100.8" customHeight="1" s="26">
       <c r="A19" t="inlineStr">
         <is>
           <t>body_file_not_found</t>
@@ -2689,7 +2697,7 @@
         </is>
       </c>
     </row>
-    <row r="22" ht="100.8" customHeight="1" s="29">
+    <row r="22" ht="100.8" customHeight="1" s="26">
       <c r="A22" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -2820,8 +2828,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="17.88671875" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
-    <col width="86.88671875" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
+    <col width="17.88671875" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="86.88671875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2848,7 +2856,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="100.8" customHeight="1" s="29">
+    <row r="4" ht="100.8" customHeight="1" s="26">
       <c r="A4" t="inlineStr">
         <is>
           <t>Body_mail</t>
@@ -2876,7 +2884,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="100.8" customHeight="1" s="29">
+    <row r="6" ht="100.8" customHeight="1" s="26">
       <c r="A6" t="inlineStr">
         <is>
           <t>Month_Body</t>
@@ -2910,7 +2918,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="100.8" customHeight="1" s="29">
+    <row r="10" ht="100.8" customHeight="1" s="26">
       <c r="A10" t="inlineStr">
         <is>
           <t>Gr Amt_Body</t>
@@ -2941,7 +2949,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="100.8" customHeight="1" s="29">
+    <row r="13" ht="100.8" customHeight="1" s="26">
       <c r="A13" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -2972,7 +2980,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="100.8" customHeight="1" s="29">
+    <row r="19" ht="100.8" customHeight="1" s="26">
       <c r="A19" t="inlineStr">
         <is>
           <t>body_file_not_found</t>
@@ -3000,7 +3008,7 @@
         </is>
       </c>
     </row>
-    <row r="22" ht="100.8" customHeight="1" s="29">
+    <row r="22" ht="100.8" customHeight="1" s="26">
       <c r="A22" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -3131,8 +3139,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="26.88671875" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
-    <col width="91.88671875" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
+    <col width="26.88671875" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="91.88671875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3159,7 +3167,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="100.8" customHeight="1" s="29">
+    <row r="4" ht="100.8" customHeight="1" s="26">
       <c r="A4" t="inlineStr">
         <is>
           <t>Body_mail</t>
@@ -3187,7 +3195,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="100.8" customHeight="1" s="29">
+    <row r="6" ht="100.8" customHeight="1" s="26">
       <c r="A6" t="inlineStr">
         <is>
           <t>Valuation Class_Body</t>
@@ -3215,7 +3223,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="100.8" customHeight="1" s="29">
+    <row r="8" ht="100.8" customHeight="1" s="26">
       <c r="A8" t="inlineStr">
         <is>
           <t>Valuation Class Text_Body</t>
@@ -3243,7 +3251,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="100.8" customHeight="1" s="29">
+    <row r="10" ht="100.8" customHeight="1" s="26">
       <c r="A10" t="inlineStr">
         <is>
           <t>Gr Amt_Body</t>
@@ -3274,7 +3282,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="100.8" customHeight="1" s="29">
+    <row r="13" ht="100.8" customHeight="1" s="26">
       <c r="A13" t="inlineStr">
         <is>
           <t>body_file_not_found</t>
@@ -3305,7 +3313,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="100.8" customHeight="1" s="29">
+    <row r="19" ht="100.8" customHeight="1" s="26">
       <c r="A19" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -3333,7 +3341,7 @@
         </is>
       </c>
     </row>
-    <row r="22" ht="100.8" customHeight="1" s="29">
+    <row r="22" ht="100.8" customHeight="1" s="26">
       <c r="A22" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -3464,8 +3472,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="29.33203125" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
-    <col width="94.6640625" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
+    <col width="29.33203125" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="94.6640625" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3531,7 +3539,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="100.8" customHeight="1" s="29">
+    <row r="8" ht="100.8" customHeight="1" s="26">
       <c r="A8" t="inlineStr">
         <is>
           <t>Body_mail</t>
@@ -3559,7 +3567,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="100.8" customHeight="1" s="29">
+    <row r="10" ht="100.8" customHeight="1" s="26">
       <c r="A10" t="inlineStr">
         <is>
           <t>GR Document_Number_Body</t>
@@ -3593,7 +3601,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="100.8" customHeight="1" s="29">
+    <row r="14" ht="100.8" customHeight="1" s="26">
       <c r="A14" t="inlineStr">
         <is>
           <t>Gr Qty_Body</t>
@@ -3621,7 +3629,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="100.8" customHeight="1" s="29">
+    <row r="17" ht="100.8" customHeight="1" s="26">
       <c r="A17" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -3652,7 +3660,7 @@
         </is>
       </c>
     </row>
-    <row r="23" ht="100.8" customHeight="1" s="29">
+    <row r="23" ht="100.8" customHeight="1" s="26">
       <c r="A23" t="inlineStr">
         <is>
           <t>body_file_not_found</t>
@@ -3680,7 +3688,7 @@
         </is>
       </c>
     </row>
-    <row r="26" ht="100.8" customHeight="1" s="29">
+    <row r="26" ht="100.8" customHeight="1" s="26">
       <c r="A26" t="inlineStr">
         <is>
           <t>Purchase_ColumnMiss_Body</t>
@@ -3708,7 +3716,7 @@
         </is>
       </c>
     </row>
-    <row r="29" ht="100.8" customHeight="1" s="29">
+    <row r="29" ht="100.8" customHeight="1" s="26">
       <c r="A29" t="inlineStr">
         <is>
           <t>MB51_ColumnMiss_Body</t>
@@ -3736,7 +3744,7 @@
         </is>
       </c>
     </row>
-    <row r="32" ht="100.8" customHeight="1" s="29">
+    <row r="32" ht="100.8" customHeight="1" s="26">
       <c r="A32" t="inlineStr">
         <is>
           <t>Material_Document_Body</t>
@@ -3770,7 +3778,7 @@
         </is>
       </c>
     </row>
-    <row r="36" ht="100.8" customHeight="1" s="29">
+    <row r="36" ht="100.8" customHeight="1" s="26">
       <c r="A36" t="inlineStr">
         <is>
           <t>Qty_unit_of_entry_Body</t>
@@ -3806,11 +3814,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="35.5546875" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
-    <col width="122" customWidth="1" style="29" min="2" max="2"/>
+    <col width="35.5546875" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="122" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.6" customHeight="1" s="29">
+    <row r="1" ht="18.6" customHeight="1" s="26">
       <c r="A1" s="14" t="inlineStr">
         <is>
           <t>Name</t>
@@ -3834,7 +3842,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="6" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A6" t="inlineStr">
         <is>
           <t>FileNotFound_Body</t>
@@ -3861,7 +3869,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="8" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A8" t="inlineStr">
         <is>
           <t>EmptyInput_Body</t>
@@ -3876,7 +3884,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="9" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A9" t="inlineStr">
         <is>
           <t>EmptyInput_Body1</t>
@@ -3903,7 +3911,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="11" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A11" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -3918,7 +3926,7 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="12" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A12" t="inlineStr">
         <is>
           <t>ColumnMiss_Body1</t>
@@ -3945,7 +3953,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="14" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A14" t="inlineStr">
         <is>
           <t>SheetMiss_Body</t>
@@ -3972,7 +3980,7 @@
         </is>
       </c>
     </row>
-    <row r="16" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="16" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A16" t="inlineStr">
         <is>
           <t>OutputNotFound_Body</t>
@@ -3999,7 +4007,7 @@
         </is>
       </c>
     </row>
-    <row r="18" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="18" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A18" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -4117,11 +4125,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="19.109375" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
-    <col width="143.88671875" customWidth="1" style="29" min="2" max="2"/>
+    <col width="19.109375" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="143.88671875" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" customHeight="1" s="29">
+    <row r="1" ht="15.6" customHeight="1" s="26">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Key</t>
@@ -4133,11 +4141,11 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="15.6" customHeight="1" s="29">
+    <row r="2" ht="15.6" customHeight="1" s="26">
       <c r="A2" s="25" t="n"/>
       <c r="B2" s="25" t="n"/>
     </row>
-    <row r="3" ht="15.6" customHeight="1" s="29">
+    <row r="3" ht="15.6" customHeight="1" s="26">
       <c r="A3" s="6" t="inlineStr">
         <is>
           <t>Subject_mail</t>
@@ -4149,7 +4157,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="93.59999999999999" customHeight="1" s="29">
+    <row r="4" ht="93.59999999999999" customHeight="1" s="26">
       <c r="A4" s="25" t="inlineStr">
         <is>
           <t>Body_mail</t>
@@ -4164,7 +4172,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="15.6" customHeight="1" s="29">
+    <row r="5" ht="15.6" customHeight="1" s="26">
       <c r="A5" s="25" t="inlineStr">
         <is>
           <t>Unit_price</t>
@@ -4176,7 +4184,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="93.59999999999999" customHeight="1" s="29">
+    <row r="6" ht="93.59999999999999" customHeight="1" s="26">
       <c r="A6" s="25" t="inlineStr">
         <is>
           <t>Unit_price_body</t>
@@ -4191,7 +4199,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="15.6" customHeight="1" s="29">
+    <row r="7" ht="15.6" customHeight="1" s="26">
       <c r="A7" s="6" t="inlineStr">
         <is>
           <t>Document is empty</t>
@@ -4203,7 +4211,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="93.59999999999999" customHeight="1" s="29">
+    <row r="8" ht="93.59999999999999" customHeight="1" s="26">
       <c r="A8" s="22" t="inlineStr">
         <is>
           <t>Doc_bod</t>
@@ -4218,7 +4226,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="15.6" customHeight="1" s="29">
+    <row r="9" ht="15.6" customHeight="1" s="26">
       <c r="A9" s="25" t="inlineStr">
         <is>
           <t>Key</t>
@@ -4230,7 +4238,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="93.59999999999999" customHeight="1" s="29">
+    <row r="10" ht="93.59999999999999" customHeight="1" s="26">
       <c r="A10" s="25" t="inlineStr">
         <is>
           <t>Key_body</t>
@@ -4245,7 +4253,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="15.6" customHeight="1" s="29">
+    <row r="11" ht="15.6" customHeight="1" s="26">
       <c r="A11" s="25" t="inlineStr">
         <is>
           <t>Syn</t>
@@ -4257,7 +4265,7 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="93.59999999999999" customHeight="1" s="29">
+    <row r="12" ht="93.59999999999999" customHeight="1" s="26">
       <c r="A12" s="25" t="inlineStr">
         <is>
           <t>Synody_</t>
@@ -4272,7 +4280,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="15.6" customHeight="1" s="29">
+    <row r="13" ht="15.6" customHeight="1" s="26">
       <c r="A13" s="25" t="inlineStr">
         <is>
           <t>File_N</t>
@@ -4284,7 +4292,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="93.59999999999999" customHeight="1" s="29">
+    <row r="14" ht="93.59999999999999" customHeight="1" s="26">
       <c r="A14" s="25" t="inlineStr">
         <is>
           <t>File_N_body</t>
@@ -4299,7 +4307,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="15.6" customHeight="1" s="29">
+    <row r="15" ht="15.6" customHeight="1" s="26">
       <c r="A15" s="25" t="inlineStr">
         <is>
           <t>Name_E</t>
@@ -4311,7 +4319,7 @@
         </is>
       </c>
     </row>
-    <row r="16" ht="93.59999999999999" customHeight="1" s="29">
+    <row r="16" ht="93.59999999999999" customHeight="1" s="26">
       <c r="A16" s="25" t="inlineStr">
         <is>
           <t>Name_E_body</t>
@@ -4326,7 +4334,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="15.6" customHeight="1" s="29">
+    <row r="17" ht="15.6" customHeight="1" s="26">
       <c r="A17" s="25" t="inlineStr">
         <is>
           <t>Value_E</t>
@@ -4338,7 +4346,7 @@
         </is>
       </c>
     </row>
-    <row r="18" ht="93.59999999999999" customHeight="1" s="29">
+    <row r="18" ht="93.59999999999999" customHeight="1" s="26">
       <c r="A18" s="25" t="inlineStr">
         <is>
           <t>Value_E_body</t>
@@ -4480,8 +4488,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="17.109375" customWidth="1" style="29" min="1" max="1"/>
-    <col width="96.109375" customWidth="1" style="29" min="2" max="2"/>
+    <col width="17.109375" customWidth="1" style="26" min="1" max="1"/>
+    <col width="96.109375" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4500,7 +4508,7 @@
       <c r="A2" s="3" t="n"/>
       <c r="B2" s="10" t="n"/>
     </row>
-    <row r="3" ht="100.8" customHeight="1" s="29">
+    <row r="3" ht="100.8" customHeight="1" s="26">
       <c r="A3" s="3" t="inlineStr">
         <is>
           <t>FileNotFoundError</t>
@@ -4515,7 +4523,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="100.8" customHeight="1" s="29">
+    <row r="4" ht="100.8" customHeight="1" s="26">
       <c r="A4" s="3" t="inlineStr">
         <is>
           <t>FileExistsError</t>
@@ -4531,7 +4539,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="115.2" customHeight="1" s="29">
+    <row r="5" ht="115.2" customHeight="1" s="26">
       <c r="A5" s="3" t="inlineStr">
         <is>
           <t>RuntimeError</t>
@@ -4548,7 +4556,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="115.2" customHeight="1" s="29">
+    <row r="6" ht="115.2" customHeight="1" s="26">
       <c r="A6" s="3" t="inlineStr">
         <is>
           <t>ValueError</t>
@@ -4565,7 +4573,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="115.2" customHeight="1" s="29">
+    <row r="7" ht="115.2" customHeight="1" s="26">
       <c r="A7" s="3" t="inlineStr">
         <is>
           <t>TypeError</t>
@@ -4582,7 +4590,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="100.8" customHeight="1" s="29">
+    <row r="8" ht="100.8" customHeight="1" s="26">
       <c r="A8" s="3" t="inlineStr">
         <is>
           <t>KeyError</t>
@@ -4753,8 +4761,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="26.5546875" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
-    <col width="90.44140625" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
+    <col width="26.5546875" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="90.44140625" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4781,7 +4789,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="3" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A3" t="inlineStr">
         <is>
           <t>ConfigFail_Body</t>
@@ -4808,7 +4816,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="5" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A5" t="inlineStr">
         <is>
           <t>FileNotFound_Body</t>
@@ -4835,7 +4843,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="7" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A7" t="inlineStr">
         <is>
           <t>EmptyInput_Body</t>
@@ -4862,7 +4870,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="9" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A9" t="inlineStr">
         <is>
           <t>EmptyVendorName_Body</t>
@@ -4889,7 +4897,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="11" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A11" t="inlineStr">
         <is>
           <t>EmptyVendorNo_Body</t>
@@ -4916,7 +4924,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="13" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A13" t="inlineStr">
         <is>
           <t>EmptyTax_Body</t>
@@ -4943,7 +4951,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="15" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A15" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -4970,7 +4978,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="17" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A17" t="inlineStr">
         <is>
           <t>SheetMiss_Body</t>
@@ -4997,7 +5005,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="19" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A19" t="inlineStr">
         <is>
           <t>OutputNotFound_Body</t>
@@ -5024,7 +5032,7 @@
         </is>
       </c>
     </row>
-    <row r="21" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="21" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A21" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -5058,11 +5066,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="32.44140625" customWidth="1" style="29" min="1" max="1"/>
-    <col width="106.33203125" customWidth="1" style="29" min="2" max="2"/>
+    <col width="32.44140625" customWidth="1" style="26" min="1" max="1"/>
+    <col width="106.33203125" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" customHeight="1" s="29">
+    <row r="1" ht="15.6" customHeight="1" s="26">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Key</t>
@@ -5074,11 +5082,11 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="15.6" customHeight="1" s="29">
+    <row r="2" ht="15.6" customHeight="1" s="26">
       <c r="A2" s="25" t="n"/>
       <c r="B2" s="25" t="n"/>
     </row>
-    <row r="3" ht="15.6" customHeight="1" s="29">
+    <row r="3" ht="15.6" customHeight="1" s="26">
       <c r="A3" s="6" t="inlineStr">
         <is>
           <t>Sourcefile_subject</t>
@@ -5090,7 +5098,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="15.6" customHeight="1" s="29">
+    <row r="4" ht="15.6" customHeight="1" s="26">
       <c r="A4" s="25" t="inlineStr">
         <is>
           <t>Body_mail1</t>
@@ -5105,7 +5113,7 @@
     <row r="5">
       <c r="B5" s="19" t="n"/>
     </row>
-    <row r="6" ht="15.6" customHeight="1" s="29">
+    <row r="6" ht="15.6" customHeight="1" s="26">
       <c r="B6" s="8" t="inlineStr">
         <is>
           <t>The given source file is empty. Hence Vendor Wise Concentration process stopped executing.</t>
@@ -5115,21 +5123,21 @@
     <row r="7">
       <c r="B7" s="19" t="n"/>
     </row>
-    <row r="8" ht="15.6" customHeight="1" s="29">
+    <row r="8" ht="15.6" customHeight="1" s="26">
       <c r="B8" s="8" t="inlineStr">
         <is>
           <t>Thanks &amp; Regards,</t>
         </is>
       </c>
     </row>
-    <row r="9" ht="15.6" customHeight="1" s="29">
+    <row r="9" ht="15.6" customHeight="1" s="26">
       <c r="B9" s="8" t="inlineStr">
         <is>
           <t>Ln &amp; Co</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="15.6" customHeight="1" s="29">
+    <row r="10" ht="15.6" customHeight="1" s="26">
       <c r="A10" s="25" t="inlineStr">
         <is>
           <t>Gr_amount</t>
@@ -5141,7 +5149,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="15.6" customHeight="1" s="29">
+    <row r="11" ht="15.6" customHeight="1" s="26">
       <c r="A11" s="25" t="inlineStr">
         <is>
           <t>Gr_amount_body</t>
@@ -5156,7 +5164,7 @@
     <row r="12">
       <c r="B12" s="19" t="n"/>
     </row>
-    <row r="13" ht="15.6" customHeight="1" s="29">
+    <row r="13" ht="15.6" customHeight="1" s="26">
       <c r="B13" s="8" t="inlineStr">
         <is>
           <t>GR Amt. in loc.cur. column in source file is empty. Hence the Vendor Wise Concentration  ended executing.</t>
@@ -5166,21 +5174,21 @@
     <row r="14">
       <c r="B14" s="19" t="n"/>
     </row>
-    <row r="15" ht="15.6" customHeight="1" s="29">
+    <row r="15" ht="15.6" customHeight="1" s="26">
       <c r="B15" s="8" t="inlineStr">
         <is>
           <t>Thanks &amp; Regards,</t>
         </is>
       </c>
     </row>
-    <row r="16" ht="15.6" customHeight="1" s="29">
+    <row r="16" ht="15.6" customHeight="1" s="26">
       <c r="B16" s="8" t="inlineStr">
         <is>
           <t>Ln &amp; Co</t>
         </is>
       </c>
     </row>
-    <row r="17" ht="15.6" customHeight="1" s="29">
+    <row r="17" ht="15.6" customHeight="1" s="26">
       <c r="A17" s="6" t="inlineStr">
         <is>
           <t>Vendor_No</t>
@@ -5192,7 +5200,7 @@
         </is>
       </c>
     </row>
-    <row r="18" ht="15.6" customHeight="1" s="29">
+    <row r="18" ht="15.6" customHeight="1" s="26">
       <c r="A18" s="27" t="inlineStr">
         <is>
           <t>Vendor_No_body</t>
@@ -5207,7 +5215,7 @@
     <row r="19">
       <c r="B19" s="19" t="n"/>
     </row>
-    <row r="20" ht="15.6" customHeight="1" s="29">
+    <row r="20" ht="15.6" customHeight="1" s="26">
       <c r="B20" s="8" t="inlineStr">
         <is>
           <t>Vendor class column empty. Hence the Vendor Wise Concentration executing.</t>
@@ -5217,14 +5225,14 @@
     <row r="21">
       <c r="B21" s="19" t="n"/>
     </row>
-    <row r="22" ht="15.6" customHeight="1" s="29">
+    <row r="22" ht="15.6" customHeight="1" s="26">
       <c r="B22" s="8" t="inlineStr">
         <is>
           <t>Thanks &amp; Regards,</t>
         </is>
       </c>
     </row>
-    <row r="23" ht="15.6" customHeight="1" s="29">
+    <row r="23" ht="15.6" customHeight="1" s="26">
       <c r="A23" s="28" t="n"/>
       <c r="B23" s="8" t="inlineStr">
         <is>
@@ -5353,8 +5361,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="24.109375" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
-    <col width="90.44140625" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
+    <col width="24.109375" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="90.44140625" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5381,7 +5389,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="3" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A3" t="inlineStr">
         <is>
           <t>FileNotFound_Body</t>
@@ -5408,7 +5416,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="5" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A5" t="inlineStr">
         <is>
           <t>EmptyInput_Body</t>
@@ -5435,7 +5443,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="7" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A7" t="inlineStr">
         <is>
           <t>Key_Body</t>
@@ -5462,7 +5470,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="9" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A9" t="inlineStr">
         <is>
           <t>GRAmt_Subject</t>
@@ -5489,7 +5497,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="11" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A11" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -5516,7 +5524,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="13" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A13" t="inlineStr">
         <is>
           <t>SheetMiss_Body</t>
@@ -5543,7 +5551,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="15" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A15" t="inlineStr">
         <is>
           <t>OutputNotFound_Body</t>
@@ -5570,7 +5578,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="17" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A17" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -5700,11 +5708,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="28.109375" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
-    <col width="86.88671875" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
+    <col width="28.109375" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="86.88671875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.8" customHeight="1" s="29">
+    <row r="1" ht="13.8" customHeight="1" s="26">
       <c r="A1" s="14" t="inlineStr">
         <is>
           <t>Name</t>
@@ -5728,7 +5736,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="3" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A3" t="inlineStr">
         <is>
           <t>FileNotFound_Body</t>
@@ -5755,7 +5763,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="5" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A5" t="inlineStr">
         <is>
           <t>EmptyInput_Body</t>
@@ -5782,7 +5790,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="7" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A7" t="inlineStr">
         <is>
           <t>Plant_Body</t>
@@ -5809,7 +5817,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="9" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A9" t="inlineStr">
         <is>
           <t>GRAmt_Subject</t>
@@ -5836,7 +5844,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="100.8" customHeight="1" s="29">
+    <row r="11" ht="100.8" customHeight="1" s="26">
       <c r="A11" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -5863,7 +5871,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="13" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A13" t="inlineStr">
         <is>
           <t>SheetMiss_Body</t>
@@ -5890,7 +5898,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="15" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A15" t="inlineStr">
         <is>
           <t>OutputNotFound_Body</t>
@@ -5917,7 +5925,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="17" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A17" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
@@ -6047,8 +6055,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="28.6640625" bestFit="1" customWidth="1" style="29" min="1" max="1"/>
-    <col width="86.88671875" bestFit="1" customWidth="1" style="29" min="2" max="2"/>
+    <col width="28.6640625" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
+    <col width="86.88671875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6075,7 +6083,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="3" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A3" t="inlineStr">
         <is>
           <t>FileNotFound_Body</t>
@@ -6102,7 +6110,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="5" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A5" t="inlineStr">
         <is>
           <t>EmptyInput_Body</t>
@@ -6129,7 +6137,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="7" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A7" t="inlineStr">
         <is>
           <t>Date_Body</t>
@@ -6156,7 +6164,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="9" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A9" t="inlineStr">
         <is>
           <t>GRAmt_Subject</t>
@@ -6183,7 +6191,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="100.8" customHeight="1" s="29">
+    <row r="11" ht="100.8" customHeight="1" s="26">
       <c r="A11" t="inlineStr">
         <is>
           <t>ColumnMiss_Body</t>
@@ -6210,7 +6218,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="13" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A13" t="inlineStr">
         <is>
           <t>SheetMiss_Body</t>
@@ -6237,7 +6245,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="15" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A15" t="inlineStr">
         <is>
           <t>OutputNotFound_Body</t>
@@ -6264,7 +6272,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="86.40000000000001" customHeight="1" s="29">
+    <row r="17" ht="86.40000000000001" customHeight="1" s="26">
       <c r="A17" t="inlineStr">
         <is>
           <t>SystemError_Body</t>

</xml_diff>

<commit_message>
LnCo as on Dec 27
</commit_message>
<xml_diff>
--- a/Lnco/Input/Config.xlsx
+++ b/Lnco/Input/Config.xlsx
@@ -534,8 +534,8 @@
   </sheetPr>
   <dimension ref="A1:B95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="114" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="114" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -1052,9 +1052,27 @@
       <c r="B58" s="23" t="n"/>
     </row>
     <row r="59">
-      <c r="B59" s="23" t="n"/>
-    </row>
-    <row r="60"/>
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>MB51_Movement_types_list</t>
+        </is>
+      </c>
+      <c r="B59" s="23" t="inlineStr">
+        <is>
+          <t>[101, 102, 122, 123]</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Inventory_mapping_exception_percentage</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>10</v>
+      </c>
+    </row>
     <row r="61"/>
     <row r="62">
       <c r="A62" s="21" t="inlineStr">
@@ -3464,10 +3482,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -3617,25 +3635,53 @@
         </is>
       </c>
     </row>
-    <row r="16">
+    <row r="15" ht="100.8" customHeight="1" s="26">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Movement Type Subject</t>
+        </is>
+      </c>
+      <c r="B15" s="16" t="inlineStr">
+        <is>
+          <t>Inventory Mapping input file column data is empty</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="100.8" customHeight="1" s="26">
       <c r="A16" t="inlineStr">
         <is>
+          <t>Movement Type Body</t>
+        </is>
+      </c>
+      <c r="B16" s="17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello,
+Purchase Register Movement Type Column data is empty. 
+Thanks &amp; Regards,
+L &amp; Co   
+                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                           </t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
           <t>SystemError_Subject</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B18" t="inlineStr">
         <is>
           <t>Inventory Mapping Process System Error</t>
         </is>
       </c>
     </row>
-    <row r="17" ht="100.8" customHeight="1" s="26">
-      <c r="A17" t="inlineStr">
+    <row r="19" ht="100.8" customHeight="1" s="26">
+      <c r="A19" t="inlineStr">
         <is>
           <t>SystemError_Body</t>
         </is>
       </c>
-      <c r="B17" s="19" t="inlineStr">
+      <c r="B19" s="19" t="inlineStr">
         <is>
           <t xml:space="preserve">Hello,
 SystemError +. Inventory Mapping  process ended.
@@ -3645,28 +3691,28 @@
         </is>
       </c>
     </row>
-    <row r="20">
-      <c r="B20" s="17" t="n"/>
-    </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="B22" s="17" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
         <is>
           <t>subject_file_not_found</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <t>Inventory Mapping Input file is missing</t>
         </is>
       </c>
     </row>
-    <row r="23" ht="100.8" customHeight="1" s="26">
-      <c r="A23" t="inlineStr">
+    <row r="25" ht="100.8" customHeight="1" s="26">
+      <c r="A25" t="inlineStr">
         <is>
           <t>body_file_not_found</t>
         </is>
       </c>
-      <c r="B23" s="17" t="inlineStr">
+      <c r="B25" s="17" t="inlineStr">
         <is>
           <t xml:space="preserve">Hello,
 Inventory Mapping Sheet Input File is Missing. 
@@ -3676,25 +3722,25 @@
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
+    <row r="27">
+      <c r="A27" t="inlineStr">
         <is>
           <t>Purchase_ColumnMiss_Subject</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B27" t="inlineStr">
         <is>
           <t>Inventory Mapping  Process column missing</t>
         </is>
       </c>
     </row>
-    <row r="26" ht="100.8" customHeight="1" s="26">
-      <c r="A26" t="inlineStr">
+    <row r="28" ht="100.8" customHeight="1" s="26">
+      <c r="A28" t="inlineStr">
         <is>
           <t>Purchase_ColumnMiss_Body</t>
         </is>
       </c>
-      <c r="B26" s="19" t="inlineStr">
+      <c r="B28" s="19" t="inlineStr">
         <is>
           <t xml:space="preserve">Hello,
 ColumnName + column not found in the input. Hence Inventory Mapping process ended.
@@ -3704,25 +3750,25 @@
         </is>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
+    <row r="30">
+      <c r="A30" t="inlineStr">
         <is>
           <t>MB51_ColumnMiss_Subject</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B30" t="inlineStr">
         <is>
           <t>Inventory Mapping  Process column missing</t>
         </is>
       </c>
     </row>
-    <row r="29" ht="100.8" customHeight="1" s="26">
-      <c r="A29" t="inlineStr">
+    <row r="31" ht="100.8" customHeight="1" s="26">
+      <c r="A31" t="inlineStr">
         <is>
           <t>MB51_ColumnMiss_Body</t>
         </is>
       </c>
-      <c r="B29" s="19" t="inlineStr">
+      <c r="B31" s="19" t="inlineStr">
         <is>
           <t xml:space="preserve">Hello,
 ColumnName + column not found in the input. Hence Inventory Mapping process ended.
@@ -3732,25 +3778,25 @@
         </is>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
+    <row r="33">
+      <c r="A33" t="inlineStr">
         <is>
           <t>Material_Document_subject</t>
         </is>
       </c>
-      <c r="B31" s="16" t="inlineStr">
+      <c r="B33" s="16" t="inlineStr">
         <is>
           <t>Inventory Mapping input file column data is empty</t>
         </is>
       </c>
     </row>
-    <row r="32" ht="100.8" customHeight="1" s="26">
-      <c r="A32" t="inlineStr">
+    <row r="34" ht="100.8" customHeight="1" s="26">
+      <c r="A34" t="inlineStr">
         <is>
           <t>Material_Document_Body</t>
         </is>
       </c>
-      <c r="B32" s="17" t="inlineStr">
+      <c r="B34" s="17" t="inlineStr">
         <is>
           <t xml:space="preserve">Hello,
 MB51  Material Document Column data is empty. 
@@ -3760,31 +3806,31 @@
         </is>
       </c>
     </row>
-    <row r="33">
-      <c r="B33" s="16" t="n"/>
-    </row>
-    <row r="34">
-      <c r="B34" s="18" t="n"/>
-    </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="B35" s="16" t="n"/>
+    </row>
+    <row r="36">
+      <c r="B36" s="18" t="n"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
         <is>
           <t>Qty_unit_of_entry_Subject</t>
         </is>
       </c>
-      <c r="B35" s="16" t="inlineStr">
+      <c r="B37" s="16" t="inlineStr">
         <is>
           <t>Inventory Mapping input file column data is empty</t>
         </is>
       </c>
     </row>
-    <row r="36" ht="100.8" customHeight="1" s="26">
-      <c r="A36" t="inlineStr">
+    <row r="38" ht="100.8" customHeight="1" s="26">
+      <c r="A38" t="inlineStr">
         <is>
           <t>Qty_unit_of_entry_Body</t>
         </is>
       </c>
-      <c r="B36" s="17" t="inlineStr">
+      <c r="B38" s="17" t="inlineStr">
         <is>
           <t xml:space="preserve">Hello,
 MB51 Qty in unit of entry  Column data is empty. 

</xml_diff>

<commit_message>
LnCo as on Dec 28
</commit_message>
<xml_diff>
--- a/Lnco/Input/Config.xlsx
+++ b/Lnco/Input/Config.xlsx
@@ -535,7 +535,7 @@
   <dimension ref="A1:B95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScale="114" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -846,7 +846,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Output_Major_Vendor_analysis</t>
+          <t>Output_Major_Vendor_analysis_Sheet_name</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">

</xml_diff>

<commit_message>
LnCo as on Jan 3 2023
</commit_message>
<xml_diff>
--- a/Lnco/Input/Config.xlsx
+++ b/Lnco/Input/Config.xlsx
@@ -532,15 +532,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B95"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="114" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="114" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="48.5546875" customWidth="1" style="26" min="1" max="1"/>
+    <col width="59.33203125" bestFit="1" customWidth="1" style="26" min="1" max="1"/>
     <col width="84.21875" bestFit="1" customWidth="1" style="26" min="2" max="2"/>
     <col width="30.77734375" bestFit="1" customWidth="1" style="26" min="4" max="4"/>
   </cols>
@@ -795,50 +795,63 @@
     <row r="28">
       <c r="A28" s="21" t="inlineStr">
         <is>
-          <t>Output_Unit_Price_Exceptions_sheetname</t>
+          <t>Output_Unit_Price_Exception_change_in_amount_sheetname</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>exceptions unit price</t>
-        </is>
-      </c>
-    </row>
-    <row r="29"/>
+          <t>Unit price- change in amount</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="21" t="inlineStr">
+        <is>
+          <t>Output_Unit_Price_Exception_change_as_per_quantity_sheetname</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Unit price as per quantity</t>
+        </is>
+      </c>
+    </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="21" t="inlineStr">
+        <is>
+          <t>Output_Unit_Price_Exception_Unit_price_wise</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Unit price as per Unit Price</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="21" t="n"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
         <is>
           <t>Output_Inventory_Mapping_Sheetname</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B32" t="inlineStr">
         <is>
           <t>Inventory Mapping</t>
         </is>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Output_inventory_mapping_exceptions_sheetname</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>exceptions – inventory mapping</t>
-        </is>
-      </c>
-    </row>
-    <row r="32"/>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Output_Security_Cutoff_Sheet_name</t>
+          <t>Output_inventory_mapping_exceptions_sheetname</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Security Cutoff</t>
+          <t>exceptions – inventory mapping</t>
         </is>
       </c>
     </row>
@@ -846,216 +859,214 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>Output_Security_Cutoff_Sheet_name</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Security Cutoff</t>
+        </is>
+      </c>
+    </row>
+    <row r="36"/>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
           <t>Output_Major_Vendor_analysis_Sheet_name</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B37" t="inlineStr">
         <is>
           <t>Major Vendor Analysis</t>
         </is>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="21" t="inlineStr">
+    <row r="38">
+      <c r="A38" s="21" t="inlineStr">
         <is>
           <t>Other Keys</t>
         </is>
       </c>
-      <c r="B36" s="21" t="inlineStr">
+      <c r="B38" s="21" t="inlineStr">
         <is>
           <t>Other Values</t>
         </is>
       </c>
     </row>
-    <row r="37">
-      <c r="B37" s="15" t="n"/>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
+    <row r="39">
+      <c r="B39" s="15" t="n"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
         <is>
           <t>purchase_register_1st_column_name</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B40" t="inlineStr">
         <is>
           <t>Plant</t>
         </is>
       </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>purchase_register_2nd_column_name</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>GR Document Number</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="B40" s="15" t="n"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>purchase_register_2nd_column_name</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>GR Document Number</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" s="15" t="n"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
           <t>MB51_first_column</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B43" t="inlineStr">
         <is>
           <t>Plant</t>
         </is>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>MB51_second_column</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Material</t>
-        </is>
-      </c>
-    </row>
-    <row r="43"/>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>LOCAL_DOTENV_FILE</t>
+          <t>MB51_second_column</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>local_new.env</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>QUALITY_DOTENV_FILE</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>quality.env</t>
-        </is>
-      </c>
-    </row>
+          <t>Material</t>
+        </is>
+      </c>
+    </row>
+    <row r="45"/>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ENV_FILE</t>
+          <t>LOCAL_DOTENV_FILE</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>LOCAL_DOTENV_FILE</t>
-        </is>
-      </c>
-    </row>
-    <row r="47"/>
+          <t>local_new.env</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>QUALITY_DOTENV_FILE</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>quality.env</t>
+        </is>
+      </c>
+    </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Request Status Name</t>
+          <t>ENV_FILE</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Request Status Name</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>New_Request_Status</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>New</t>
-        </is>
-      </c>
-    </row>
+          <t>LOCAL_DOTENV_FILE</t>
+        </is>
+      </c>
+    </row>
+    <row r="49"/>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>In_Progress_Request_Status</t>
+          <t>Request Status Name</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>In Progress</t>
+          <t>Request Status Name</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Success_Request_Status</t>
+          <t>New_Request_Status</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Completed</t>
+          <t>New</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Fail_Request_Status</t>
+          <t>In_Progress_Request_Status</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Failed</t>
-        </is>
-      </c>
-    </row>
-    <row r="53"/>
+          <t>In Progress</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Success_Request_Status</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+    </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
+          <t>Fail_Request_Status</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+    </row>
+    <row r="55"/>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
           <t>To_Mail_Address</t>
         </is>
       </c>
-      <c r="B54" s="15" t="inlineStr">
+      <c r="B56" s="15" t="inlineStr">
         <is>
           <t>kalyan.gundu@bradsol.com</t>
         </is>
       </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>CC_Mail_Address</t>
-        </is>
-      </c>
-      <c r="B55" s="15" t="inlineStr">
-        <is>
-          <t>kalyan.gundu@bradsol.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="B56" s="23" t="n"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>security_cutoff_date_list</t>
-        </is>
-      </c>
-      <c r="B57" s="23" t="inlineStr">
-        <is>
-          <t>[26, 27, 28, 29, 30, 31]</t>
+          <t>CC_Mail_Address</t>
+        </is>
+      </c>
+      <c r="B57" s="15" t="inlineStr">
+        <is>
+          <t>kalyan.gundu@bradsol.com</t>
         </is>
       </c>
     </row>
@@ -1065,252 +1076,288 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
+          <t>security_cutoff_date_list</t>
+        </is>
+      </c>
+      <c r="B59" s="23" t="inlineStr">
+        <is>
+          <t>[26, 27, 28, 29, 30, 31]</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" s="23" t="n"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
           <t>MB51_Movement_types_list</t>
         </is>
       </c>
-      <c r="B59" s="23" t="inlineStr">
+      <c r="B61" s="23" t="inlineStr">
         <is>
           <t>[101, 102, 122, 123]</t>
         </is>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
+    <row r="62">
+      <c r="A62" t="inlineStr">
         <is>
           <t>Inventory_mapping_exception_percentage</t>
         </is>
       </c>
-      <c r="B60" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61"/>
-    <row r="62">
-      <c r="A62" s="21" t="inlineStr">
-        <is>
-          <t>Sheet Name keys in Config File</t>
-        </is>
-      </c>
-      <c r="B62" s="21" t="inlineStr">
-        <is>
-          <t>SheetName values in Config file</t>
-        </is>
+      <c r="B62" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Config_Comparatives_Purchase_sheetname</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>Purchase Wise Comparatives</t>
-        </is>
+          <t>unit_price_comparison_unit_price_exception_percentage</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Config_Comparatives_Month_sheetname</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>Month Wise Comparatives</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>Config_Comparatives_Plant_sheetname</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>Plant Wise Comparatives</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>Config_Comparatives_Dom&amp;Imp_sheetname</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>Dom&amp;Imp Wise Comparatives</t>
-        </is>
-      </c>
-    </row>
+          <t>unit_price_comparison_quantity_exception_percentage</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65"/>
+    <row r="66"/>
     <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>Config_Comparatives_Vendor_sheetname</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>Vendor Wise Comparatives</t>
-        </is>
-      </c>
-    </row>
-    <row r="68"/>
+      <c r="A67" s="21" t="inlineStr">
+        <is>
+          <t>Sheet Name keys in Config File</t>
+        </is>
+      </c>
+      <c r="B67" s="21" t="inlineStr">
+        <is>
+          <t>SheetName values in Config file</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Config_Comparatives_Purchase_sheetname</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Purchase Wise Comparatives</t>
+        </is>
+      </c>
+    </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Config_Concentrations_Purchase_sheetname</t>
+          <t>Config_Comparatives_Month_sheetname</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Purchase Wise Concentration</t>
+          <t>Month Wise Comparatives</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Config_Concentrations_Month_sheetname</t>
+          <t>Config_Comparatives_Plant_sheetname</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Month Wise Concentration</t>
+          <t>Plant Wise Comparatives</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Config_Concentrations_Plant_sheetname</t>
+          <t>Config_Comparatives_Dom&amp;Imp_sheetname</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Plant Wise Concentration</t>
+          <t>Dom&amp;Imp Wise Comparatives</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Config_Concentrations_Dom&amp;Imp_sheetname</t>
+          <t>Config_Comparatives_Vendor_sheetname</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Dom&amp;Imp Wise Concentration</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>Config_Concentration_Vendor_sheetname</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>Vendor Wise Concentration</t>
-        </is>
-      </c>
-    </row>
-    <row r="74"/>
+          <t>Vendor Wise Comparatives</t>
+        </is>
+      </c>
+    </row>
+    <row r="73"/>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Config_Concentrations_Purchase_sheetname</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Purchase Wise Concentration</t>
+        </is>
+      </c>
+    </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Config_Duplication_of_Vendor_sheetname</t>
+          <t>Config_Concentrations_Month_sheetname</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Duplication Of Vendor</t>
+          <t>Month Wise Concentration</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Config_Average_Day_Purchase_sheetname</t>
+          <t>Config_Concentrations_Plant_sheetname</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Average Day Purchase</t>
+          <t>Plant Wise Concentration</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Config_Same_Material_Purchases_DVDP_sheetname</t>
+          <t>Config_Concentrations_Dom&amp;Imp_sheetname</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>SMP from DVnDP</t>
+          <t>Dom&amp;Imp Wise Concentration</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Config_Unit_Price_Comparison_sheetname</t>
+          <t>Config_Concentration_Vendor_sheetname</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Unit Price Comparison</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>Config_Inventory_Mapping_Sheetname</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>Inventory Mapping</t>
-        </is>
-      </c>
-    </row>
-    <row r="80"/>
+          <t>Vendor Wise Concentration</t>
+        </is>
+      </c>
+    </row>
+    <row r="79"/>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Config_Duplication_of_Vendor_sheetname</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Duplication Of Vendor</t>
+        </is>
+      </c>
+    </row>
     <row r="81">
-      <c r="A81" s="21" t="inlineStr">
-        <is>
-          <t>Mails related Keys</t>
-        </is>
-      </c>
-      <c r="B81" s="21" t="inlineStr">
-        <is>
-          <t>Values</t>
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Config_Average_Day_Purchase_sheetname</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Average Day Purchase</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
+          <t>Config_Same_Material_Purchases_DVDP_sheetname</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>SMP from DVnDP</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Config_Unit_Price_Comparison_sheetname</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Unit Price Comparison</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Config_Inventory_Mapping_Sheetname</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Inventory Mapping</t>
+        </is>
+      </c>
+    </row>
+    <row r="85"/>
+    <row r="86">
+      <c r="A86" s="21" t="inlineStr">
+        <is>
+          <t>Mails related Keys</t>
+        </is>
+      </c>
+      <c r="B86" s="21" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
           <t>Start_Mail_Subject</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr">
+      <c r="B87" t="inlineStr">
         <is>
           <t xml:space="preserve">Bot execution is started </t>
         </is>
       </c>
     </row>
-    <row r="83" ht="86.40000000000001" customHeight="1" s="26">
-      <c r="A83" t="inlineStr">
+    <row r="88" ht="86.40000000000001" customHeight="1" s="26">
+      <c r="A88" t="inlineStr">
         <is>
           <t>Start_Mail_Body</t>
         </is>
       </c>
-      <c r="B83" s="19" t="inlineStr">
+      <c r="B88" s="19" t="inlineStr">
         <is>
           <t>Hello,
 Bot has started processing the purchase register report automation
@@ -1319,26 +1366,26 @@
         </is>
       </c>
     </row>
-    <row r="84"/>
-    <row r="85">
-      <c r="A85" t="inlineStr">
+    <row r="89"/>
+    <row r="90">
+      <c r="A90" t="inlineStr">
         <is>
           <t>Success_Mail_Subject</t>
         </is>
       </c>
-      <c r="B85" t="inlineStr">
+      <c r="B90" t="inlineStr">
         <is>
           <t xml:space="preserve">Bot execution is completed </t>
         </is>
       </c>
     </row>
-    <row r="86" ht="86.40000000000001" customHeight="1" s="26">
-      <c r="A86" t="inlineStr">
+    <row r="91" ht="86.40000000000001" customHeight="1" s="26">
+      <c r="A91" t="inlineStr">
         <is>
           <t>Success_Mail_Body</t>
         </is>
       </c>
-      <c r="B86" s="19" t="inlineStr">
+      <c r="B91" s="19" t="inlineStr">
         <is>
           <t>Hello,
 Bot has Successfully completed the purchase register report automation.
@@ -1347,26 +1394,26 @@
         </is>
       </c>
     </row>
-    <row r="87"/>
-    <row r="88">
-      <c r="A88" t="inlineStr">
+    <row r="92"/>
+    <row r="93">
+      <c r="A93" t="inlineStr">
         <is>
           <t>subject_file_not_found</t>
         </is>
       </c>
-      <c r="B88" t="inlineStr">
+      <c r="B93" t="inlineStr">
         <is>
           <t>Bot Execution is stopped - Input file is missing</t>
         </is>
       </c>
     </row>
-    <row r="89" ht="100.8" customHeight="1" s="26">
-      <c r="A89" t="inlineStr">
+    <row r="94" ht="100.8" customHeight="1" s="26">
+      <c r="A94" t="inlineStr">
         <is>
           <t>body_file_not_found</t>
         </is>
       </c>
-      <c r="B89" s="17" t="inlineStr">
+      <c r="B94" s="17" t="inlineStr">
         <is>
           <t xml:space="preserve">Hello,
 Purchase Register Input File is Missing. Hence stopping the execution of the program.
@@ -1376,28 +1423,28 @@
         </is>
       </c>
     </row>
-    <row r="90">
-      <c r="B90" s="13" t="n"/>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
+    <row r="95">
+      <c r="B95" s="13" t="n"/>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
         <is>
           <t>subject_sheet_not_found</t>
         </is>
       </c>
-      <c r="B91" t="inlineStr">
+      <c r="B96" t="inlineStr">
         <is>
           <t>Bot Execution is stopped - Input file sheet is missing</t>
         </is>
       </c>
     </row>
-    <row r="92" ht="100.8" customHeight="1" s="26">
-      <c r="A92" t="inlineStr">
+    <row r="97" ht="100.8" customHeight="1" s="26">
+      <c r="A97" t="inlineStr">
         <is>
           <t>body_sheet_not_found</t>
         </is>
       </c>
-      <c r="B92" s="17" t="inlineStr">
+      <c r="B97" s="17" t="inlineStr">
         <is>
           <t xml:space="preserve">Hello,
 Purchase Register Input File sheet is Missing. Hence stopping the execution of the program.
@@ -1407,26 +1454,26 @@
         </is>
       </c>
     </row>
-    <row r="93"/>
-    <row r="94">
-      <c r="A94" t="inlineStr">
+    <row r="98"/>
+    <row r="99">
+      <c r="A99" t="inlineStr">
         <is>
           <t>subject_in_progress_request_found</t>
         </is>
       </c>
-      <c r="B94" t="inlineStr">
+      <c r="B99" t="inlineStr">
         <is>
           <t>Bot Execution is stopped - prior requests are in progress</t>
         </is>
       </c>
     </row>
-    <row r="95" ht="100.8" customHeight="1" s="26">
-      <c r="A95" t="inlineStr">
+    <row r="100" ht="100.8" customHeight="1" s="26">
+      <c r="A100" t="inlineStr">
         <is>
           <t>body_in_progress_request_found</t>
         </is>
       </c>
-      <c r="B95" s="17" t="inlineStr">
+      <c r="B100" s="17" t="inlineStr">
         <is>
           <t xml:space="preserve">Hello,
 The bot is executing prior requests. Hence stopping the execution of the program.
@@ -1438,13 +1485,13 @@
     </row>
   </sheetData>
   <dataValidations xWindow="832" yWindow="791" count="1">
-    <dataValidation sqref="B46:B47" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Select Correct File" error="Should be same as Input message provided" promptTitle="Select Env File type" prompt="LOCAL_DOTENV_FILE (or) QUALTIY_DOTENV_FILE" type="list">
-      <formula1>$A$44:$A$45</formula1>
+    <dataValidation sqref="B48:B49" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Select Correct File" error="Should be same as Input message provided" promptTitle="Select Env File type" prompt="LOCAL_DOTENV_FILE (or) QUALTIY_DOTENV_FILE" type="list">
+      <formula1>$A$46:$A$47</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B54" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B55" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B56" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B57" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -3866,7 +3913,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
LnCo as on Jan 04 2023
</commit_message>
<xml_diff>
--- a/Lnco/Input/Config.xlsx
+++ b/Lnco/Input/Config.xlsx
@@ -532,10 +532,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B100"/>
+  <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="114" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="114" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -651,7 +651,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>exceptions – COMPARITIVES</t>
+          <t>exceptions – COMPARATIVES</t>
         </is>
       </c>
     </row>
@@ -881,207 +881,194 @@
         </is>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="21" t="inlineStr">
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40">
+      <c r="A40" s="21" t="inlineStr">
         <is>
           <t>Other Keys</t>
         </is>
       </c>
-      <c r="B38" s="21" t="inlineStr">
+      <c r="B40" s="21" t="inlineStr">
         <is>
           <t>Other Values</t>
         </is>
       </c>
     </row>
-    <row r="39">
-      <c r="B39" s="15" t="n"/>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
+    <row r="41">
+      <c r="B41" s="15" t="n"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
         <is>
           <t>purchase_register_1st_column_name</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B42" t="inlineStr">
         <is>
           <t>Plant</t>
         </is>
       </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>purchase_register_2nd_column_name</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>GR Document Number</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="B42" s="15" t="n"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>purchase_register_2nd_column_name</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>GR Document Number</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" s="15" t="n"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
           <t>MB51_first_column</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B45" t="inlineStr">
         <is>
           <t>Plant</t>
         </is>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>MB51_second_column</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Material</t>
-        </is>
-      </c>
-    </row>
-    <row r="45"/>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>LOCAL_DOTENV_FILE</t>
+          <t>MB51_second_column</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>local_new.env</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>QUALITY_DOTENV_FILE</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>quality.env</t>
-        </is>
-      </c>
-    </row>
+          <t>Material</t>
+        </is>
+      </c>
+    </row>
+    <row r="47"/>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ENV_FILE</t>
+          <t>LOCAL_DOTENV_FILE</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>LOCAL_DOTENV_FILE</t>
-        </is>
-      </c>
-    </row>
-    <row r="49"/>
+          <t>local_new.env</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>QUALITY_DOTENV_FILE</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>quality.env</t>
+        </is>
+      </c>
+    </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Request Status Name</t>
+          <t>ENV_FILE</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Request Status Name</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>New_Request_Status</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>New</t>
-        </is>
-      </c>
-    </row>
+          <t>LOCAL_DOTENV_FILE</t>
+        </is>
+      </c>
+    </row>
+    <row r="51"/>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>In_Progress_Request_Status</t>
+          <t>Request Status Name</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>In Progress</t>
+          <t>Request Status Name</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Success_Request_Status</t>
+          <t>New_Request_Status</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Completed</t>
+          <t>New</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Fail_Request_Status</t>
+          <t>In_Progress_Request_Status</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Failed</t>
-        </is>
-      </c>
-    </row>
-    <row r="55"/>
+          <t>In Progress</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Success_Request_Status</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+    </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
+          <t>Fail_Request_Status</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+    </row>
+    <row r="57"/>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
           <t>To_Mail_Address</t>
         </is>
       </c>
-      <c r="B56" s="15" t="inlineStr">
+      <c r="B58" s="15" t="inlineStr">
         <is>
           <t>kalyan.gundu@bradsol.com</t>
         </is>
       </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>CC_Mail_Address</t>
-        </is>
-      </c>
-      <c r="B57" s="15" t="inlineStr">
-        <is>
-          <t>kalyan.gundu@bradsol.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="B58" s="23" t="n"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>security_cutoff_date_list</t>
-        </is>
-      </c>
-      <c r="B59" s="23" t="inlineStr">
-        <is>
-          <t>[26, 27, 28, 29, 30, 31]</t>
+          <t>CC_Mail_Address</t>
+        </is>
+      </c>
+      <c r="B59" s="15" t="inlineStr">
+        <is>
+          <t>kalyan.gundu@bradsol.com</t>
         </is>
       </c>
     </row>
@@ -1091,273 +1078,288 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>MB51_Movement_types_list</t>
+          <t>security_cutoff_date_list</t>
         </is>
       </c>
       <c r="B61" s="23" t="inlineStr">
         <is>
-          <t>[101, 102, 122, 123]</t>
+          <t>[26, 27, 28, 29, 30, 31]</t>
         </is>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>Inventory_mapping_exception_percentage</t>
-        </is>
-      </c>
-      <c r="B62" t="n">
-        <v>50</v>
-      </c>
+      <c r="B62" s="23" t="n"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>unit_price_comparison_unit_price_exception_percentage</t>
-        </is>
-      </c>
-      <c r="B63" t="n">
-        <v>5</v>
+          <t>MB51_Movement_types_list</t>
+        </is>
+      </c>
+      <c r="B63" s="23" t="inlineStr">
+        <is>
+          <t>[101, 102, 122, 123]</t>
+        </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
+          <t>Inventory_mapping_exception_percentage</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>unit_price_comparison_unit_price_exception_percentage</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
           <t>unit_price_comparison_quantity_exception_percentage</t>
         </is>
       </c>
-      <c r="B64" t="n">
+      <c r="B66" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="65"/>
-    <row r="66"/>
-    <row r="67">
-      <c r="A67" s="21" t="inlineStr">
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69">
+      <c r="A69" s="21" t="inlineStr">
         <is>
           <t>Sheet Name keys in Config File</t>
         </is>
       </c>
-      <c r="B67" s="21" t="inlineStr">
+      <c r="B69" s="21" t="inlineStr">
         <is>
           <t>SheetName values in Config file</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Config_Comparatives_Purchase_sheetname</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>Purchase Wise Comparatives</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>Config_Comparatives_Month_sheetname</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>Month Wise Comparatives</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Config_Comparatives_Plant_sheetname</t>
+          <t>Config_Comparatives_Purchase_sheetname</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Plant Wise Comparatives</t>
+          <t>Purchase Wise Comparatives</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Config_Comparatives_Dom&amp;Imp_sheetname</t>
+          <t>Config_Comparatives_Month_sheetname</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Dom&amp;Imp Wise Comparatives</t>
+          <t>Month Wise Comparatives</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Config_Comparatives_Vendor_sheetname</t>
+          <t>Config_Comparatives_Plant_sheetname</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Vendor Wise Comparatives</t>
-        </is>
-      </c>
-    </row>
-    <row r="73"/>
+          <t>Plant Wise Comparatives</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Config_Comparatives_Dom&amp;Imp_sheetname</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Dom&amp;Imp Wise Comparatives</t>
+        </is>
+      </c>
+    </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Config_Concentrations_Purchase_sheetname</t>
+          <t>Config_Comparatives_Vendor_sheetname</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Purchase Wise Concentration</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>Config_Concentrations_Month_sheetname</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>Month Wise Concentration</t>
-        </is>
-      </c>
-    </row>
+          <t>Vendor Wise Comparatives</t>
+        </is>
+      </c>
+    </row>
+    <row r="75"/>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Config_Concentrations_Plant_sheetname</t>
+          <t>Config_Concentrations_Purchase_sheetname</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Plant Wise Concentration</t>
+          <t>Purchase Wise Concentration</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Config_Concentrations_Dom&amp;Imp_sheetname</t>
+          <t>Config_Concentrations_Month_sheetname</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Dom&amp;Imp Wise Concentration</t>
+          <t>Month Wise Concentration</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Config_Concentration_Vendor_sheetname</t>
+          <t>Config_Concentrations_Plant_sheetname</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Vendor Wise Concentration</t>
-        </is>
-      </c>
-    </row>
-    <row r="79"/>
+          <t>Plant Wise Concentration</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Config_Concentrations_Dom&amp;Imp_sheetname</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Dom&amp;Imp Wise Concentration</t>
+        </is>
+      </c>
+    </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Config_Duplication_of_Vendor_sheetname</t>
+          <t>Config_Concentration_Vendor_sheetname</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Duplication Of Vendor</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>Config_Average_Day_Purchase_sheetname</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>Average Day Purchase</t>
-        </is>
-      </c>
-    </row>
+          <t>Vendor Wise Concentration</t>
+        </is>
+      </c>
+    </row>
+    <row r="81"/>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Config_Same_Material_Purchases_DVDP_sheetname</t>
+          <t>Config_Duplication_of_Vendor_sheetname</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>SMP from DVnDP</t>
+          <t>Duplication Of Vendor</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Config_Unit_Price_Comparison_sheetname</t>
+          <t>Config_Average_Day_Purchase_sheetname</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Unit Price Comparison</t>
+          <t>Average Day Purchase</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
+          <t>Config_Same_Material_Purchases_DVDP_sheetname</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>SMP from DVnDP</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Config_Unit_Price_Comparison_sheetname</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Unit Price Comparison</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
           <t>Config_Inventory_Mapping_Sheetname</t>
         </is>
       </c>
-      <c r="B84" t="inlineStr">
+      <c r="B86" t="inlineStr">
         <is>
           <t>Inventory Mapping</t>
         </is>
       </c>
     </row>
-    <row r="85"/>
-    <row r="86">
-      <c r="A86" s="21" t="inlineStr">
+    <row r="87"/>
+    <row r="88">
+      <c r="A88" s="21" t="inlineStr">
         <is>
           <t>Mails related Keys</t>
         </is>
       </c>
-      <c r="B86" s="21" t="inlineStr">
+      <c r="B88" s="21" t="inlineStr">
         <is>
           <t>Values</t>
         </is>
       </c>
     </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
+    <row r="89">
+      <c r="A89" t="inlineStr">
         <is>
           <t>Start_Mail_Subject</t>
         </is>
       </c>
-      <c r="B87" t="inlineStr">
+      <c r="B89" t="inlineStr">
         <is>
           <t xml:space="preserve">Bot execution is started </t>
         </is>
       </c>
     </row>
-    <row r="88" ht="86.40000000000001" customHeight="1" s="26">
-      <c r="A88" t="inlineStr">
+    <row r="90" ht="86.40000000000001" customHeight="1" s="26">
+      <c r="A90" t="inlineStr">
         <is>
           <t>Start_Mail_Body</t>
         </is>
       </c>
-      <c r="B88" s="19" t="inlineStr">
+      <c r="B90" s="19" t="inlineStr">
         <is>
           <t>Hello,
 Bot has started processing the purchase register report automation
@@ -1366,26 +1368,26 @@
         </is>
       </c>
     </row>
-    <row r="89"/>
-    <row r="90">
-      <c r="A90" t="inlineStr">
+    <row r="91"/>
+    <row r="92">
+      <c r="A92" t="inlineStr">
         <is>
           <t>Success_Mail_Subject</t>
         </is>
       </c>
-      <c r="B90" t="inlineStr">
+      <c r="B92" t="inlineStr">
         <is>
           <t xml:space="preserve">Bot execution is completed </t>
         </is>
       </c>
     </row>
-    <row r="91" ht="86.40000000000001" customHeight="1" s="26">
-      <c r="A91" t="inlineStr">
+    <row r="93" ht="86.40000000000001" customHeight="1" s="26">
+      <c r="A93" t="inlineStr">
         <is>
           <t>Success_Mail_Body</t>
         </is>
       </c>
-      <c r="B91" s="19" t="inlineStr">
+      <c r="B93" s="19" t="inlineStr">
         <is>
           <t>Hello,
 Bot has Successfully completed the purchase register report automation.
@@ -1394,26 +1396,26 @@
         </is>
       </c>
     </row>
-    <row r="92"/>
-    <row r="93">
-      <c r="A93" t="inlineStr">
+    <row r="94"/>
+    <row r="95">
+      <c r="A95" t="inlineStr">
         <is>
           <t>subject_file_not_found</t>
         </is>
       </c>
-      <c r="B93" t="inlineStr">
+      <c r="B95" t="inlineStr">
         <is>
           <t>Bot Execution is stopped - Input file is missing</t>
         </is>
       </c>
     </row>
-    <row r="94" ht="100.8" customHeight="1" s="26">
-      <c r="A94" t="inlineStr">
+    <row r="96" ht="100.8" customHeight="1" s="26">
+      <c r="A96" t="inlineStr">
         <is>
           <t>body_file_not_found</t>
         </is>
       </c>
-      <c r="B94" s="17" t="inlineStr">
+      <c r="B96" s="17" t="inlineStr">
         <is>
           <t xml:space="preserve">Hello,
 Purchase Register Input File is Missing. Hence stopping the execution of the program.
@@ -1423,28 +1425,28 @@
         </is>
       </c>
     </row>
-    <row r="95">
-      <c r="B95" s="13" t="n"/>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
+    <row r="97">
+      <c r="B97" s="13" t="n"/>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
         <is>
           <t>subject_sheet_not_found</t>
         </is>
       </c>
-      <c r="B96" t="inlineStr">
+      <c r="B98" t="inlineStr">
         <is>
           <t>Bot Execution is stopped - Input file sheet is missing</t>
         </is>
       </c>
     </row>
-    <row r="97" ht="100.8" customHeight="1" s="26">
-      <c r="A97" t="inlineStr">
+    <row r="99" ht="100.8" customHeight="1" s="26">
+      <c r="A99" t="inlineStr">
         <is>
           <t>body_sheet_not_found</t>
         </is>
       </c>
-      <c r="B97" s="17" t="inlineStr">
+      <c r="B99" s="17" t="inlineStr">
         <is>
           <t xml:space="preserve">Hello,
 Purchase Register Input File sheet is Missing. Hence stopping the execution of the program.
@@ -1454,26 +1456,26 @@
         </is>
       </c>
     </row>
-    <row r="98"/>
-    <row r="99">
-      <c r="A99" t="inlineStr">
+    <row r="100"/>
+    <row r="101">
+      <c r="A101" t="inlineStr">
         <is>
           <t>subject_in_progress_request_found</t>
         </is>
       </c>
-      <c r="B99" t="inlineStr">
+      <c r="B101" t="inlineStr">
         <is>
           <t>Bot Execution is stopped - prior requests are in progress</t>
         </is>
       </c>
     </row>
-    <row r="100" ht="100.8" customHeight="1" s="26">
-      <c r="A100" t="inlineStr">
+    <row r="102" ht="100.8" customHeight="1" s="26">
+      <c r="A102" t="inlineStr">
         <is>
           <t>body_in_progress_request_found</t>
         </is>
       </c>
-      <c r="B100" s="17" t="inlineStr">
+      <c r="B102" s="17" t="inlineStr">
         <is>
           <t xml:space="preserve">Hello,
 The bot is executing prior requests. Hence stopping the execution of the program.
@@ -1485,13 +1487,13 @@
     </row>
   </sheetData>
   <dataValidations xWindow="832" yWindow="791" count="1">
-    <dataValidation sqref="B48:B49" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Select Correct File" error="Should be same as Input message provided" promptTitle="Select Env File type" prompt="LOCAL_DOTENV_FILE (or) QUALTIY_DOTENV_FILE" type="list">
-      <formula1>$A$46:$A$47</formula1>
+    <dataValidation sqref="B50:B51" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Select Correct File" error="Should be same as Input message provided" promptTitle="Select Env File type" prompt="LOCAL_DOTENV_FILE (or) QUALTIY_DOTENV_FILE" type="list">
+      <formula1>$A$48:$A$49</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B56" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B57" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B58" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B59" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -3542,8 +3544,8 @@
   </sheetPr>
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -3572,7 +3574,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Row Labels</t>
+          <t>GR Document Number</t>
         </is>
       </c>
     </row>
@@ -3913,7 +3915,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
LnCO as on 19 Jan 2023
</commit_message>
<xml_diff>
--- a/Lnco/Input/Config.xlsx
+++ b/Lnco/Input/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BRADSOL-User\Documents\GitHub\brad-lnco-projects\Lnco\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0363E3B8-A68F-41E4-BD86-A8AB83DFC7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D43D5C-4CD6-49CB-A09B-2218EAF250F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="954" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4204,12 +4204,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4220,6 +4214,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6296,8 +6296,8 @@
   </sheetPr>
   <dimension ref="A1:B146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="114" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="114" workbookViewId="0">
+      <selection activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6332,7 +6332,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="25" t="s">
         <v>452</v>
       </c>
     </row>
@@ -6840,7 +6840,7 @@
       </c>
     </row>
     <row r="90" spans="1:2">
-      <c r="A90" s="29" t="s">
+      <c r="A90" s="25" t="s">
         <v>453</v>
       </c>
     </row>
@@ -8058,7 +8058,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="29" t="s">
         <v>254</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -8066,27 +8066,27 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="26"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="19"/>
     </row>
     <row r="6" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A6" s="26"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="8" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="26"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="19"/>
     </row>
     <row r="8" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A8" s="26"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="8" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A9" s="26"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="8" t="s">
         <v>258</v>
       </c>
@@ -8100,7 +8100,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="29" t="s">
         <v>261</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -8108,27 +8108,27 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="26"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="19"/>
     </row>
     <row r="13" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A13" s="26"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="8" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="26"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="19"/>
     </row>
     <row r="15" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A15" s="26"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="8" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A16" s="26"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="8" t="s">
         <v>258</v>
       </c>
@@ -8142,7 +8142,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="31" t="s">
         <v>265</v>
       </c>
       <c r="B18" s="8" t="s">
@@ -8150,27 +8150,27 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="26"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="19"/>
     </row>
     <row r="20" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A20" s="26"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="8" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="26"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="19"/>
     </row>
     <row r="22" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A22" s="26"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="8" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A23" s="28"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="8" t="s">
         <v>258</v>
       </c>
@@ -11266,7 +11266,7 @@
     </row>
     <row r="2" spans="1:2" ht="15.6">
       <c r="A2" s="24"/>
-      <c r="B2" s="30"/>
+      <c r="B2" s="26"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
@@ -11556,7 +11556,7 @@
     </row>
     <row r="2" spans="1:2" ht="15.6">
       <c r="A2" s="24"/>
-      <c r="B2" s="30"/>
+      <c r="B2" s="26"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
@@ -11904,7 +11904,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="100.95" customHeight="1">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="27" t="s">
         <v>648</v>
       </c>
       <c r="B10" s="17" t="s">
@@ -12247,7 +12247,7 @@
     </row>
     <row r="2" spans="1:2" ht="15.6">
       <c r="A2" s="24"/>
-      <c r="B2" s="32"/>
+      <c r="B2" s="28"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
LnCO as on 20 Jan 2023
</commit_message>
<xml_diff>
--- a/Lnco/Input/Config.xlsx
+++ b/Lnco/Input/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BRADSOL-User\Documents\GitHub\brad-lnco-projects\Lnco\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEB019F-0B1D-4DFF-BBA4-6FE69ACA94BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E611B7-0404-4C5B-B7C4-5D2ECA3228C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="954" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="954" firstSheet="8" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequence Check" sheetId="18" r:id="rId1"/>
@@ -6092,7 +6092,7 @@
   </sheetPr>
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -6607,8 +6607,8 @@
   </sheetPr>
   <dimension ref="A1:B167"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" zoomScale="114" workbookViewId="0">
-      <selection activeCell="A151" sqref="A151"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="114" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
LnCo as on Jan 23 2023
</commit_message>
<xml_diff>
--- a/Lnco/Input/Config.xlsx
+++ b/Lnco/Input/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BRADSOL-User\Documents\GitHub\brad-lnco-projects\Lnco\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E611B7-0404-4C5B-B7C4-5D2ECA3228C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888B9A90-516C-4D80-9311-A384B63A92FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="954" firstSheet="8" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="Sequence Check" sheetId="18" r:id="rId1"/>
     <sheet name="GST Rate Check" sheetId="17" r:id="rId2"/>
     <sheet name="Customer_Wise_Concentration" sheetId="19" r:id="rId3"/>
-    <sheet name="Month_Wise_Concentration" sheetId="20" r:id="rId4"/>
-    <sheet name="Plant_Wise_Concentration" sheetId="21" r:id="rId5"/>
+    <sheet name="Sales_Month_Wise_Concentration" sheetId="20" r:id="rId4"/>
+    <sheet name="Sales_Plant_Wise_Concentration" sheetId="21" r:id="rId5"/>
     <sheet name="Type_of_Sale_Wise_Concentration" sheetId="22" r:id="rId6"/>
     <sheet name="SalesRegister_Vs_Mb51" sheetId="23" r:id="rId7"/>
     <sheet name="Product_Mix_Comparision" sheetId="24" r:id="rId8"/>
@@ -1823,12 +1823,6 @@
     <t>Config_Concentrations_Customer_sheetname</t>
   </si>
   <si>
-    <t>Month_Wise_Concentration</t>
-  </si>
-  <si>
-    <t>Plant_Wise_Concentration</t>
-  </si>
-  <si>
     <t>Config_Concentrations_Type_of_sale_sheetname</t>
   </si>
   <si>
@@ -4134,6 +4128,12 @@
   </si>
   <si>
     <t>PITTI  RAIL AND ENGINEERING COMPONE,Pitti Casting Private Limited,PITTI TRADE AND INVESTMENT PVT. LTD</t>
+  </si>
+  <si>
+    <t>Sales_Month_Wise_Concentration</t>
+  </si>
+  <si>
+    <t>Sales_Plant_Wise_Concentration</t>
   </si>
 </sst>
 </file>
@@ -4835,7 +4835,7 @@
         <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="86.4" customHeight="1">
@@ -4843,7 +4843,7 @@
         <v>133</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4851,7 +4851,7 @@
         <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="86.4" customHeight="1">
@@ -4859,7 +4859,7 @@
         <v>127</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.6" customHeight="1">
@@ -4867,7 +4867,7 @@
         <v>288</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="86.4" customHeight="1">
@@ -4875,295 +4875,295 @@
         <v>290</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="86.4" customHeight="1">
       <c r="A9" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="86.4" customHeight="1">
       <c r="A11" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="86.4" customHeight="1">
       <c r="A13" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="86.4" customHeight="1">
       <c r="A15" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="86.4" customHeight="1">
       <c r="A17" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="86.4" customHeight="1">
       <c r="A19" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="86.4" customHeight="1">
       <c r="A21" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="86.4" customHeight="1">
       <c r="A23" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="86.4" customHeight="1">
       <c r="A25" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="86.4" customHeight="1">
       <c r="A27" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="86.4" customHeight="1">
       <c r="A29" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="86.4" customHeight="1">
       <c r="A31" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="86.4" customHeight="1">
       <c r="A33" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="86.4" customHeight="1">
       <c r="A35" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="86.4" customHeight="1">
       <c r="A37" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="86.4" customHeight="1">
       <c r="A39" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="86.4" customHeight="1">
       <c r="A41" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="86.4" customHeight="1">
       <c r="A43" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -5174,34 +5174,34 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="86.4" customHeight="1">
       <c r="A47" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="86.4" customHeight="1">
       <c r="A49" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -5209,7 +5209,7 @@
         <v>141</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="86.4" customHeight="1">
@@ -5217,23 +5217,23 @@
         <v>143</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.6" customHeight="1">
       <c r="A52" s="24" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="93.6" customHeight="1">
       <c r="A53" s="24" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -5241,7 +5241,7 @@
         <v>145</v>
       </c>
       <c r="B54" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="86.4" customHeight="1">
@@ -5249,7 +5249,7 @@
         <v>147</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -5257,7 +5257,7 @@
         <v>121</v>
       </c>
       <c r="B56" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="86.4" customHeight="1">
@@ -5265,119 +5265,119 @@
         <v>123</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15.6" customHeight="1">
       <c r="A58" s="24" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="93.6" customHeight="1">
       <c r="A59" s="24" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.6" customHeight="1">
       <c r="A60" s="24" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="93.6" customHeight="1">
       <c r="A61" s="24" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.6" customHeight="1">
       <c r="A62" s="24" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="93.6" customHeight="1">
       <c r="A63" s="24" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15.6" customHeight="1">
       <c r="A64" s="24" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B64" s="24" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="93.6" customHeight="1">
       <c r="A65" s="24" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15.6" customHeight="1">
       <c r="A66" s="24" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="93.6" customHeight="1">
       <c r="A67" s="24" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15.6" customHeight="1">
       <c r="A68" s="24" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="93.6" customHeight="1">
       <c r="A69" s="24" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15.6" customHeight="1">
       <c r="A70" s="24" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="93.6" customHeight="1">
       <c r="A71" s="24" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
     </row>
   </sheetData>
@@ -5415,7 +5415,7 @@
         <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="86.4">
@@ -5423,7 +5423,7 @@
         <v>133</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5431,7 +5431,7 @@
         <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="86.4">
@@ -5439,119 +5439,119 @@
         <v>127</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="86.4">
       <c r="A7" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="86.4">
       <c r="A9" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="86.4">
       <c r="A11" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="86.4">
       <c r="A13" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="86.4">
       <c r="A15" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="86.4">
       <c r="A17" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="86.4">
       <c r="A19" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -5559,7 +5559,7 @@
         <v>141</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="86.4">
@@ -5567,23 +5567,23 @@
         <v>143</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.6">
       <c r="A22" s="24" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="93.6">
       <c r="A23" s="24" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -5591,7 +5591,7 @@
         <v>145</v>
       </c>
       <c r="B24" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="86.4">
@@ -5599,7 +5599,7 @@
         <v>147</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -5607,7 +5607,7 @@
         <v>121</v>
       </c>
       <c r="B26" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="86.4">
@@ -5615,119 +5615,119 @@
         <v>123</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.6">
       <c r="A28" s="24" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="93.6">
       <c r="A29" s="24" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.6">
       <c r="A30" s="24" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="93.6">
       <c r="A31" s="24" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.6">
       <c r="A32" s="24" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="93.6">
       <c r="A33" s="24" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.6">
       <c r="A34" s="24" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="93.6">
       <c r="A35" s="24" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.6">
       <c r="A36" s="24" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="93.6">
       <c r="A37" s="24" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.6">
       <c r="A38" s="24" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="93.6">
       <c r="A39" s="24" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.6">
       <c r="A40" s="24" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="93.6">
       <c r="A41" s="24" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
     </row>
   </sheetData>
@@ -5765,7 +5765,7 @@
         <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="86.4">
@@ -5773,7 +5773,7 @@
         <v>133</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5781,7 +5781,7 @@
         <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="86.4">
@@ -5789,119 +5789,119 @@
         <v>127</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="86.4">
       <c r="A7" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="86.4">
       <c r="A9" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="86.4">
       <c r="A11" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="86.4">
       <c r="A13" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="86.4">
       <c r="A15" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="86.4">
       <c r="A17" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="86.4">
       <c r="A19" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -5909,7 +5909,7 @@
         <v>141</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="86.4">
@@ -5917,23 +5917,23 @@
         <v>143</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.6">
       <c r="A22" s="24" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="93.6">
       <c r="A23" s="24" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -5941,7 +5941,7 @@
         <v>145</v>
       </c>
       <c r="B24" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="86.4">
@@ -5949,7 +5949,7 @@
         <v>147</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -5957,7 +5957,7 @@
         <v>121</v>
       </c>
       <c r="B26" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="86.4">
@@ -5965,119 +5965,119 @@
         <v>123</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.6">
       <c r="A28" s="24" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="93.6">
       <c r="A29" s="24" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.6">
       <c r="A30" s="24" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="93.6">
       <c r="A31" s="24" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.6">
       <c r="A32" s="24" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="93.6">
       <c r="A33" s="24" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.6">
       <c r="A34" s="24" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="93.6">
       <c r="A35" s="24" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.6">
       <c r="A36" s="24" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="93.6">
       <c r="A37" s="24" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.6">
       <c r="A38" s="24" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="93.6">
       <c r="A39" s="24" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.6">
       <c r="A40" s="24" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="109.2">
       <c r="A41" s="24" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
     </row>
   </sheetData>
@@ -6115,7 +6115,7 @@
         <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="86.4">
@@ -6123,7 +6123,7 @@
         <v>133</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6131,7 +6131,7 @@
         <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="86.4">
@@ -6139,103 +6139,103 @@
         <v>127</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="86.4">
       <c r="A7" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="86.4">
       <c r="A9" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="86.4">
       <c r="A11" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="86.4">
       <c r="A13" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="86.4">
       <c r="A15" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.6">
       <c r="A16" s="24" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="93.6">
       <c r="A17" s="24" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -6243,7 +6243,7 @@
         <v>145</v>
       </c>
       <c r="B18" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="86.4">
@@ -6251,7 +6251,7 @@
         <v>147</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -6259,7 +6259,7 @@
         <v>121</v>
       </c>
       <c r="B20" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="86.4">
@@ -6267,119 +6267,119 @@
         <v>123</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.6">
       <c r="A22" s="24" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="93.6">
       <c r="A23" s="24" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.6">
       <c r="A24" s="24" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="93.6">
       <c r="A25" s="24" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.6">
       <c r="A26" s="24" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="93.6">
       <c r="A27" s="24" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.6">
       <c r="A28" s="24" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="93.6">
       <c r="A29" s="24" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.6">
       <c r="A30" s="24" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="93.6">
       <c r="A31" s="24" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.6">
       <c r="A32" s="24" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="93.6">
       <c r="A33" s="24" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.6">
       <c r="A34" s="24" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="93.6">
       <c r="A35" s="24" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
   </sheetData>
@@ -6415,15 +6415,15 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="B2" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -6431,7 +6431,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="B4">
         <v>25</v>
@@ -6439,26 +6439,26 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="B5" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="B6" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B7" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6474,18 +6474,18 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -6557,7 +6557,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="B38" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -6607,8 +6607,8 @@
   </sheetPr>
   <dimension ref="A1:B167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="114" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="114" workbookViewId="0">
+      <selection activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7215,18 +7215,18 @@
     </row>
     <row r="100" spans="1:2" ht="15.6" customHeight="1">
       <c r="A100" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="B100" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="15.6" customHeight="1">
       <c r="A101" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="B101" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="15.6" customHeight="1"/>
@@ -7249,26 +7249,26 @@
     <row r="105" spans="1:2" ht="15.6" customHeight="1"/>
     <row r="106" spans="1:2" ht="15.6" customHeight="1">
       <c r="A106" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="B106" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="15.6" customHeight="1">
       <c r="A107" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="B107" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="15.6" customHeight="1">
       <c r="A108" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="B108" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -7346,7 +7346,7 @@
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="B123">
         <v>25</v>
@@ -7354,18 +7354,18 @@
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="B124" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="B126" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -7381,7 +7381,7 @@
         <v>469</v>
       </c>
       <c r="B132" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -7389,7 +7389,7 @@
         <v>89</v>
       </c>
       <c r="B133" t="s">
-        <v>470</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -7397,39 +7397,39 @@
         <v>90</v>
       </c>
       <c r="B134" t="s">
-        <v>471</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B135" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="15.6" customHeight="1">
       <c r="A136" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B136" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="15.6" customHeight="1">
       <c r="A137" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B137" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="15.6" customHeight="1">
       <c r="A138" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B138" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="15.6" customHeight="1"/>
@@ -7443,67 +7443,67 @@
     </row>
     <row r="141" spans="1:2" ht="15.6" customHeight="1">
       <c r="A141" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B141" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="15.6" customHeight="1">
       <c r="A142" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="B142" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="15.6" customHeight="1">
       <c r="A143" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="B143" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="15.6" customHeight="1"/>
     <row r="145" spans="1:2" ht="15.6" customHeight="1">
       <c r="A145" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B145" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="15.6" customHeight="1">
       <c r="A146" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B146" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="15.6" customHeight="1">
       <c r="A147" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="B147" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="15.6" customHeight="1">
       <c r="A148" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="B148" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="15.6" customHeight="1">
       <c r="A149" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="B149" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -7516,10 +7516,10 @@
     </row>
     <row r="151" spans="1:2" ht="15.6" customHeight="1">
       <c r="A151" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B151" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="15.6" customHeight="1"/>
@@ -7634,7 +7634,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8865,7 +8865,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -9087,8 +9087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -9310,8 +9310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -10652,7 +10652,7 @@
         <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="100.8">
@@ -10660,7 +10660,7 @@
         <v>133</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -10668,7 +10668,7 @@
         <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="86.4">
@@ -10676,31 +10676,31 @@
         <v>127</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.6">
       <c r="A6" s="24" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="86.4">
       <c r="A7" s="24" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="86.4">
@@ -10708,55 +10708,55 @@
         <v>375</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="86.4">
       <c r="A11" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="86.4">
       <c r="A13" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.6">
       <c r="A14" s="24" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="93.6">
       <c r="A15" s="24" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -10764,7 +10764,7 @@
         <v>145</v>
       </c>
       <c r="B16" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="86.4">
@@ -10772,7 +10772,7 @@
         <v>147</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -10780,7 +10780,7 @@
         <v>121</v>
       </c>
       <c r="B18" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="86.4">
@@ -10788,119 +10788,119 @@
         <v>123</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.6">
       <c r="A20" s="24" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="93.6">
       <c r="A21" s="24" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.6">
       <c r="A22" s="24" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="93.6">
       <c r="A23" s="24" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.6">
       <c r="A24" s="24" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="93.6">
       <c r="A25" s="24" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.6">
       <c r="A26" s="24" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="93.6">
       <c r="A27" s="24" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.6">
       <c r="A28" s="24" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="93.6">
       <c r="A29" s="24" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.6">
       <c r="A30" s="24" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="93.6">
       <c r="A31" s="24" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.6">
       <c r="A32" s="24" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="93.6">
       <c r="A33" s="24" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
   </sheetData>
@@ -11358,8 +11358,8 @@
   </sheetPr>
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -11381,7 +11381,7 @@
         <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="86.4">
@@ -11389,7 +11389,7 @@
         <v>133</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -11397,7 +11397,7 @@
         <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="86.4">
@@ -11405,12 +11405,12 @@
         <v>127</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.6">
       <c r="A6" s="24" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>300</v>
@@ -11418,15 +11418,15 @@
     </row>
     <row r="7" spans="1:2" ht="86.4">
       <c r="A7" s="24" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>300</v>
@@ -11437,55 +11437,55 @@
         <v>375</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="86.4">
       <c r="A11" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="86.4">
       <c r="A13" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.6">
       <c r="A14" s="24" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="93.6">
       <c r="A15" s="24" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -11493,7 +11493,7 @@
         <v>145</v>
       </c>
       <c r="B16" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="86.4">
@@ -11501,7 +11501,7 @@
         <v>147</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -11509,7 +11509,7 @@
         <v>121</v>
       </c>
       <c r="B18" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="86.4">
@@ -11517,119 +11517,119 @@
         <v>123</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.6">
       <c r="A20" s="24" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="93.6">
       <c r="A21" s="24" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.6">
       <c r="A22" s="24" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="93.6">
       <c r="A23" s="24" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.6">
       <c r="A24" s="24" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="93.6">
       <c r="A25" s="24" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.6">
       <c r="A26" s="24" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="93.6">
       <c r="A27" s="24" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.6">
       <c r="A28" s="24" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="93.6">
       <c r="A29" s="24" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.6">
       <c r="A30" s="24" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="93.6">
       <c r="A31" s="24" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.6">
       <c r="A32" s="24" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="93.6">
       <c r="A33" s="24" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
   </sheetData>
@@ -11645,7 +11645,7 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -11671,7 +11671,7 @@
         <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="86.4">
@@ -11679,7 +11679,7 @@
         <v>133</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -11700,7 +11700,7 @@
     </row>
     <row r="7" spans="1:2" ht="15.6">
       <c r="A7" s="24" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>289</v>
@@ -11708,10 +11708,10 @@
     </row>
     <row r="8" spans="1:2" ht="86.4">
       <c r="A8" s="24" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -11732,50 +11732,50 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="86.4">
       <c r="A12" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="86.4">
       <c r="A14" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.6">
       <c r="A15" s="24" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="93.6">
       <c r="A16" s="24" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -11783,7 +11783,7 @@
         <v>145</v>
       </c>
       <c r="B17" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="86.4">
@@ -11791,7 +11791,7 @@
         <v>147</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -11799,7 +11799,7 @@
         <v>121</v>
       </c>
       <c r="B19" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="86.4">
@@ -11807,119 +11807,119 @@
         <v>123</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.6">
       <c r="A21" s="24" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="93.6">
       <c r="A22" s="24" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.6">
       <c r="A23" s="24" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="93.6">
       <c r="A24" s="24" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.6">
       <c r="A25" s="24" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="93.6">
       <c r="A26" s="24" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.6">
       <c r="A27" s="24" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="93.6">
       <c r="A28" s="24" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.6">
       <c r="A29" s="24" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="93.6">
       <c r="A30" s="24" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.6">
       <c r="A31" s="24" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="93.6">
       <c r="A32" s="24" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.6">
       <c r="A33" s="24" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="93.6">
       <c r="A34" s="24" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
   </sheetData>
@@ -11961,7 +11961,7 @@
         <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="100.8">
@@ -11969,7 +11969,7 @@
         <v>133</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -11977,7 +11977,7 @@
         <v>125</v>
       </c>
       <c r="B5" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="86.4">
@@ -11985,87 +11985,87 @@
         <v>127</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.6">
       <c r="A7" s="24" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="86.4">
       <c r="A8" s="24" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="86.4">
       <c r="A10" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="86.4">
       <c r="A12" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="86.4">
       <c r="A14" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.6">
       <c r="A15" s="24" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="93.6">
       <c r="A16" s="24" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -12073,7 +12073,7 @@
         <v>145</v>
       </c>
       <c r="B17" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="86.4">
@@ -12081,7 +12081,7 @@
         <v>147</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -12089,7 +12089,7 @@
         <v>121</v>
       </c>
       <c r="B19" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="86.4">
@@ -12097,119 +12097,119 @@
         <v>123</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.6">
       <c r="A21" s="24" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="93.6">
       <c r="A22" s="24" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.6">
       <c r="A23" s="24" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="93.6">
       <c r="A24" s="24" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.6">
       <c r="A25" s="24" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="93.6">
       <c r="A26" s="24" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.6">
       <c r="A27" s="24" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="93.6">
       <c r="A28" s="24" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.6">
       <c r="A29" s="24" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="93.6">
       <c r="A30" s="24" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.6">
       <c r="A31" s="24" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="93.6">
       <c r="A32" s="24" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.6">
       <c r="A33" s="24" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="93.6">
       <c r="A34" s="24" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
   </sheetData>
@@ -12250,7 +12250,7 @@
         <v>353</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="100.95" customHeight="1">
@@ -12258,55 +12258,55 @@
         <v>165</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="100.95" customHeight="1">
       <c r="A6" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="100.95" customHeight="1">
       <c r="A8" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="100.95" customHeight="1">
       <c r="A10" s="27" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -12314,7 +12314,7 @@
         <v>145</v>
       </c>
       <c r="B11" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="100.95" customHeight="1">
@@ -12322,71 +12322,71 @@
         <v>147</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="86.4" customHeight="1">
       <c r="A14" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="86.4" customHeight="1">
       <c r="A16" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="86.4" customHeight="1">
       <c r="A18" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B19" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="100.95" customHeight="1">
       <c r="A20" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -12394,7 +12394,7 @@
         <v>421</v>
       </c>
       <c r="B21" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="100.95" customHeight="1">
@@ -12402,119 +12402,119 @@
         <v>422</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="100.95" customHeight="1">
       <c r="A24" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="100.95" customHeight="1">
       <c r="A26" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="100.95" customHeight="1">
       <c r="A28" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.6" customHeight="1">
       <c r="A29" s="24" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="93.6" customHeight="1">
       <c r="A30" s="24" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.6" customHeight="1">
       <c r="A31" s="24" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="93.6" customHeight="1">
       <c r="A32" s="24" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.6" customHeight="1">
       <c r="A33" s="24" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="93.6" customHeight="1">
       <c r="A34" s="24" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.6" customHeight="1">
       <c r="A35" s="24" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="93.6" customHeight="1">
       <c r="A36" s="24" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -12522,7 +12522,7 @@
         <v>145</v>
       </c>
       <c r="B37" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="86.4" customHeight="1">
@@ -12530,7 +12530,7 @@
         <v>147</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -12538,7 +12538,7 @@
         <v>121</v>
       </c>
       <c r="B39" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="86.4" customHeight="1">
@@ -12546,71 +12546,71 @@
         <v>123</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.6" customHeight="1">
       <c r="A41" s="24" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="93.6" customHeight="1">
       <c r="A42" s="24" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.6" customHeight="1">
       <c r="A43" s="24" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B43" s="24" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="93.6" customHeight="1">
       <c r="A44" s="24" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.6" customHeight="1">
       <c r="A45" s="24" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="93.6" customHeight="1">
       <c r="A46" s="24" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.6" customHeight="1">
       <c r="A47" s="24" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="93.6" customHeight="1">
       <c r="A48" s="24" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
   </sheetData>
@@ -12652,7 +12652,7 @@
         <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="86.4">
@@ -12660,7 +12660,7 @@
         <v>133</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -12668,7 +12668,7 @@
         <v>125</v>
       </c>
       <c r="B5" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="86.4">
@@ -12676,87 +12676,87 @@
         <v>127</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.6">
       <c r="A7" s="24" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="86.4">
       <c r="A8" s="24" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="86.4">
       <c r="A10" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="86.4">
       <c r="A12" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="86.4">
       <c r="A14" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="86.4">
       <c r="A16" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -12764,7 +12764,7 @@
         <v>141</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="86.4">
@@ -12772,23 +12772,23 @@
         <v>143</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.6">
       <c r="A19" s="24" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="93.6">
       <c r="A20" s="24" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -12796,7 +12796,7 @@
         <v>145</v>
       </c>
       <c r="B21" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="86.4">
@@ -12804,7 +12804,7 @@
         <v>147</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -12812,7 +12812,7 @@
         <v>121</v>
       </c>
       <c r="B23" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="86.4">
@@ -12820,119 +12820,119 @@
         <v>123</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.6">
       <c r="A25" s="24" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="93.6">
       <c r="A26" s="24" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.6">
       <c r="A27" s="24" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="93.6">
       <c r="A28" s="24" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.6">
       <c r="A29" s="24" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="93.6">
       <c r="A30" s="24" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.6">
       <c r="A31" s="24" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="93.6">
       <c r="A32" s="24" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.6">
       <c r="A33" s="24" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="93.6">
       <c r="A34" s="24" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.6">
       <c r="A35" s="24" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="93.6">
       <c r="A36" s="24" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.6">
       <c r="A37" s="24" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="93.6">
       <c r="A38" s="24" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
   </sheetData>
@@ -12974,7 +12974,7 @@
         <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="100.95" customHeight="1">
@@ -12982,7 +12982,7 @@
         <v>133</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -12990,7 +12990,7 @@
         <v>125</v>
       </c>
       <c r="B5" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="86.4" customHeight="1">
@@ -12998,199 +12998,199 @@
         <v>127</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="86.4" customHeight="1">
       <c r="A8" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="86.4" customHeight="1">
       <c r="A10" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="86.4" customHeight="1">
       <c r="A12" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="86.4" customHeight="1">
       <c r="A14" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="86.4" customHeight="1">
       <c r="A16" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="86.4" customHeight="1">
       <c r="A18" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="86.4" customHeight="1">
       <c r="A20" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="86.4" customHeight="1">
       <c r="A22" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="86.4" customHeight="1">
       <c r="A24" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="86.4" customHeight="1">
       <c r="A26" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="86.4" customHeight="1">
       <c r="A28" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="86.4" customHeight="1">
       <c r="A30" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -13198,34 +13198,34 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="86.4" customHeight="1">
       <c r="A33" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.6" customHeight="1">
       <c r="A34" s="24" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="109.2" customHeight="1">
       <c r="A35" s="24" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -13233,7 +13233,7 @@
         <v>145</v>
       </c>
       <c r="B36" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="100.95" customHeight="1">
@@ -13241,7 +13241,7 @@
         <v>147</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -13249,7 +13249,7 @@
         <v>121</v>
       </c>
       <c r="B38" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="86.4" customHeight="1">
@@ -13257,119 +13257,119 @@
         <v>123</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.6" customHeight="1">
       <c r="A40" s="24" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="93.6" customHeight="1">
       <c r="A41" s="24" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.6" customHeight="1">
       <c r="A42" s="24" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="93.6" customHeight="1">
       <c r="A43" s="24" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.6" customHeight="1">
       <c r="A44" s="24" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="93.6" customHeight="1">
       <c r="A45" s="24" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.6" customHeight="1">
       <c r="A46" s="24" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="93.6" customHeight="1">
       <c r="A47" s="24" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.6" customHeight="1">
       <c r="A48" s="24" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="93.6" customHeight="1">
       <c r="A49" s="24" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.6" customHeight="1">
       <c r="A50" s="24" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="93.6" customHeight="1">
       <c r="A51" s="24" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.6" customHeight="1">
       <c r="A52" s="24" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="93.6" customHeight="1">
       <c r="A53" s="24" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LnCo as on Jan 30 2022
</commit_message>
<xml_diff>
--- a/Lnco/Input/Config.xlsx
+++ b/Lnco/Input/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BRADSOL-User\Documents\GitHub\brad-lnco-projects\Lnco\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170FCD5F-17DC-4FB5-B596-F16C99F54135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307FBEA5-F956-4501-AF1F-0B04088FE6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="954" firstSheet="25" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="954" firstSheet="13" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequence Check" sheetId="18" r:id="rId1"/>
@@ -45,12 +45,25 @@
     <sheet name="Purchase Wise Comparatives" sheetId="15" r:id="rId30"/>
     <sheet name="Inventory Mapping" sheetId="16" r:id="rId31"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1937" uniqueCount="1027">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1937" uniqueCount="1029">
   <si>
     <t>Key</t>
   </si>
@@ -4157,6 +4170,18 @@
 Thanks &amp; Regards,
 L &amp; Co   
                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                            </t>
+  </si>
+  <si>
+    <t>Hello,
+Bot has started processing the {0} automation
+Thanks &amp; Regards,
+ LN &amp; Co</t>
+  </si>
+  <si>
+    <t>Hello,
+Bot has Successfully completed the {0} automation.
+Thanks &amp; Regards,
+ LN &amp; Co</t>
   </si>
 </sst>
 </file>
@@ -6630,8 +6655,8 @@
   </sheetPr>
   <dimension ref="A1:B167"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="114" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A159" zoomScale="114" workbookViewId="0">
+      <selection activeCell="B165" sqref="B165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7567,7 +7592,7 @@
         <v>102</v>
       </c>
       <c r="B155" s="19" t="s">
-        <v>103</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -7583,7 +7608,7 @@
         <v>106</v>
       </c>
       <c r="B158" s="19" t="s">
-        <v>107</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -7656,8 +7681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8086,8 +8111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -11148,8 +11173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
LnCo as on Mar 1 2023
Included Purchase register feedback points
</commit_message>
<xml_diff>
--- a/Lnco/Input/Config.xlsx
+++ b/Lnco/Input/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BRADSOL-User\Documents\GitHub\brad-lnco-projects\Lnco\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307FBEA5-F956-4501-AF1F-0B04088FE6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088534BC-A04B-4FE7-B280-5A4DF7CF4AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="954" firstSheet="13" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1937" uniqueCount="1029">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1937" uniqueCount="1030">
   <si>
     <t>Key</t>
   </si>
@@ -4182,6 +4182,9 @@
 Bot has Successfully completed the {0} automation.
 Thanks &amp; Regards,
  LN &amp; Co</t>
+  </si>
+  <si>
+    <t>SM FROM SVDP</t>
   </si>
 </sst>
 </file>
@@ -6655,8 +6658,8 @@
   </sheetPr>
   <dimension ref="A1:B167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" zoomScale="114" workbookViewId="0">
-      <selection activeCell="B165" sqref="B165"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="114" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6828,7 +6831,7 @@
         <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="29" spans="1:2">

</xml_diff>